<commit_message>
Unity & Uren reg
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -575,19 +575,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -869,7 +869,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -881,7 +881,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L50" sqref="L50"/>
+      <selection pane="bottomLeft" activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -940,15 +940,15 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="49"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
@@ -1167,11 +1167,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.625</v>
+        <v>0.65625</v>
       </c>
       <c r="O7" s="14" t="s">
         <v>39</v>
@@ -1229,30 +1229,30 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="49"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1459,30 +1459,30 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="47"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="49"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1687,30 +1687,30 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="48"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="47"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="49"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -1915,30 +1915,30 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="48"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="47"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="49"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2145,30 +2145,30 @@
       <c r="L40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A41" s="48"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="45"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="49"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2377,30 +2377,30 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="48"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
+      <c r="A49" s="47"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="47"/>
+      <c r="J49" s="47"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="46"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="47"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="49"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2605,30 +2605,30 @@
       <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="48"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="48"/>
-      <c r="J57" s="48"/>
+      <c r="A57" s="47"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="47"/>
+      <c r="J57" s="47"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="45"/>
-      <c r="C58" s="46"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="46"/>
-      <c r="F58" s="46"/>
-      <c r="G58" s="46"/>
-      <c r="H58" s="46"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="47"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="49"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -2718,7 +2718,9 @@
       <c r="G61" s="6">
         <v>6</v>
       </c>
-      <c r="H61" s="30"/>
+      <c r="H61" s="30">
+        <v>5</v>
+      </c>
       <c r="I61" s="6">
         <v>6</v>
       </c>
@@ -2786,7 +2788,7 @@
       </c>
       <c r="H64" s="35">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I64" s="35">
         <f>SUM(I59:I63)</f>
@@ -2797,30 +2799,30 @@
       <c r="L64" s="8"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A65" s="48"/>
-      <c r="B65" s="48"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="48"/>
-      <c r="H65" s="48"/>
-      <c r="I65" s="48"/>
-      <c r="J65" s="48"/>
+      <c r="A65" s="47"/>
+      <c r="B65" s="47"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="47"/>
+      <c r="I65" s="47"/>
+      <c r="J65" s="47"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="45"/>
-      <c r="C66" s="46"/>
-      <c r="D66" s="46"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="46"/>
-      <c r="H66" s="46"/>
-      <c r="I66" s="46"/>
-      <c r="J66" s="47"/>
+      <c r="B66" s="48"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="45"/>
+      <c r="J66" s="49"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -2955,30 +2957,30 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A73" s="48"/>
-      <c r="B73" s="48"/>
-      <c r="C73" s="48"/>
-      <c r="D73" s="48"/>
-      <c r="E73" s="48"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="48"/>
-      <c r="H73" s="48"/>
-      <c r="I73" s="48"/>
-      <c r="J73" s="48"/>
+      <c r="A73" s="47"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="47"/>
+      <c r="E73" s="47"/>
+      <c r="F73" s="47"/>
+      <c r="G73" s="47"/>
+      <c r="H73" s="47"/>
+      <c r="I73" s="47"/>
+      <c r="J73" s="47"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="45"/>
-      <c r="C74" s="46"/>
-      <c r="D74" s="46"/>
-      <c r="E74" s="46"/>
-      <c r="F74" s="46"/>
-      <c r="G74" s="46"/>
-      <c r="H74" s="46"/>
-      <c r="I74" s="46"/>
-      <c r="J74" s="47"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="45"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
+      <c r="F74" s="45"/>
+      <c r="G74" s="45"/>
+      <c r="H74" s="45"/>
+      <c r="I74" s="45"/>
+      <c r="J74" s="49"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3075,30 +3077,30 @@
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A81" s="48"/>
-      <c r="B81" s="48"/>
-      <c r="C81" s="48"/>
-      <c r="D81" s="48"/>
-      <c r="E81" s="48"/>
-      <c r="F81" s="48"/>
-      <c r="G81" s="48"/>
-      <c r="H81" s="48"/>
-      <c r="I81" s="48"/>
-      <c r="J81" s="48"/>
+      <c r="A81" s="47"/>
+      <c r="B81" s="47"/>
+      <c r="C81" s="47"/>
+      <c r="D81" s="47"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="47"/>
+      <c r="G81" s="47"/>
+      <c r="H81" s="47"/>
+      <c r="I81" s="47"/>
+      <c r="J81" s="47"/>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="45"/>
-      <c r="C82" s="46"/>
-      <c r="D82" s="46"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="46"/>
-      <c r="G82" s="46"/>
-      <c r="H82" s="46"/>
-      <c r="I82" s="46"/>
-      <c r="J82" s="47"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="45"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="45"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="45"/>
+      <c r="I82" s="45"/>
+      <c r="J82" s="49"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3195,30 +3197,30 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A89" s="48"/>
-      <c r="B89" s="48"/>
-      <c r="C89" s="48"/>
-      <c r="D89" s="48"/>
-      <c r="E89" s="48"/>
-      <c r="F89" s="48"/>
-      <c r="G89" s="48"/>
-      <c r="H89" s="48"/>
-      <c r="I89" s="48"/>
-      <c r="J89" s="48"/>
+      <c r="A89" s="47"/>
+      <c r="B89" s="47"/>
+      <c r="C89" s="47"/>
+      <c r="D89" s="47"/>
+      <c r="E89" s="47"/>
+      <c r="F89" s="47"/>
+      <c r="G89" s="47"/>
+      <c r="H89" s="47"/>
+      <c r="I89" s="47"/>
+      <c r="J89" s="47"/>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="45"/>
-      <c r="C90" s="46"/>
-      <c r="D90" s="46"/>
-      <c r="E90" s="46"/>
-      <c r="F90" s="46"/>
-      <c r="G90" s="46"/>
-      <c r="H90" s="46"/>
-      <c r="I90" s="46"/>
-      <c r="J90" s="47"/>
+      <c r="B90" s="48"/>
+      <c r="C90" s="45"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="45"/>
+      <c r="F90" s="45"/>
+      <c r="G90" s="45"/>
+      <c r="H90" s="45"/>
+      <c r="I90" s="45"/>
+      <c r="J90" s="49"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3315,30 +3317,30 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A97" s="48"/>
-      <c r="B97" s="48"/>
-      <c r="C97" s="48"/>
-      <c r="D97" s="48"/>
-      <c r="E97" s="48"/>
-      <c r="F97" s="48"/>
-      <c r="G97" s="48"/>
-      <c r="H97" s="48"/>
-      <c r="I97" s="48"/>
-      <c r="J97" s="48"/>
+      <c r="A97" s="47"/>
+      <c r="B97" s="47"/>
+      <c r="C97" s="47"/>
+      <c r="D97" s="47"/>
+      <c r="E97" s="47"/>
+      <c r="F97" s="47"/>
+      <c r="G97" s="47"/>
+      <c r="H97" s="47"/>
+      <c r="I97" s="47"/>
+      <c r="J97" s="47"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="45"/>
-      <c r="C98" s="46"/>
-      <c r="D98" s="46"/>
-      <c r="E98" s="46"/>
-      <c r="F98" s="46"/>
-      <c r="G98" s="46"/>
-      <c r="H98" s="46"/>
-      <c r="I98" s="46"/>
-      <c r="J98" s="47"/>
+      <c r="B98" s="48"/>
+      <c r="C98" s="45"/>
+      <c r="D98" s="45"/>
+      <c r="E98" s="45"/>
+      <c r="F98" s="45"/>
+      <c r="G98" s="45"/>
+      <c r="H98" s="45"/>
+      <c r="I98" s="45"/>
+      <c r="J98" s="49"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -3435,30 +3437,30 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A105" s="48"/>
-      <c r="B105" s="48"/>
-      <c r="C105" s="48"/>
-      <c r="D105" s="48"/>
-      <c r="E105" s="48"/>
-      <c r="F105" s="48"/>
-      <c r="G105" s="48"/>
-      <c r="H105" s="48"/>
-      <c r="I105" s="48"/>
-      <c r="J105" s="48"/>
+      <c r="A105" s="47"/>
+      <c r="B105" s="47"/>
+      <c r="C105" s="47"/>
+      <c r="D105" s="47"/>
+      <c r="E105" s="47"/>
+      <c r="F105" s="47"/>
+      <c r="G105" s="47"/>
+      <c r="H105" s="47"/>
+      <c r="I105" s="47"/>
+      <c r="J105" s="47"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="45"/>
-      <c r="C106" s="46"/>
-      <c r="D106" s="46"/>
-      <c r="E106" s="46"/>
-      <c r="F106" s="46"/>
-      <c r="G106" s="46"/>
-      <c r="H106" s="46"/>
-      <c r="I106" s="46"/>
-      <c r="J106" s="47"/>
+      <c r="B106" s="48"/>
+      <c r="C106" s="45"/>
+      <c r="D106" s="45"/>
+      <c r="E106" s="45"/>
+      <c r="F106" s="45"/>
+      <c r="G106" s="45"/>
+      <c r="H106" s="45"/>
+      <c r="I106" s="45"/>
+      <c r="J106" s="49"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -3555,30 +3557,30 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A113" s="48"/>
-      <c r="B113" s="48"/>
-      <c r="C113" s="48"/>
-      <c r="D113" s="48"/>
-      <c r="E113" s="48"/>
-      <c r="F113" s="48"/>
-      <c r="G113" s="48"/>
-      <c r="H113" s="48"/>
-      <c r="I113" s="48"/>
-      <c r="J113" s="48"/>
+      <c r="A113" s="47"/>
+      <c r="B113" s="47"/>
+      <c r="C113" s="47"/>
+      <c r="D113" s="47"/>
+      <c r="E113" s="47"/>
+      <c r="F113" s="47"/>
+      <c r="G113" s="47"/>
+      <c r="H113" s="47"/>
+      <c r="I113" s="47"/>
+      <c r="J113" s="47"/>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="45"/>
-      <c r="C114" s="46"/>
-      <c r="D114" s="46"/>
-      <c r="E114" s="46"/>
-      <c r="F114" s="46"/>
-      <c r="G114" s="46"/>
-      <c r="H114" s="46"/>
-      <c r="I114" s="46"/>
-      <c r="J114" s="47"/>
+      <c r="B114" s="48"/>
+      <c r="C114" s="45"/>
+      <c r="D114" s="45"/>
+      <c r="E114" s="45"/>
+      <c r="F114" s="45"/>
+      <c r="G114" s="45"/>
+      <c r="H114" s="45"/>
+      <c r="I114" s="45"/>
+      <c r="J114" s="49"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -3675,30 +3677,30 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A121" s="48"/>
-      <c r="B121" s="48"/>
-      <c r="C121" s="48"/>
-      <c r="D121" s="48"/>
-      <c r="E121" s="48"/>
-      <c r="F121" s="48"/>
-      <c r="G121" s="48"/>
-      <c r="H121" s="48"/>
-      <c r="I121" s="48"/>
-      <c r="J121" s="48"/>
+      <c r="A121" s="47"/>
+      <c r="B121" s="47"/>
+      <c r="C121" s="47"/>
+      <c r="D121" s="47"/>
+      <c r="E121" s="47"/>
+      <c r="F121" s="47"/>
+      <c r="G121" s="47"/>
+      <c r="H121" s="47"/>
+      <c r="I121" s="47"/>
+      <c r="J121" s="47"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="45"/>
-      <c r="C122" s="46"/>
-      <c r="D122" s="46"/>
-      <c r="E122" s="46"/>
-      <c r="F122" s="46"/>
-      <c r="G122" s="46"/>
-      <c r="H122" s="46"/>
-      <c r="I122" s="46"/>
-      <c r="J122" s="47"/>
+      <c r="B122" s="48"/>
+      <c r="C122" s="45"/>
+      <c r="D122" s="45"/>
+      <c r="E122" s="45"/>
+      <c r="F122" s="45"/>
+      <c r="G122" s="45"/>
+      <c r="H122" s="45"/>
+      <c r="I122" s="45"/>
+      <c r="J122" s="49"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -3795,30 +3797,30 @@
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A129" s="48"/>
-      <c r="B129" s="48"/>
-      <c r="C129" s="48"/>
-      <c r="D129" s="48"/>
-      <c r="E129" s="48"/>
-      <c r="F129" s="48"/>
-      <c r="G129" s="48"/>
-      <c r="H129" s="48"/>
-      <c r="I129" s="48"/>
-      <c r="J129" s="48"/>
+      <c r="A129" s="47"/>
+      <c r="B129" s="47"/>
+      <c r="C129" s="47"/>
+      <c r="D129" s="47"/>
+      <c r="E129" s="47"/>
+      <c r="F129" s="47"/>
+      <c r="G129" s="47"/>
+      <c r="H129" s="47"/>
+      <c r="I129" s="47"/>
+      <c r="J129" s="47"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="45"/>
-      <c r="C130" s="46"/>
-      <c r="D130" s="46"/>
-      <c r="E130" s="46"/>
-      <c r="F130" s="46"/>
-      <c r="G130" s="46"/>
-      <c r="H130" s="46"/>
-      <c r="I130" s="46"/>
-      <c r="J130" s="47"/>
+      <c r="B130" s="48"/>
+      <c r="C130" s="45"/>
+      <c r="D130" s="45"/>
+      <c r="E130" s="45"/>
+      <c r="F130" s="45"/>
+      <c r="G130" s="45"/>
+      <c r="H130" s="45"/>
+      <c r="I130" s="45"/>
+      <c r="J130" s="49"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -3915,30 +3917,30 @@
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A137" s="48"/>
-      <c r="B137" s="48"/>
-      <c r="C137" s="48"/>
-      <c r="D137" s="48"/>
-      <c r="E137" s="48"/>
-      <c r="F137" s="48"/>
-      <c r="G137" s="48"/>
-      <c r="H137" s="48"/>
-      <c r="I137" s="48"/>
-      <c r="J137" s="48"/>
+      <c r="A137" s="47"/>
+      <c r="B137" s="47"/>
+      <c r="C137" s="47"/>
+      <c r="D137" s="47"/>
+      <c r="E137" s="47"/>
+      <c r="F137" s="47"/>
+      <c r="G137" s="47"/>
+      <c r="H137" s="47"/>
+      <c r="I137" s="47"/>
+      <c r="J137" s="47"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="45"/>
-      <c r="C138" s="46"/>
-      <c r="D138" s="46"/>
-      <c r="E138" s="46"/>
-      <c r="F138" s="46"/>
-      <c r="G138" s="46"/>
-      <c r="H138" s="46"/>
-      <c r="I138" s="46"/>
-      <c r="J138" s="47"/>
+      <c r="B138" s="48"/>
+      <c r="C138" s="45"/>
+      <c r="D138" s="45"/>
+      <c r="E138" s="45"/>
+      <c r="F138" s="45"/>
+      <c r="G138" s="45"/>
+      <c r="H138" s="45"/>
+      <c r="I138" s="45"/>
+      <c r="J138" s="49"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -4035,30 +4037,30 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A145" s="48"/>
-      <c r="B145" s="48"/>
-      <c r="C145" s="48"/>
-      <c r="D145" s="48"/>
-      <c r="E145" s="48"/>
-      <c r="F145" s="48"/>
-      <c r="G145" s="48"/>
-      <c r="H145" s="48"/>
-      <c r="I145" s="48"/>
-      <c r="J145" s="48"/>
+      <c r="A145" s="47"/>
+      <c r="B145" s="47"/>
+      <c r="C145" s="47"/>
+      <c r="D145" s="47"/>
+      <c r="E145" s="47"/>
+      <c r="F145" s="47"/>
+      <c r="G145" s="47"/>
+      <c r="H145" s="47"/>
+      <c r="I145" s="47"/>
+      <c r="J145" s="47"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="45"/>
-      <c r="C146" s="46"/>
-      <c r="D146" s="46"/>
-      <c r="E146" s="46"/>
-      <c r="F146" s="46"/>
-      <c r="G146" s="46"/>
-      <c r="H146" s="46"/>
-      <c r="I146" s="46"/>
-      <c r="J146" s="47"/>
+      <c r="B146" s="48"/>
+      <c r="C146" s="45"/>
+      <c r="D146" s="45"/>
+      <c r="E146" s="45"/>
+      <c r="F146" s="45"/>
+      <c r="G146" s="45"/>
+      <c r="H146" s="45"/>
+      <c r="I146" s="45"/>
+      <c r="J146" s="49"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -4155,30 +4157,30 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A153" s="48"/>
-      <c r="B153" s="48"/>
-      <c r="C153" s="48"/>
-      <c r="D153" s="48"/>
-      <c r="E153" s="48"/>
-      <c r="F153" s="48"/>
-      <c r="G153" s="48"/>
-      <c r="H153" s="48"/>
-      <c r="I153" s="48"/>
-      <c r="J153" s="48"/>
+      <c r="A153" s="47"/>
+      <c r="B153" s="47"/>
+      <c r="C153" s="47"/>
+      <c r="D153" s="47"/>
+      <c r="E153" s="47"/>
+      <c r="F153" s="47"/>
+      <c r="G153" s="47"/>
+      <c r="H153" s="47"/>
+      <c r="I153" s="47"/>
+      <c r="J153" s="47"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="45"/>
-      <c r="C154" s="46"/>
-      <c r="D154" s="46"/>
-      <c r="E154" s="46"/>
-      <c r="F154" s="46"/>
-      <c r="G154" s="46"/>
-      <c r="H154" s="46"/>
-      <c r="I154" s="46"/>
-      <c r="J154" s="47"/>
+      <c r="B154" s="48"/>
+      <c r="C154" s="45"/>
+      <c r="D154" s="45"/>
+      <c r="E154" s="45"/>
+      <c r="F154" s="45"/>
+      <c r="G154" s="45"/>
+      <c r="H154" s="45"/>
+      <c r="I154" s="45"/>
+      <c r="J154" s="49"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -4275,30 +4277,30 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A161" s="48"/>
-      <c r="B161" s="48"/>
-      <c r="C161" s="48"/>
-      <c r="D161" s="48"/>
-      <c r="E161" s="48"/>
-      <c r="F161" s="48"/>
-      <c r="G161" s="48"/>
-      <c r="H161" s="48"/>
-      <c r="I161" s="48"/>
-      <c r="J161" s="48"/>
+      <c r="A161" s="47"/>
+      <c r="B161" s="47"/>
+      <c r="C161" s="47"/>
+      <c r="D161" s="47"/>
+      <c r="E161" s="47"/>
+      <c r="F161" s="47"/>
+      <c r="G161" s="47"/>
+      <c r="H161" s="47"/>
+      <c r="I161" s="47"/>
+      <c r="J161" s="47"/>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="45"/>
-      <c r="C162" s="46"/>
-      <c r="D162" s="46"/>
-      <c r="E162" s="46"/>
-      <c r="F162" s="46"/>
-      <c r="G162" s="46"/>
-      <c r="H162" s="46"/>
-      <c r="I162" s="46"/>
-      <c r="J162" s="47"/>
+      <c r="B162" s="48"/>
+      <c r="C162" s="45"/>
+      <c r="D162" s="45"/>
+      <c r="E162" s="45"/>
+      <c r="F162" s="45"/>
+      <c r="G162" s="45"/>
+      <c r="H162" s="45"/>
+      <c r="I162" s="45"/>
+      <c r="J162" s="49"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -4395,30 +4397,30 @@
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A169" s="48"/>
-      <c r="B169" s="48"/>
-      <c r="C169" s="48"/>
-      <c r="D169" s="48"/>
-      <c r="E169" s="48"/>
-      <c r="F169" s="48"/>
-      <c r="G169" s="48"/>
-      <c r="H169" s="48"/>
-      <c r="I169" s="48"/>
-      <c r="J169" s="48"/>
+      <c r="A169" s="47"/>
+      <c r="B169" s="47"/>
+      <c r="C169" s="47"/>
+      <c r="D169" s="47"/>
+      <c r="E169" s="47"/>
+      <c r="F169" s="47"/>
+      <c r="G169" s="47"/>
+      <c r="H169" s="47"/>
+      <c r="I169" s="47"/>
+      <c r="J169" s="47"/>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="45"/>
-      <c r="C170" s="46"/>
-      <c r="D170" s="46"/>
-      <c r="E170" s="46"/>
-      <c r="F170" s="46"/>
-      <c r="G170" s="46"/>
-      <c r="H170" s="46"/>
-      <c r="I170" s="46"/>
-      <c r="J170" s="47"/>
+      <c r="B170" s="48"/>
+      <c r="C170" s="45"/>
+      <c r="D170" s="45"/>
+      <c r="E170" s="45"/>
+      <c r="F170" s="45"/>
+      <c r="G170" s="45"/>
+      <c r="H170" s="45"/>
+      <c r="I170" s="45"/>
+      <c r="J170" s="49"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -4515,63 +4517,31 @@
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="46"/>
-      <c r="B177" s="46"/>
-      <c r="C177" s="46"/>
-      <c r="D177" s="46"/>
-      <c r="E177" s="46"/>
-      <c r="F177" s="46"/>
-      <c r="G177" s="46"/>
-      <c r="H177" s="46"/>
-      <c r="I177" s="46"/>
-      <c r="J177" s="46"/>
+      <c r="A177" s="45"/>
+      <c r="B177" s="45"/>
+      <c r="C177" s="45"/>
+      <c r="D177" s="45"/>
+      <c r="E177" s="45"/>
+      <c r="F177" s="45"/>
+      <c r="G177" s="45"/>
+      <c r="H177" s="45"/>
+      <c r="I177" s="45"/>
+      <c r="J177" s="45"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="49"/>
-      <c r="B178" s="49"/>
-      <c r="C178" s="49"/>
-      <c r="D178" s="49"/>
-      <c r="E178" s="49"/>
-      <c r="F178" s="49"/>
-      <c r="G178" s="49"/>
-      <c r="H178" s="49"/>
-      <c r="I178" s="49"/>
-      <c r="J178" s="49"/>
+      <c r="A178" s="46"/>
+      <c r="B178" s="46"/>
+      <c r="C178" s="46"/>
+      <c r="D178" s="46"/>
+      <c r="E178" s="46"/>
+      <c r="F178" s="46"/>
+      <c r="G178" s="46"/>
+      <c r="H178" s="46"/>
+      <c r="I178" s="46"/>
+      <c r="J178" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="B154:J154"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="B162:J162"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="B170:J170"/>
-    <mergeCell ref="B146:J146"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B114:J114"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="B122:J122"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="B130:J130"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="B138:J138"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="B98:J98"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A97:J97"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="B2:J2"/>
@@ -4585,6 +4555,38 @@
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B98:J98"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="B82:J82"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="B146:J146"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="B114:J114"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="B122:J122"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="B130:J130"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="B138:J138"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="B154:J154"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="B162:J162"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="B170:J170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add colliders in lvl 1, uren reg
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="54">
   <si>
     <t>Maandag</t>
   </si>
@@ -473,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -575,19 +575,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -869,7 +872,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -880,8 +883,8 @@
   <dimension ref="A1:O178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K65" sqref="K65"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -940,29 +943,29 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="49"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.98795180722891562</v>
+        <v>0.98830409356725146</v>
       </c>
       <c r="O2" s="9" t="s">
         <v>35</v>
@@ -1003,11 +1006,11 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.86746987951807231</v>
+        <v>0.87134502923976609</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>34</v>
@@ -1048,11 +1051,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.98795180722891562</v>
+        <v>0.98830409356725146</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>36</v>
@@ -1093,11 +1096,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.96385542168674698</v>
+        <v>0.96491228070175439</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>37</v>
@@ -1124,11 +1127,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.76506024096385539</v>
+        <v>0.77192982456140347</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>38</v>
@@ -1167,11 +1170,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.66867469879518071</v>
+        <v>0.67836257309941517</v>
       </c>
       <c r="O7" s="14" t="s">
         <v>39</v>
@@ -1218,41 +1221,41 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.97590361445783136</v>
+        <v>0.97660818713450293</v>
       </c>
       <c r="O8" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="49"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1459,30 +1462,30 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="49"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="47"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1687,30 +1690,30 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="49"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="47"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -1915,30 +1918,30 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="47"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="48"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="45"/>
-      <c r="J34" s="49"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="47"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2145,30 +2148,30 @@
       <c r="L40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A41" s="47"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
+      <c r="A41" s="48"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="48"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="49"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="47"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2377,30 +2380,30 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="47"/>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="47"/>
-      <c r="I49" s="47"/>
-      <c r="J49" s="47"/>
+      <c r="A49" s="48"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="48"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
-      <c r="J50" s="49"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="47"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2605,30 +2608,30 @@
       <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="47"/>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="47"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="47"/>
-      <c r="I57" s="47"/>
-      <c r="J57" s="47"/>
+      <c r="A57" s="48"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="48"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="49"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="47"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -2837,30 +2840,30 @@
       <c r="L64" s="8"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A65" s="47"/>
-      <c r="B65" s="47"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="47"/>
-      <c r="H65" s="47"/>
-      <c r="I65" s="47"/>
-      <c r="J65" s="47"/>
+      <c r="A65" s="48"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="48"/>
+      <c r="D65" s="48"/>
+      <c r="E65" s="48"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="48"/>
+      <c r="I65" s="48"/>
+      <c r="J65" s="48"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="48"/>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
-      <c r="F66" s="45"/>
-      <c r="G66" s="45"/>
-      <c r="H66" s="45"/>
-      <c r="I66" s="45"/>
-      <c r="J66" s="49"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="47"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -2995,39 +2998,48 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A73" s="47"/>
-      <c r="B73" s="47"/>
-      <c r="C73" s="47"/>
-      <c r="D73" s="47"/>
-      <c r="E73" s="47"/>
-      <c r="F73" s="47"/>
-      <c r="G73" s="47"/>
-      <c r="H73" s="47"/>
-      <c r="I73" s="47"/>
-      <c r="J73" s="47"/>
+      <c r="A73" s="48"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="48"/>
+      <c r="F73" s="48"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="48"/>
+      <c r="I73" s="48"/>
+      <c r="J73" s="48"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="48"/>
-      <c r="C74" s="45"/>
-      <c r="D74" s="45"/>
-      <c r="E74" s="45"/>
-      <c r="F74" s="45"/>
-      <c r="G74" s="45"/>
-      <c r="H74" s="45"/>
-      <c r="I74" s="45"/>
-      <c r="J74" s="49"/>
+      <c r="B74" s="45"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="46"/>
+      <c r="H74" s="46"/>
+      <c r="I74" s="46"/>
+      <c r="J74" s="47"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
     <row r="75" spans="1:12">
-      <c r="A75" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B75" s="8"/>
-      <c r="J75" s="1"/>
+      <c r="A75" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="21"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="40"/>
+      <c r="F75" s="40"/>
+      <c r="G75" s="40"/>
+      <c r="H75" s="40"/>
+      <c r="I75" s="40"/>
+      <c r="J75" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="K75" s="23"/>
       <c r="L75" s="8"/>
     </row>
@@ -3035,7 +3047,30 @@
       <c r="A76" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B76" s="8"/>
+      <c r="B76" s="8">
+        <v>5</v>
+      </c>
+      <c r="C76" s="6">
+        <v>5</v>
+      </c>
+      <c r="D76" s="6">
+        <v>5</v>
+      </c>
+      <c r="E76" s="6">
+        <v>5</v>
+      </c>
+      <c r="F76" s="6">
+        <v>5</v>
+      </c>
+      <c r="G76" s="6">
+        <v>5</v>
+      </c>
+      <c r="H76" s="50">
+        <v>5</v>
+      </c>
+      <c r="I76" s="6">
+        <v>5</v>
+      </c>
       <c r="J76" s="1"/>
       <c r="K76" s="23"/>
       <c r="L76" s="8"/>
@@ -3080,65 +3115,65 @@
       </c>
       <c r="B80" s="34">
         <f>B75+B76+B77+B78+B79</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C80" s="35">
         <f t="shared" ref="C80:H80" si="9">SUM(C75:C79)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D80" s="35">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E80" s="35">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F80" s="35">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G80" s="35">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H80" s="35">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I80" s="35">
         <f>SUM(I75:I79)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J80" s="36"/>
       <c r="K80" s="23"/>
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A81" s="47"/>
-      <c r="B81" s="47"/>
-      <c r="C81" s="47"/>
-      <c r="D81" s="47"/>
-      <c r="E81" s="47"/>
-      <c r="F81" s="47"/>
-      <c r="G81" s="47"/>
-      <c r="H81" s="47"/>
-      <c r="I81" s="47"/>
-      <c r="J81" s="47"/>
+      <c r="A81" s="48"/>
+      <c r="B81" s="48"/>
+      <c r="C81" s="48"/>
+      <c r="D81" s="48"/>
+      <c r="E81" s="48"/>
+      <c r="F81" s="48"/>
+      <c r="G81" s="48"/>
+      <c r="H81" s="48"/>
+      <c r="I81" s="48"/>
+      <c r="J81" s="48"/>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="48"/>
-      <c r="C82" s="45"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="45"/>
-      <c r="F82" s="45"/>
-      <c r="G82" s="45"/>
-      <c r="H82" s="45"/>
-      <c r="I82" s="45"/>
-      <c r="J82" s="49"/>
+      <c r="B82" s="45"/>
+      <c r="C82" s="46"/>
+      <c r="D82" s="46"/>
+      <c r="E82" s="46"/>
+      <c r="F82" s="46"/>
+      <c r="G82" s="46"/>
+      <c r="H82" s="46"/>
+      <c r="I82" s="46"/>
+      <c r="J82" s="47"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3235,30 +3270,30 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A89" s="47"/>
-      <c r="B89" s="47"/>
-      <c r="C89" s="47"/>
-      <c r="D89" s="47"/>
-      <c r="E89" s="47"/>
-      <c r="F89" s="47"/>
-      <c r="G89" s="47"/>
-      <c r="H89" s="47"/>
-      <c r="I89" s="47"/>
-      <c r="J89" s="47"/>
+      <c r="A89" s="48"/>
+      <c r="B89" s="48"/>
+      <c r="C89" s="48"/>
+      <c r="D89" s="48"/>
+      <c r="E89" s="48"/>
+      <c r="F89" s="48"/>
+      <c r="G89" s="48"/>
+      <c r="H89" s="48"/>
+      <c r="I89" s="48"/>
+      <c r="J89" s="48"/>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="48"/>
-      <c r="C90" s="45"/>
-      <c r="D90" s="45"/>
-      <c r="E90" s="45"/>
-      <c r="F90" s="45"/>
-      <c r="G90" s="45"/>
-      <c r="H90" s="45"/>
-      <c r="I90" s="45"/>
-      <c r="J90" s="49"/>
+      <c r="B90" s="45"/>
+      <c r="C90" s="46"/>
+      <c r="D90" s="46"/>
+      <c r="E90" s="46"/>
+      <c r="F90" s="46"/>
+      <c r="G90" s="46"/>
+      <c r="H90" s="46"/>
+      <c r="I90" s="46"/>
+      <c r="J90" s="47"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3355,30 +3390,30 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A97" s="47"/>
-      <c r="B97" s="47"/>
-      <c r="C97" s="47"/>
-      <c r="D97" s="47"/>
-      <c r="E97" s="47"/>
-      <c r="F97" s="47"/>
-      <c r="G97" s="47"/>
-      <c r="H97" s="47"/>
-      <c r="I97" s="47"/>
-      <c r="J97" s="47"/>
+      <c r="A97" s="48"/>
+      <c r="B97" s="48"/>
+      <c r="C97" s="48"/>
+      <c r="D97" s="48"/>
+      <c r="E97" s="48"/>
+      <c r="F97" s="48"/>
+      <c r="G97" s="48"/>
+      <c r="H97" s="48"/>
+      <c r="I97" s="48"/>
+      <c r="J97" s="48"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="48"/>
-      <c r="C98" s="45"/>
-      <c r="D98" s="45"/>
-      <c r="E98" s="45"/>
-      <c r="F98" s="45"/>
-      <c r="G98" s="45"/>
-      <c r="H98" s="45"/>
-      <c r="I98" s="45"/>
-      <c r="J98" s="49"/>
+      <c r="B98" s="45"/>
+      <c r="C98" s="46"/>
+      <c r="D98" s="46"/>
+      <c r="E98" s="46"/>
+      <c r="F98" s="46"/>
+      <c r="G98" s="46"/>
+      <c r="H98" s="46"/>
+      <c r="I98" s="46"/>
+      <c r="J98" s="47"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -3475,30 +3510,30 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A105" s="47"/>
-      <c r="B105" s="47"/>
-      <c r="C105" s="47"/>
-      <c r="D105" s="47"/>
-      <c r="E105" s="47"/>
-      <c r="F105" s="47"/>
-      <c r="G105" s="47"/>
-      <c r="H105" s="47"/>
-      <c r="I105" s="47"/>
-      <c r="J105" s="47"/>
+      <c r="A105" s="48"/>
+      <c r="B105" s="48"/>
+      <c r="C105" s="48"/>
+      <c r="D105" s="48"/>
+      <c r="E105" s="48"/>
+      <c r="F105" s="48"/>
+      <c r="G105" s="48"/>
+      <c r="H105" s="48"/>
+      <c r="I105" s="48"/>
+      <c r="J105" s="48"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="48"/>
-      <c r="C106" s="45"/>
-      <c r="D106" s="45"/>
-      <c r="E106" s="45"/>
-      <c r="F106" s="45"/>
-      <c r="G106" s="45"/>
-      <c r="H106" s="45"/>
-      <c r="I106" s="45"/>
-      <c r="J106" s="49"/>
+      <c r="B106" s="45"/>
+      <c r="C106" s="46"/>
+      <c r="D106" s="46"/>
+      <c r="E106" s="46"/>
+      <c r="F106" s="46"/>
+      <c r="G106" s="46"/>
+      <c r="H106" s="46"/>
+      <c r="I106" s="46"/>
+      <c r="J106" s="47"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -3595,30 +3630,30 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A113" s="47"/>
-      <c r="B113" s="47"/>
-      <c r="C113" s="47"/>
-      <c r="D113" s="47"/>
-      <c r="E113" s="47"/>
-      <c r="F113" s="47"/>
-      <c r="G113" s="47"/>
-      <c r="H113" s="47"/>
-      <c r="I113" s="47"/>
-      <c r="J113" s="47"/>
+      <c r="A113" s="48"/>
+      <c r="B113" s="48"/>
+      <c r="C113" s="48"/>
+      <c r="D113" s="48"/>
+      <c r="E113" s="48"/>
+      <c r="F113" s="48"/>
+      <c r="G113" s="48"/>
+      <c r="H113" s="48"/>
+      <c r="I113" s="48"/>
+      <c r="J113" s="48"/>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="48"/>
-      <c r="C114" s="45"/>
-      <c r="D114" s="45"/>
-      <c r="E114" s="45"/>
-      <c r="F114" s="45"/>
-      <c r="G114" s="45"/>
-      <c r="H114" s="45"/>
-      <c r="I114" s="45"/>
-      <c r="J114" s="49"/>
+      <c r="B114" s="45"/>
+      <c r="C114" s="46"/>
+      <c r="D114" s="46"/>
+      <c r="E114" s="46"/>
+      <c r="F114" s="46"/>
+      <c r="G114" s="46"/>
+      <c r="H114" s="46"/>
+      <c r="I114" s="46"/>
+      <c r="J114" s="47"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -3715,30 +3750,30 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A121" s="47"/>
-      <c r="B121" s="47"/>
-      <c r="C121" s="47"/>
-      <c r="D121" s="47"/>
-      <c r="E121" s="47"/>
-      <c r="F121" s="47"/>
-      <c r="G121" s="47"/>
-      <c r="H121" s="47"/>
-      <c r="I121" s="47"/>
-      <c r="J121" s="47"/>
+      <c r="A121" s="48"/>
+      <c r="B121" s="48"/>
+      <c r="C121" s="48"/>
+      <c r="D121" s="48"/>
+      <c r="E121" s="48"/>
+      <c r="F121" s="48"/>
+      <c r="G121" s="48"/>
+      <c r="H121" s="48"/>
+      <c r="I121" s="48"/>
+      <c r="J121" s="48"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="48"/>
-      <c r="C122" s="45"/>
-      <c r="D122" s="45"/>
-      <c r="E122" s="45"/>
-      <c r="F122" s="45"/>
-      <c r="G122" s="45"/>
-      <c r="H122" s="45"/>
-      <c r="I122" s="45"/>
-      <c r="J122" s="49"/>
+      <c r="B122" s="45"/>
+      <c r="C122" s="46"/>
+      <c r="D122" s="46"/>
+      <c r="E122" s="46"/>
+      <c r="F122" s="46"/>
+      <c r="G122" s="46"/>
+      <c r="H122" s="46"/>
+      <c r="I122" s="46"/>
+      <c r="J122" s="47"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -3835,30 +3870,30 @@
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A129" s="47"/>
-      <c r="B129" s="47"/>
-      <c r="C129" s="47"/>
-      <c r="D129" s="47"/>
-      <c r="E129" s="47"/>
-      <c r="F129" s="47"/>
-      <c r="G129" s="47"/>
-      <c r="H129" s="47"/>
-      <c r="I129" s="47"/>
-      <c r="J129" s="47"/>
+      <c r="A129" s="48"/>
+      <c r="B129" s="48"/>
+      <c r="C129" s="48"/>
+      <c r="D129" s="48"/>
+      <c r="E129" s="48"/>
+      <c r="F129" s="48"/>
+      <c r="G129" s="48"/>
+      <c r="H129" s="48"/>
+      <c r="I129" s="48"/>
+      <c r="J129" s="48"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="48"/>
-      <c r="C130" s="45"/>
-      <c r="D130" s="45"/>
-      <c r="E130" s="45"/>
-      <c r="F130" s="45"/>
-      <c r="G130" s="45"/>
-      <c r="H130" s="45"/>
-      <c r="I130" s="45"/>
-      <c r="J130" s="49"/>
+      <c r="B130" s="45"/>
+      <c r="C130" s="46"/>
+      <c r="D130" s="46"/>
+      <c r="E130" s="46"/>
+      <c r="F130" s="46"/>
+      <c r="G130" s="46"/>
+      <c r="H130" s="46"/>
+      <c r="I130" s="46"/>
+      <c r="J130" s="47"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -3955,30 +3990,30 @@
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A137" s="47"/>
-      <c r="B137" s="47"/>
-      <c r="C137" s="47"/>
-      <c r="D137" s="47"/>
-      <c r="E137" s="47"/>
-      <c r="F137" s="47"/>
-      <c r="G137" s="47"/>
-      <c r="H137" s="47"/>
-      <c r="I137" s="47"/>
-      <c r="J137" s="47"/>
+      <c r="A137" s="48"/>
+      <c r="B137" s="48"/>
+      <c r="C137" s="48"/>
+      <c r="D137" s="48"/>
+      <c r="E137" s="48"/>
+      <c r="F137" s="48"/>
+      <c r="G137" s="48"/>
+      <c r="H137" s="48"/>
+      <c r="I137" s="48"/>
+      <c r="J137" s="48"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="48"/>
-      <c r="C138" s="45"/>
-      <c r="D138" s="45"/>
-      <c r="E138" s="45"/>
-      <c r="F138" s="45"/>
-      <c r="G138" s="45"/>
-      <c r="H138" s="45"/>
-      <c r="I138" s="45"/>
-      <c r="J138" s="49"/>
+      <c r="B138" s="45"/>
+      <c r="C138" s="46"/>
+      <c r="D138" s="46"/>
+      <c r="E138" s="46"/>
+      <c r="F138" s="46"/>
+      <c r="G138" s="46"/>
+      <c r="H138" s="46"/>
+      <c r="I138" s="46"/>
+      <c r="J138" s="47"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -4075,30 +4110,30 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A145" s="47"/>
-      <c r="B145" s="47"/>
-      <c r="C145" s="47"/>
-      <c r="D145" s="47"/>
-      <c r="E145" s="47"/>
-      <c r="F145" s="47"/>
-      <c r="G145" s="47"/>
-      <c r="H145" s="47"/>
-      <c r="I145" s="47"/>
-      <c r="J145" s="47"/>
+      <c r="A145" s="48"/>
+      <c r="B145" s="48"/>
+      <c r="C145" s="48"/>
+      <c r="D145" s="48"/>
+      <c r="E145" s="48"/>
+      <c r="F145" s="48"/>
+      <c r="G145" s="48"/>
+      <c r="H145" s="48"/>
+      <c r="I145" s="48"/>
+      <c r="J145" s="48"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="48"/>
-      <c r="C146" s="45"/>
-      <c r="D146" s="45"/>
-      <c r="E146" s="45"/>
-      <c r="F146" s="45"/>
-      <c r="G146" s="45"/>
-      <c r="H146" s="45"/>
-      <c r="I146" s="45"/>
-      <c r="J146" s="49"/>
+      <c r="B146" s="45"/>
+      <c r="C146" s="46"/>
+      <c r="D146" s="46"/>
+      <c r="E146" s="46"/>
+      <c r="F146" s="46"/>
+      <c r="G146" s="46"/>
+      <c r="H146" s="46"/>
+      <c r="I146" s="46"/>
+      <c r="J146" s="47"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -4195,30 +4230,30 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A153" s="47"/>
-      <c r="B153" s="47"/>
-      <c r="C153" s="47"/>
-      <c r="D153" s="47"/>
-      <c r="E153" s="47"/>
-      <c r="F153" s="47"/>
-      <c r="G153" s="47"/>
-      <c r="H153" s="47"/>
-      <c r="I153" s="47"/>
-      <c r="J153" s="47"/>
+      <c r="A153" s="48"/>
+      <c r="B153" s="48"/>
+      <c r="C153" s="48"/>
+      <c r="D153" s="48"/>
+      <c r="E153" s="48"/>
+      <c r="F153" s="48"/>
+      <c r="G153" s="48"/>
+      <c r="H153" s="48"/>
+      <c r="I153" s="48"/>
+      <c r="J153" s="48"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="48"/>
-      <c r="C154" s="45"/>
-      <c r="D154" s="45"/>
-      <c r="E154" s="45"/>
-      <c r="F154" s="45"/>
-      <c r="G154" s="45"/>
-      <c r="H154" s="45"/>
-      <c r="I154" s="45"/>
-      <c r="J154" s="49"/>
+      <c r="B154" s="45"/>
+      <c r="C154" s="46"/>
+      <c r="D154" s="46"/>
+      <c r="E154" s="46"/>
+      <c r="F154" s="46"/>
+      <c r="G154" s="46"/>
+      <c r="H154" s="46"/>
+      <c r="I154" s="46"/>
+      <c r="J154" s="47"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -4315,30 +4350,30 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A161" s="47"/>
-      <c r="B161" s="47"/>
-      <c r="C161" s="47"/>
-      <c r="D161" s="47"/>
-      <c r="E161" s="47"/>
-      <c r="F161" s="47"/>
-      <c r="G161" s="47"/>
-      <c r="H161" s="47"/>
-      <c r="I161" s="47"/>
-      <c r="J161" s="47"/>
+      <c r="A161" s="48"/>
+      <c r="B161" s="48"/>
+      <c r="C161" s="48"/>
+      <c r="D161" s="48"/>
+      <c r="E161" s="48"/>
+      <c r="F161" s="48"/>
+      <c r="G161" s="48"/>
+      <c r="H161" s="48"/>
+      <c r="I161" s="48"/>
+      <c r="J161" s="48"/>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="48"/>
-      <c r="C162" s="45"/>
-      <c r="D162" s="45"/>
-      <c r="E162" s="45"/>
-      <c r="F162" s="45"/>
-      <c r="G162" s="45"/>
-      <c r="H162" s="45"/>
-      <c r="I162" s="45"/>
-      <c r="J162" s="49"/>
+      <c r="B162" s="45"/>
+      <c r="C162" s="46"/>
+      <c r="D162" s="46"/>
+      <c r="E162" s="46"/>
+      <c r="F162" s="46"/>
+      <c r="G162" s="46"/>
+      <c r="H162" s="46"/>
+      <c r="I162" s="46"/>
+      <c r="J162" s="47"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -4435,30 +4470,30 @@
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A169" s="47"/>
-      <c r="B169" s="47"/>
-      <c r="C169" s="47"/>
-      <c r="D169" s="47"/>
-      <c r="E169" s="47"/>
-      <c r="F169" s="47"/>
-      <c r="G169" s="47"/>
-      <c r="H169" s="47"/>
-      <c r="I169" s="47"/>
-      <c r="J169" s="47"/>
+      <c r="A169" s="48"/>
+      <c r="B169" s="48"/>
+      <c r="C169" s="48"/>
+      <c r="D169" s="48"/>
+      <c r="E169" s="48"/>
+      <c r="F169" s="48"/>
+      <c r="G169" s="48"/>
+      <c r="H169" s="48"/>
+      <c r="I169" s="48"/>
+      <c r="J169" s="48"/>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="48"/>
-      <c r="C170" s="45"/>
-      <c r="D170" s="45"/>
-      <c r="E170" s="45"/>
-      <c r="F170" s="45"/>
-      <c r="G170" s="45"/>
-      <c r="H170" s="45"/>
-      <c r="I170" s="45"/>
-      <c r="J170" s="49"/>
+      <c r="B170" s="45"/>
+      <c r="C170" s="46"/>
+      <c r="D170" s="46"/>
+      <c r="E170" s="46"/>
+      <c r="F170" s="46"/>
+      <c r="G170" s="46"/>
+      <c r="H170" s="46"/>
+      <c r="I170" s="46"/>
+      <c r="J170" s="47"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -4555,31 +4590,63 @@
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="45"/>
-      <c r="B177" s="45"/>
-      <c r="C177" s="45"/>
-      <c r="D177" s="45"/>
-      <c r="E177" s="45"/>
-      <c r="F177" s="45"/>
-      <c r="G177" s="45"/>
-      <c r="H177" s="45"/>
-      <c r="I177" s="45"/>
-      <c r="J177" s="45"/>
+      <c r="A177" s="46"/>
+      <c r="B177" s="46"/>
+      <c r="C177" s="46"/>
+      <c r="D177" s="46"/>
+      <c r="E177" s="46"/>
+      <c r="F177" s="46"/>
+      <c r="G177" s="46"/>
+      <c r="H177" s="46"/>
+      <c r="I177" s="46"/>
+      <c r="J177" s="46"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="46"/>
-      <c r="B178" s="46"/>
-      <c r="C178" s="46"/>
-      <c r="D178" s="46"/>
-      <c r="E178" s="46"/>
-      <c r="F178" s="46"/>
-      <c r="G178" s="46"/>
-      <c r="H178" s="46"/>
-      <c r="I178" s="46"/>
-      <c r="J178" s="46"/>
+      <c r="A178" s="49"/>
+      <c r="B178" s="49"/>
+      <c r="C178" s="49"/>
+      <c r="D178" s="49"/>
+      <c r="E178" s="49"/>
+      <c r="F178" s="49"/>
+      <c r="G178" s="49"/>
+      <c r="H178" s="49"/>
+      <c r="I178" s="49"/>
+      <c r="J178" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="B154:J154"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="B162:J162"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="B170:J170"/>
+    <mergeCell ref="B146:J146"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="B114:J114"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="B122:J122"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="B130:J130"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="B138:J138"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="B98:J98"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="B82:J82"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A97:J97"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="B2:J2"/>
@@ -4593,38 +4660,6 @@
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B98:J98"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A97:J97"/>
-    <mergeCell ref="B146:J146"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B114:J114"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="B122:J122"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="B130:J130"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="B138:J138"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="B154:J154"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="B162:J162"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="B170:J170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Level 1, uren reg
test player added to lvl 1,
colider fix lvl 1
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -473,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -575,6 +575,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -590,7 +593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -883,8 +886,8 @@
   <dimension ref="A1:O178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -943,29 +946,29 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.98830409356725146</v>
+        <v>0.98863636363636365</v>
       </c>
       <c r="O2" s="9" t="s">
         <v>35</v>
@@ -1006,11 +1009,11 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.87134502923976609</v>
+        <v>0.875</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>34</v>
@@ -1051,11 +1054,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.98830409356725146</v>
+        <v>0.98863636363636365</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>36</v>
@@ -1100,7 +1103,7 @@
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.96491228070175439</v>
+        <v>0.9375</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>37</v>
@@ -1131,7 +1134,7 @@
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.77192982456140347</v>
+        <v>0.75</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>38</v>
@@ -1174,7 +1177,7 @@
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.67836257309941517</v>
+        <v>0.65909090909090906</v>
       </c>
       <c r="O7" s="14" t="s">
         <v>39</v>
@@ -1221,41 +1224,41 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.97660818713450293</v>
+        <v>0.97727272727272729</v>
       </c>
       <c r="O8" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="48"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1462,30 +1465,30 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="47"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="48"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1690,30 +1693,30 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="48"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="47"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="48"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -1918,30 +1921,30 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="48"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="47"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="48"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2148,30 +2151,30 @@
       <c r="L40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A41" s="48"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="45"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="47"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="48"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2380,30 +2383,30 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="48"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
+      <c r="A49" s="49"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="49"/>
+      <c r="J49" s="49"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="46"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="47"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="48"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2608,30 +2611,30 @@
       <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="48"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="48"/>
-      <c r="J57" s="48"/>
+      <c r="A57" s="49"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="49"/>
+      <c r="I57" s="49"/>
+      <c r="J57" s="49"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="45"/>
-      <c r="C58" s="46"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="46"/>
-      <c r="F58" s="46"/>
-      <c r="G58" s="46"/>
-      <c r="H58" s="46"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="47"/>
+      <c r="B58" s="46"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="47"/>
+      <c r="J58" s="48"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -2840,30 +2843,30 @@
       <c r="L64" s="8"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A65" s="48"/>
-      <c r="B65" s="48"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="48"/>
-      <c r="H65" s="48"/>
-      <c r="I65" s="48"/>
-      <c r="J65" s="48"/>
+      <c r="A65" s="49"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49"/>
+      <c r="I65" s="49"/>
+      <c r="J65" s="49"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="45"/>
-      <c r="C66" s="46"/>
-      <c r="D66" s="46"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="46"/>
-      <c r="H66" s="46"/>
-      <c r="I66" s="46"/>
-      <c r="J66" s="47"/>
+      <c r="B66" s="46"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="47"/>
+      <c r="I66" s="47"/>
+      <c r="J66" s="48"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -2998,30 +3001,30 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A73" s="48"/>
-      <c r="B73" s="48"/>
-      <c r="C73" s="48"/>
-      <c r="D73" s="48"/>
-      <c r="E73" s="48"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="48"/>
-      <c r="H73" s="48"/>
-      <c r="I73" s="48"/>
-      <c r="J73" s="48"/>
+      <c r="A73" s="49"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="49"/>
+      <c r="E73" s="49"/>
+      <c r="F73" s="49"/>
+      <c r="G73" s="49"/>
+      <c r="H73" s="49"/>
+      <c r="I73" s="49"/>
+      <c r="J73" s="49"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="45"/>
-      <c r="C74" s="46"/>
-      <c r="D74" s="46"/>
-      <c r="E74" s="46"/>
-      <c r="F74" s="46"/>
-      <c r="G74" s="46"/>
-      <c r="H74" s="46"/>
-      <c r="I74" s="46"/>
-      <c r="J74" s="47"/>
+      <c r="B74" s="46"/>
+      <c r="C74" s="47"/>
+      <c r="D74" s="47"/>
+      <c r="E74" s="47"/>
+      <c r="F74" s="47"/>
+      <c r="G74" s="47"/>
+      <c r="H74" s="47"/>
+      <c r="I74" s="47"/>
+      <c r="J74" s="48"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3065,7 +3068,7 @@
       <c r="G76" s="6">
         <v>5</v>
       </c>
-      <c r="H76" s="50">
+      <c r="H76" s="45">
         <v>5</v>
       </c>
       <c r="I76" s="6">
@@ -3079,7 +3082,26 @@
       <c r="A77" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B77" s="8"/>
+      <c r="B77" s="8">
+        <v>5</v>
+      </c>
+      <c r="C77" s="6">
+        <v>5</v>
+      </c>
+      <c r="D77" s="6">
+        <v>5</v>
+      </c>
+      <c r="E77" s="6">
+        <v>5</v>
+      </c>
+      <c r="F77" s="51"/>
+      <c r="G77" s="28">
+        <v>0</v>
+      </c>
+      <c r="H77" s="51"/>
+      <c r="I77" s="6">
+        <v>5</v>
+      </c>
       <c r="J77" s="1"/>
       <c r="K77" s="23"/>
       <c r="L77" s="8"/>
@@ -3115,19 +3137,19 @@
       </c>
       <c r="B80" s="34">
         <f>B75+B76+B77+B78+B79</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C80" s="35">
         <f t="shared" ref="C80:H80" si="9">SUM(C75:C79)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D80" s="35">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E80" s="35">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F80" s="35">
         <f t="shared" si="9"/>
@@ -3143,37 +3165,37 @@
       </c>
       <c r="I80" s="35">
         <f>SUM(I75:I79)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J80" s="36"/>
       <c r="K80" s="23"/>
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A81" s="48"/>
-      <c r="B81" s="48"/>
-      <c r="C81" s="48"/>
-      <c r="D81" s="48"/>
-      <c r="E81" s="48"/>
-      <c r="F81" s="48"/>
-      <c r="G81" s="48"/>
-      <c r="H81" s="48"/>
-      <c r="I81" s="48"/>
-      <c r="J81" s="48"/>
+      <c r="A81" s="49"/>
+      <c r="B81" s="49"/>
+      <c r="C81" s="49"/>
+      <c r="D81" s="49"/>
+      <c r="E81" s="49"/>
+      <c r="F81" s="49"/>
+      <c r="G81" s="49"/>
+      <c r="H81" s="49"/>
+      <c r="I81" s="49"/>
+      <c r="J81" s="49"/>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="45"/>
-      <c r="C82" s="46"/>
-      <c r="D82" s="46"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="46"/>
-      <c r="G82" s="46"/>
-      <c r="H82" s="46"/>
-      <c r="I82" s="46"/>
-      <c r="J82" s="47"/>
+      <c r="B82" s="46"/>
+      <c r="C82" s="47"/>
+      <c r="D82" s="47"/>
+      <c r="E82" s="47"/>
+      <c r="F82" s="47"/>
+      <c r="G82" s="47"/>
+      <c r="H82" s="47"/>
+      <c r="I82" s="47"/>
+      <c r="J82" s="48"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3270,30 +3292,30 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A89" s="48"/>
-      <c r="B89" s="48"/>
-      <c r="C89" s="48"/>
-      <c r="D89" s="48"/>
-      <c r="E89" s="48"/>
-      <c r="F89" s="48"/>
-      <c r="G89" s="48"/>
-      <c r="H89" s="48"/>
-      <c r="I89" s="48"/>
-      <c r="J89" s="48"/>
+      <c r="A89" s="49"/>
+      <c r="B89" s="49"/>
+      <c r="C89" s="49"/>
+      <c r="D89" s="49"/>
+      <c r="E89" s="49"/>
+      <c r="F89" s="49"/>
+      <c r="G89" s="49"/>
+      <c r="H89" s="49"/>
+      <c r="I89" s="49"/>
+      <c r="J89" s="49"/>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="45"/>
-      <c r="C90" s="46"/>
-      <c r="D90" s="46"/>
-      <c r="E90" s="46"/>
-      <c r="F90" s="46"/>
-      <c r="G90" s="46"/>
-      <c r="H90" s="46"/>
-      <c r="I90" s="46"/>
-      <c r="J90" s="47"/>
+      <c r="B90" s="46"/>
+      <c r="C90" s="47"/>
+      <c r="D90" s="47"/>
+      <c r="E90" s="47"/>
+      <c r="F90" s="47"/>
+      <c r="G90" s="47"/>
+      <c r="H90" s="47"/>
+      <c r="I90" s="47"/>
+      <c r="J90" s="48"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3390,30 +3412,30 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A97" s="48"/>
-      <c r="B97" s="48"/>
-      <c r="C97" s="48"/>
-      <c r="D97" s="48"/>
-      <c r="E97" s="48"/>
-      <c r="F97" s="48"/>
-      <c r="G97" s="48"/>
-      <c r="H97" s="48"/>
-      <c r="I97" s="48"/>
-      <c r="J97" s="48"/>
+      <c r="A97" s="49"/>
+      <c r="B97" s="49"/>
+      <c r="C97" s="49"/>
+      <c r="D97" s="49"/>
+      <c r="E97" s="49"/>
+      <c r="F97" s="49"/>
+      <c r="G97" s="49"/>
+      <c r="H97" s="49"/>
+      <c r="I97" s="49"/>
+      <c r="J97" s="49"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="45"/>
-      <c r="C98" s="46"/>
-      <c r="D98" s="46"/>
-      <c r="E98" s="46"/>
-      <c r="F98" s="46"/>
-      <c r="G98" s="46"/>
-      <c r="H98" s="46"/>
-      <c r="I98" s="46"/>
-      <c r="J98" s="47"/>
+      <c r="B98" s="46"/>
+      <c r="C98" s="47"/>
+      <c r="D98" s="47"/>
+      <c r="E98" s="47"/>
+      <c r="F98" s="47"/>
+      <c r="G98" s="47"/>
+      <c r="H98" s="47"/>
+      <c r="I98" s="47"/>
+      <c r="J98" s="48"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -3510,30 +3532,30 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A105" s="48"/>
-      <c r="B105" s="48"/>
-      <c r="C105" s="48"/>
-      <c r="D105" s="48"/>
-      <c r="E105" s="48"/>
-      <c r="F105" s="48"/>
-      <c r="G105" s="48"/>
-      <c r="H105" s="48"/>
-      <c r="I105" s="48"/>
-      <c r="J105" s="48"/>
+      <c r="A105" s="49"/>
+      <c r="B105" s="49"/>
+      <c r="C105" s="49"/>
+      <c r="D105" s="49"/>
+      <c r="E105" s="49"/>
+      <c r="F105" s="49"/>
+      <c r="G105" s="49"/>
+      <c r="H105" s="49"/>
+      <c r="I105" s="49"/>
+      <c r="J105" s="49"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="45"/>
-      <c r="C106" s="46"/>
-      <c r="D106" s="46"/>
-      <c r="E106" s="46"/>
-      <c r="F106" s="46"/>
-      <c r="G106" s="46"/>
-      <c r="H106" s="46"/>
-      <c r="I106" s="46"/>
-      <c r="J106" s="47"/>
+      <c r="B106" s="46"/>
+      <c r="C106" s="47"/>
+      <c r="D106" s="47"/>
+      <c r="E106" s="47"/>
+      <c r="F106" s="47"/>
+      <c r="G106" s="47"/>
+      <c r="H106" s="47"/>
+      <c r="I106" s="47"/>
+      <c r="J106" s="48"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -3630,30 +3652,30 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A113" s="48"/>
-      <c r="B113" s="48"/>
-      <c r="C113" s="48"/>
-      <c r="D113" s="48"/>
-      <c r="E113" s="48"/>
-      <c r="F113" s="48"/>
-      <c r="G113" s="48"/>
-      <c r="H113" s="48"/>
-      <c r="I113" s="48"/>
-      <c r="J113" s="48"/>
+      <c r="A113" s="49"/>
+      <c r="B113" s="49"/>
+      <c r="C113" s="49"/>
+      <c r="D113" s="49"/>
+      <c r="E113" s="49"/>
+      <c r="F113" s="49"/>
+      <c r="G113" s="49"/>
+      <c r="H113" s="49"/>
+      <c r="I113" s="49"/>
+      <c r="J113" s="49"/>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="45"/>
-      <c r="C114" s="46"/>
-      <c r="D114" s="46"/>
-      <c r="E114" s="46"/>
-      <c r="F114" s="46"/>
-      <c r="G114" s="46"/>
-      <c r="H114" s="46"/>
-      <c r="I114" s="46"/>
-      <c r="J114" s="47"/>
+      <c r="B114" s="46"/>
+      <c r="C114" s="47"/>
+      <c r="D114" s="47"/>
+      <c r="E114" s="47"/>
+      <c r="F114" s="47"/>
+      <c r="G114" s="47"/>
+      <c r="H114" s="47"/>
+      <c r="I114" s="47"/>
+      <c r="J114" s="48"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -3750,30 +3772,30 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A121" s="48"/>
-      <c r="B121" s="48"/>
-      <c r="C121" s="48"/>
-      <c r="D121" s="48"/>
-      <c r="E121" s="48"/>
-      <c r="F121" s="48"/>
-      <c r="G121" s="48"/>
-      <c r="H121" s="48"/>
-      <c r="I121" s="48"/>
-      <c r="J121" s="48"/>
+      <c r="A121" s="49"/>
+      <c r="B121" s="49"/>
+      <c r="C121" s="49"/>
+      <c r="D121" s="49"/>
+      <c r="E121" s="49"/>
+      <c r="F121" s="49"/>
+      <c r="G121" s="49"/>
+      <c r="H121" s="49"/>
+      <c r="I121" s="49"/>
+      <c r="J121" s="49"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="45"/>
-      <c r="C122" s="46"/>
-      <c r="D122" s="46"/>
-      <c r="E122" s="46"/>
-      <c r="F122" s="46"/>
-      <c r="G122" s="46"/>
-      <c r="H122" s="46"/>
-      <c r="I122" s="46"/>
-      <c r="J122" s="47"/>
+      <c r="B122" s="46"/>
+      <c r="C122" s="47"/>
+      <c r="D122" s="47"/>
+      <c r="E122" s="47"/>
+      <c r="F122" s="47"/>
+      <c r="G122" s="47"/>
+      <c r="H122" s="47"/>
+      <c r="I122" s="47"/>
+      <c r="J122" s="48"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -3870,30 +3892,30 @@
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A129" s="48"/>
-      <c r="B129" s="48"/>
-      <c r="C129" s="48"/>
-      <c r="D129" s="48"/>
-      <c r="E129" s="48"/>
-      <c r="F129" s="48"/>
-      <c r="G129" s="48"/>
-      <c r="H129" s="48"/>
-      <c r="I129" s="48"/>
-      <c r="J129" s="48"/>
+      <c r="A129" s="49"/>
+      <c r="B129" s="49"/>
+      <c r="C129" s="49"/>
+      <c r="D129" s="49"/>
+      <c r="E129" s="49"/>
+      <c r="F129" s="49"/>
+      <c r="G129" s="49"/>
+      <c r="H129" s="49"/>
+      <c r="I129" s="49"/>
+      <c r="J129" s="49"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="45"/>
-      <c r="C130" s="46"/>
-      <c r="D130" s="46"/>
-      <c r="E130" s="46"/>
-      <c r="F130" s="46"/>
-      <c r="G130" s="46"/>
-      <c r="H130" s="46"/>
-      <c r="I130" s="46"/>
-      <c r="J130" s="47"/>
+      <c r="B130" s="46"/>
+      <c r="C130" s="47"/>
+      <c r="D130" s="47"/>
+      <c r="E130" s="47"/>
+      <c r="F130" s="47"/>
+      <c r="G130" s="47"/>
+      <c r="H130" s="47"/>
+      <c r="I130" s="47"/>
+      <c r="J130" s="48"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -3990,30 +4012,30 @@
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A137" s="48"/>
-      <c r="B137" s="48"/>
-      <c r="C137" s="48"/>
-      <c r="D137" s="48"/>
-      <c r="E137" s="48"/>
-      <c r="F137" s="48"/>
-      <c r="G137" s="48"/>
-      <c r="H137" s="48"/>
-      <c r="I137" s="48"/>
-      <c r="J137" s="48"/>
+      <c r="A137" s="49"/>
+      <c r="B137" s="49"/>
+      <c r="C137" s="49"/>
+      <c r="D137" s="49"/>
+      <c r="E137" s="49"/>
+      <c r="F137" s="49"/>
+      <c r="G137" s="49"/>
+      <c r="H137" s="49"/>
+      <c r="I137" s="49"/>
+      <c r="J137" s="49"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="45"/>
-      <c r="C138" s="46"/>
-      <c r="D138" s="46"/>
-      <c r="E138" s="46"/>
-      <c r="F138" s="46"/>
-      <c r="G138" s="46"/>
-      <c r="H138" s="46"/>
-      <c r="I138" s="46"/>
-      <c r="J138" s="47"/>
+      <c r="B138" s="46"/>
+      <c r="C138" s="47"/>
+      <c r="D138" s="47"/>
+      <c r="E138" s="47"/>
+      <c r="F138" s="47"/>
+      <c r="G138" s="47"/>
+      <c r="H138" s="47"/>
+      <c r="I138" s="47"/>
+      <c r="J138" s="48"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -4110,30 +4132,30 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A145" s="48"/>
-      <c r="B145" s="48"/>
-      <c r="C145" s="48"/>
-      <c r="D145" s="48"/>
-      <c r="E145" s="48"/>
-      <c r="F145" s="48"/>
-      <c r="G145" s="48"/>
-      <c r="H145" s="48"/>
-      <c r="I145" s="48"/>
-      <c r="J145" s="48"/>
+      <c r="A145" s="49"/>
+      <c r="B145" s="49"/>
+      <c r="C145" s="49"/>
+      <c r="D145" s="49"/>
+      <c r="E145" s="49"/>
+      <c r="F145" s="49"/>
+      <c r="G145" s="49"/>
+      <c r="H145" s="49"/>
+      <c r="I145" s="49"/>
+      <c r="J145" s="49"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="45"/>
-      <c r="C146" s="46"/>
-      <c r="D146" s="46"/>
-      <c r="E146" s="46"/>
-      <c r="F146" s="46"/>
-      <c r="G146" s="46"/>
-      <c r="H146" s="46"/>
-      <c r="I146" s="46"/>
-      <c r="J146" s="47"/>
+      <c r="B146" s="46"/>
+      <c r="C146" s="47"/>
+      <c r="D146" s="47"/>
+      <c r="E146" s="47"/>
+      <c r="F146" s="47"/>
+      <c r="G146" s="47"/>
+      <c r="H146" s="47"/>
+      <c r="I146" s="47"/>
+      <c r="J146" s="48"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -4230,30 +4252,30 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A153" s="48"/>
-      <c r="B153" s="48"/>
-      <c r="C153" s="48"/>
-      <c r="D153" s="48"/>
-      <c r="E153" s="48"/>
-      <c r="F153" s="48"/>
-      <c r="G153" s="48"/>
-      <c r="H153" s="48"/>
-      <c r="I153" s="48"/>
-      <c r="J153" s="48"/>
+      <c r="A153" s="49"/>
+      <c r="B153" s="49"/>
+      <c r="C153" s="49"/>
+      <c r="D153" s="49"/>
+      <c r="E153" s="49"/>
+      <c r="F153" s="49"/>
+      <c r="G153" s="49"/>
+      <c r="H153" s="49"/>
+      <c r="I153" s="49"/>
+      <c r="J153" s="49"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="45"/>
-      <c r="C154" s="46"/>
-      <c r="D154" s="46"/>
-      <c r="E154" s="46"/>
-      <c r="F154" s="46"/>
-      <c r="G154" s="46"/>
-      <c r="H154" s="46"/>
-      <c r="I154" s="46"/>
-      <c r="J154" s="47"/>
+      <c r="B154" s="46"/>
+      <c r="C154" s="47"/>
+      <c r="D154" s="47"/>
+      <c r="E154" s="47"/>
+      <c r="F154" s="47"/>
+      <c r="G154" s="47"/>
+      <c r="H154" s="47"/>
+      <c r="I154" s="47"/>
+      <c r="J154" s="48"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -4350,30 +4372,30 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A161" s="48"/>
-      <c r="B161" s="48"/>
-      <c r="C161" s="48"/>
-      <c r="D161" s="48"/>
-      <c r="E161" s="48"/>
-      <c r="F161" s="48"/>
-      <c r="G161" s="48"/>
-      <c r="H161" s="48"/>
-      <c r="I161" s="48"/>
-      <c r="J161" s="48"/>
+      <c r="A161" s="49"/>
+      <c r="B161" s="49"/>
+      <c r="C161" s="49"/>
+      <c r="D161" s="49"/>
+      <c r="E161" s="49"/>
+      <c r="F161" s="49"/>
+      <c r="G161" s="49"/>
+      <c r="H161" s="49"/>
+      <c r="I161" s="49"/>
+      <c r="J161" s="49"/>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="45"/>
-      <c r="C162" s="46"/>
-      <c r="D162" s="46"/>
-      <c r="E162" s="46"/>
-      <c r="F162" s="46"/>
-      <c r="G162" s="46"/>
-      <c r="H162" s="46"/>
-      <c r="I162" s="46"/>
-      <c r="J162" s="47"/>
+      <c r="B162" s="46"/>
+      <c r="C162" s="47"/>
+      <c r="D162" s="47"/>
+      <c r="E162" s="47"/>
+      <c r="F162" s="47"/>
+      <c r="G162" s="47"/>
+      <c r="H162" s="47"/>
+      <c r="I162" s="47"/>
+      <c r="J162" s="48"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -4470,30 +4492,30 @@
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A169" s="48"/>
-      <c r="B169" s="48"/>
-      <c r="C169" s="48"/>
-      <c r="D169" s="48"/>
-      <c r="E169" s="48"/>
-      <c r="F169" s="48"/>
-      <c r="G169" s="48"/>
-      <c r="H169" s="48"/>
-      <c r="I169" s="48"/>
-      <c r="J169" s="48"/>
+      <c r="A169" s="49"/>
+      <c r="B169" s="49"/>
+      <c r="C169" s="49"/>
+      <c r="D169" s="49"/>
+      <c r="E169" s="49"/>
+      <c r="F169" s="49"/>
+      <c r="G169" s="49"/>
+      <c r="H169" s="49"/>
+      <c r="I169" s="49"/>
+      <c r="J169" s="49"/>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="45"/>
-      <c r="C170" s="46"/>
-      <c r="D170" s="46"/>
-      <c r="E170" s="46"/>
-      <c r="F170" s="46"/>
-      <c r="G170" s="46"/>
-      <c r="H170" s="46"/>
-      <c r="I170" s="46"/>
-      <c r="J170" s="47"/>
+      <c r="B170" s="46"/>
+      <c r="C170" s="47"/>
+      <c r="D170" s="47"/>
+      <c r="E170" s="47"/>
+      <c r="F170" s="47"/>
+      <c r="G170" s="47"/>
+      <c r="H170" s="47"/>
+      <c r="I170" s="47"/>
+      <c r="J170" s="48"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -4590,28 +4612,28 @@
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="46"/>
-      <c r="B177" s="46"/>
-      <c r="C177" s="46"/>
-      <c r="D177" s="46"/>
-      <c r="E177" s="46"/>
-      <c r="F177" s="46"/>
-      <c r="G177" s="46"/>
-      <c r="H177" s="46"/>
-      <c r="I177" s="46"/>
-      <c r="J177" s="46"/>
+      <c r="A177" s="47"/>
+      <c r="B177" s="47"/>
+      <c r="C177" s="47"/>
+      <c r="D177" s="47"/>
+      <c r="E177" s="47"/>
+      <c r="F177" s="47"/>
+      <c r="G177" s="47"/>
+      <c r="H177" s="47"/>
+      <c r="I177" s="47"/>
+      <c r="J177" s="47"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="49"/>
-      <c r="B178" s="49"/>
-      <c r="C178" s="49"/>
-      <c r="D178" s="49"/>
-      <c r="E178" s="49"/>
-      <c r="F178" s="49"/>
-      <c r="G178" s="49"/>
-      <c r="H178" s="49"/>
-      <c r="I178" s="49"/>
-      <c r="J178" s="49"/>
+      <c r="A178" s="50"/>
+      <c r="B178" s="50"/>
+      <c r="C178" s="50"/>
+      <c r="D178" s="50"/>
+      <c r="E178" s="50"/>
+      <c r="F178" s="50"/>
+      <c r="G178" s="50"/>
+      <c r="H178" s="50"/>
+      <c r="I178" s="50"/>
+      <c r="J178" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="45">

</xml_diff>

<commit_message>
Level 1 temponary scale fix, uren reg
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -578,22 +578,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -875,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -887,7 +887,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L77" sqref="L77"/>
+      <selection pane="bottomLeft" activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -946,7 +946,7 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
       <c r="E2" s="47"/>
@@ -954,7 +954,7 @@
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
       <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
@@ -1099,11 +1099,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.9375</v>
+        <v>0.96022727272727271</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>37</v>
@@ -1250,7 +1250,7 @@
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="46"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="47"/>
       <c r="D10" s="47"/>
       <c r="E10" s="47"/>
@@ -1258,7 +1258,7 @@
       <c r="G10" s="47"/>
       <c r="H10" s="47"/>
       <c r="I10" s="47"/>
-      <c r="J10" s="48"/>
+      <c r="J10" s="51"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1480,7 +1480,7 @@
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="46"/>
+      <c r="B18" s="50"/>
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
       <c r="E18" s="47"/>
@@ -1488,7 +1488,7 @@
       <c r="G18" s="47"/>
       <c r="H18" s="47"/>
       <c r="I18" s="47"/>
-      <c r="J18" s="48"/>
+      <c r="J18" s="51"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1708,7 +1708,7 @@
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="46"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="47"/>
       <c r="D26" s="47"/>
       <c r="E26" s="47"/>
@@ -1716,7 +1716,7 @@
       <c r="G26" s="47"/>
       <c r="H26" s="47"/>
       <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
+      <c r="J26" s="51"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -1936,7 +1936,7 @@
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="46"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="47"/>
       <c r="D34" s="47"/>
       <c r="E34" s="47"/>
@@ -1944,7 +1944,7 @@
       <c r="G34" s="47"/>
       <c r="H34" s="47"/>
       <c r="I34" s="47"/>
-      <c r="J34" s="48"/>
+      <c r="J34" s="51"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2166,7 +2166,7 @@
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="46"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="47"/>
       <c r="D42" s="47"/>
       <c r="E42" s="47"/>
@@ -2174,7 +2174,7 @@
       <c r="G42" s="47"/>
       <c r="H42" s="47"/>
       <c r="I42" s="47"/>
-      <c r="J42" s="48"/>
+      <c r="J42" s="51"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2398,7 +2398,7 @@
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="46"/>
+      <c r="B50" s="50"/>
       <c r="C50" s="47"/>
       <c r="D50" s="47"/>
       <c r="E50" s="47"/>
@@ -2406,7 +2406,7 @@
       <c r="G50" s="47"/>
       <c r="H50" s="47"/>
       <c r="I50" s="47"/>
-      <c r="J50" s="48"/>
+      <c r="J50" s="51"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2626,7 +2626,7 @@
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="46"/>
+      <c r="B58" s="50"/>
       <c r="C58" s="47"/>
       <c r="D58" s="47"/>
       <c r="E58" s="47"/>
@@ -2634,7 +2634,7 @@
       <c r="G58" s="47"/>
       <c r="H58" s="47"/>
       <c r="I58" s="47"/>
-      <c r="J58" s="48"/>
+      <c r="J58" s="51"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -2858,7 +2858,7 @@
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="46"/>
+      <c r="B66" s="50"/>
       <c r="C66" s="47"/>
       <c r="D66" s="47"/>
       <c r="E66" s="47"/>
@@ -2866,7 +2866,7 @@
       <c r="G66" s="47"/>
       <c r="H66" s="47"/>
       <c r="I66" s="47"/>
-      <c r="J66" s="48"/>
+      <c r="J66" s="51"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -3016,7 +3016,7 @@
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="46"/>
+      <c r="B74" s="50"/>
       <c r="C74" s="47"/>
       <c r="D74" s="47"/>
       <c r="E74" s="47"/>
@@ -3024,7 +3024,7 @@
       <c r="G74" s="47"/>
       <c r="H74" s="47"/>
       <c r="I74" s="47"/>
-      <c r="J74" s="48"/>
+      <c r="J74" s="51"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3094,11 +3094,13 @@
       <c r="E77" s="6">
         <v>5</v>
       </c>
-      <c r="F77" s="51"/>
+      <c r="F77" s="30">
+        <v>4</v>
+      </c>
       <c r="G77" s="28">
         <v>0</v>
       </c>
-      <c r="H77" s="51"/>
+      <c r="H77" s="46"/>
       <c r="I77" s="6">
         <v>5</v>
       </c>
@@ -3153,7 +3155,7 @@
       </c>
       <c r="F80" s="35">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G80" s="35">
         <f t="shared" si="9"/>
@@ -3187,7 +3189,7 @@
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="46"/>
+      <c r="B82" s="50"/>
       <c r="C82" s="47"/>
       <c r="D82" s="47"/>
       <c r="E82" s="47"/>
@@ -3195,7 +3197,7 @@
       <c r="G82" s="47"/>
       <c r="H82" s="47"/>
       <c r="I82" s="47"/>
-      <c r="J82" s="48"/>
+      <c r="J82" s="51"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3307,7 +3309,7 @@
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="46"/>
+      <c r="B90" s="50"/>
       <c r="C90" s="47"/>
       <c r="D90" s="47"/>
       <c r="E90" s="47"/>
@@ -3315,7 +3317,7 @@
       <c r="G90" s="47"/>
       <c r="H90" s="47"/>
       <c r="I90" s="47"/>
-      <c r="J90" s="48"/>
+      <c r="J90" s="51"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3427,7 +3429,7 @@
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="46"/>
+      <c r="B98" s="50"/>
       <c r="C98" s="47"/>
       <c r="D98" s="47"/>
       <c r="E98" s="47"/>
@@ -3435,7 +3437,7 @@
       <c r="G98" s="47"/>
       <c r="H98" s="47"/>
       <c r="I98" s="47"/>
-      <c r="J98" s="48"/>
+      <c r="J98" s="51"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -3547,7 +3549,7 @@
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="46"/>
+      <c r="B106" s="50"/>
       <c r="C106" s="47"/>
       <c r="D106" s="47"/>
       <c r="E106" s="47"/>
@@ -3555,7 +3557,7 @@
       <c r="G106" s="47"/>
       <c r="H106" s="47"/>
       <c r="I106" s="47"/>
-      <c r="J106" s="48"/>
+      <c r="J106" s="51"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -3667,7 +3669,7 @@
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="46"/>
+      <c r="B114" s="50"/>
       <c r="C114" s="47"/>
       <c r="D114" s="47"/>
       <c r="E114" s="47"/>
@@ -3675,7 +3677,7 @@
       <c r="G114" s="47"/>
       <c r="H114" s="47"/>
       <c r="I114" s="47"/>
-      <c r="J114" s="48"/>
+      <c r="J114" s="51"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -3787,7 +3789,7 @@
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="46"/>
+      <c r="B122" s="50"/>
       <c r="C122" s="47"/>
       <c r="D122" s="47"/>
       <c r="E122" s="47"/>
@@ -3795,7 +3797,7 @@
       <c r="G122" s="47"/>
       <c r="H122" s="47"/>
       <c r="I122" s="47"/>
-      <c r="J122" s="48"/>
+      <c r="J122" s="51"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -3907,7 +3909,7 @@
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="46"/>
+      <c r="B130" s="50"/>
       <c r="C130" s="47"/>
       <c r="D130" s="47"/>
       <c r="E130" s="47"/>
@@ -3915,7 +3917,7 @@
       <c r="G130" s="47"/>
       <c r="H130" s="47"/>
       <c r="I130" s="47"/>
-      <c r="J130" s="48"/>
+      <c r="J130" s="51"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -4027,7 +4029,7 @@
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="46"/>
+      <c r="B138" s="50"/>
       <c r="C138" s="47"/>
       <c r="D138" s="47"/>
       <c r="E138" s="47"/>
@@ -4035,7 +4037,7 @@
       <c r="G138" s="47"/>
       <c r="H138" s="47"/>
       <c r="I138" s="47"/>
-      <c r="J138" s="48"/>
+      <c r="J138" s="51"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -4147,7 +4149,7 @@
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="46"/>
+      <c r="B146" s="50"/>
       <c r="C146" s="47"/>
       <c r="D146" s="47"/>
       <c r="E146" s="47"/>
@@ -4155,7 +4157,7 @@
       <c r="G146" s="47"/>
       <c r="H146" s="47"/>
       <c r="I146" s="47"/>
-      <c r="J146" s="48"/>
+      <c r="J146" s="51"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -4267,7 +4269,7 @@
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="46"/>
+      <c r="B154" s="50"/>
       <c r="C154" s="47"/>
       <c r="D154" s="47"/>
       <c r="E154" s="47"/>
@@ -4275,7 +4277,7 @@
       <c r="G154" s="47"/>
       <c r="H154" s="47"/>
       <c r="I154" s="47"/>
-      <c r="J154" s="48"/>
+      <c r="J154" s="51"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -4387,7 +4389,7 @@
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="46"/>
+      <c r="B162" s="50"/>
       <c r="C162" s="47"/>
       <c r="D162" s="47"/>
       <c r="E162" s="47"/>
@@ -4395,7 +4397,7 @@
       <c r="G162" s="47"/>
       <c r="H162" s="47"/>
       <c r="I162" s="47"/>
-      <c r="J162" s="48"/>
+      <c r="J162" s="51"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -4507,7 +4509,7 @@
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="46"/>
+      <c r="B170" s="50"/>
       <c r="C170" s="47"/>
       <c r="D170" s="47"/>
       <c r="E170" s="47"/>
@@ -4515,7 +4517,7 @@
       <c r="G170" s="47"/>
       <c r="H170" s="47"/>
       <c r="I170" s="47"/>
-      <c r="J170" s="48"/>
+      <c r="J170" s="51"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -4624,51 +4626,19 @@
       <c r="J177" s="47"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="50"/>
-      <c r="B178" s="50"/>
-      <c r="C178" s="50"/>
-      <c r="D178" s="50"/>
-      <c r="E178" s="50"/>
-      <c r="F178" s="50"/>
-      <c r="G178" s="50"/>
-      <c r="H178" s="50"/>
-      <c r="I178" s="50"/>
-      <c r="J178" s="50"/>
+      <c r="A178" s="48"/>
+      <c r="B178" s="48"/>
+      <c r="C178" s="48"/>
+      <c r="D178" s="48"/>
+      <c r="E178" s="48"/>
+      <c r="F178" s="48"/>
+      <c r="G178" s="48"/>
+      <c r="H178" s="48"/>
+      <c r="I178" s="48"/>
+      <c r="J178" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="B154:J154"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="B162:J162"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="B170:J170"/>
-    <mergeCell ref="B146:J146"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B114:J114"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="B122:J122"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="B130:J130"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="B138:J138"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="B98:J98"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A97:J97"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="B2:J2"/>
@@ -4682,6 +4652,38 @@
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B98:J98"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="B82:J82"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="B146:J146"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="B114:J114"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="B122:J122"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="B130:J130"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="B138:J138"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="B154:J154"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="B162:J162"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="B170:J170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Scripts sortout, uren reg, lvl 1 edits
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="61">
   <si>
     <t>Maandag</t>
   </si>
@@ -181,6 +181,27 @@
   </si>
   <si>
     <t>Chantal tandards, Robert doctor</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>Art Lead</t>
+  </si>
+  <si>
+    <t>Plannings Manager</t>
+  </si>
+  <si>
+    <t>Dev Lead</t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Level Designer</t>
   </si>
 </sst>
 </file>
@@ -288,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -469,11 +490,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -578,22 +608,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -875,7 +944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -883,11 +952,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O178"/>
+  <dimension ref="A1:P178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L77" sqref="L77"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L80" sqref="L80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -901,9 +970,10 @@
     <col min="13" max="13" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.140625" style="17" customWidth="1"/>
     <col min="15" max="15" width="12.140625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1">
       <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
@@ -942,39 +1012,42 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.9887640449438202</v>
-      </c>
-      <c r="O2" s="9" t="s">
+        <v>0.98901098901098905</v>
+      </c>
+      <c r="O2" s="58" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" s="51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1009,17 +1082,20 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.8764044943820225</v>
-      </c>
-      <c r="O3" s="11" t="s">
+        <v>0.87912087912087911</v>
+      </c>
+      <c r="O3" s="59" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" s="52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1054,17 +1130,20 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.9887640449438202</v>
-      </c>
-      <c r="O4" s="10" t="s">
+        <v>0.98901098901098905</v>
+      </c>
+      <c r="O4" s="60" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4" s="53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1099,17 +1178,20 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.9606741573033708</v>
-      </c>
-      <c r="O5" s="12" t="s">
+        <v>0.96153846153846156</v>
+      </c>
+      <c r="O5" s="61" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5" s="54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
@@ -1130,17 +1212,20 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.7528089887640449</v>
-      </c>
-      <c r="O6" s="13" t="s">
+        <v>0.75824175824175821</v>
+      </c>
+      <c r="O6" s="62" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1">
+      <c r="P6" s="55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1173,17 +1258,20 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.6629213483146067</v>
-      </c>
-      <c r="O7" s="14" t="s">
+        <v>0.6648351648351648</v>
+      </c>
+      <c r="O7" s="63" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1">
+      <c r="P7" s="56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1">
       <c r="A8" s="33" t="s">
         <v>11</v>
       </c>
@@ -1224,45 +1312,48 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.97752808988764039</v>
-      </c>
-      <c r="O8" s="18" t="s">
+        <v>0.97802197802197799</v>
+      </c>
+      <c r="O8" s="64" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P8" s="57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="50"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
@@ -1296,7 +1387,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -1328,7 +1419,7 @@
       <c r="K12" s="23"/>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1360,7 +1451,7 @@
       <c r="K13" s="23"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -1392,7 +1483,7 @@
       <c r="K14" s="23"/>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1">
+    <row r="15" spans="1:16" ht="15.75" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1424,7 +1515,7 @@
       <c r="K15" s="23"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1">
+    <row r="16" spans="1:16" ht="15.75" thickBot="1">
       <c r="A16" s="33" t="s">
         <v>6</v>
       </c>
@@ -1465,30 +1556,30 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="50"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1693,30 +1784,30 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="50"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="50"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -1921,30 +2012,30 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="50"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="49"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="50"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2151,30 +2242,30 @@
       <c r="L40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A41" s="50"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="50"/>
+      <c r="A41" s="48"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="49"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="50"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2383,30 +2474,30 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="50"/>
-      <c r="B49" s="50"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
+      <c r="A49" s="48"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="48"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="49"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="50"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2611,30 +2702,30 @@
       <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="50"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="50"/>
+      <c r="A57" s="48"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="48"/>
-      <c r="E58" s="48"/>
-      <c r="F58" s="48"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="48"/>
-      <c r="I58" s="48"/>
-      <c r="J58" s="49"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="50"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -2843,30 +2934,30 @@
       <c r="L64" s="8"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A65" s="50"/>
-      <c r="B65" s="50"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="50"/>
-      <c r="E65" s="50"/>
-      <c r="F65" s="50"/>
-      <c r="G65" s="50"/>
-      <c r="H65" s="50"/>
-      <c r="I65" s="50"/>
-      <c r="J65" s="50"/>
+      <c r="A65" s="48"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="48"/>
+      <c r="D65" s="48"/>
+      <c r="E65" s="48"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="48"/>
+      <c r="I65" s="48"/>
+      <c r="J65" s="48"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="47"/>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48"/>
-      <c r="I66" s="48"/>
-      <c r="J66" s="49"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="50"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -3001,30 +3092,30 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A73" s="50"/>
-      <c r="B73" s="50"/>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="50"/>
-      <c r="H73" s="50"/>
-      <c r="I73" s="50"/>
-      <c r="J73" s="50"/>
+      <c r="A73" s="48"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="48"/>
+      <c r="F73" s="48"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="48"/>
+      <c r="I73" s="48"/>
+      <c r="J73" s="48"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="47"/>
-      <c r="C74" s="48"/>
-      <c r="D74" s="48"/>
-      <c r="E74" s="48"/>
-      <c r="F74" s="48"/>
-      <c r="G74" s="48"/>
-      <c r="H74" s="48"/>
-      <c r="I74" s="48"/>
-      <c r="J74" s="49"/>
+      <c r="B74" s="49"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="46"/>
+      <c r="H74" s="46"/>
+      <c r="I74" s="46"/>
+      <c r="J74" s="50"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3100,7 +3191,7 @@
       <c r="G77" s="28">
         <v>0</v>
       </c>
-      <c r="H77" s="46">
+      <c r="H77" s="30">
         <v>0</v>
       </c>
       <c r="I77" s="6">
@@ -3146,14 +3237,30 @@
       <c r="A79" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-      <c r="I79" s="7"/>
+      <c r="B79" s="7">
+        <v>4</v>
+      </c>
+      <c r="C79" s="7">
+        <v>4</v>
+      </c>
+      <c r="D79" s="7">
+        <v>4</v>
+      </c>
+      <c r="E79" s="7">
+        <v>4</v>
+      </c>
+      <c r="F79" s="7">
+        <v>4</v>
+      </c>
+      <c r="G79" s="7">
+        <v>4</v>
+      </c>
+      <c r="H79" s="31">
+        <v>3</v>
+      </c>
+      <c r="I79" s="7">
+        <v>4</v>
+      </c>
       <c r="J79" s="2"/>
       <c r="K79" s="23"/>
       <c r="L79" s="8"/>
@@ -3164,65 +3271,65 @@
       </c>
       <c r="B80" s="34">
         <f>B75+B76+B77+B78+B79</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C80" s="35">
         <f t="shared" ref="C80:H80" si="9">SUM(C75:C79)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D80" s="35">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E80" s="35">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F80" s="35">
         <f t="shared" si="9"/>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G80" s="35">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H80" s="35">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I80" s="35">
         <f>SUM(I75:I79)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J80" s="36"/>
       <c r="K80" s="23"/>
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A81" s="50"/>
-      <c r="B81" s="50"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="50"/>
-      <c r="E81" s="50"/>
-      <c r="F81" s="50"/>
-      <c r="G81" s="50"/>
-      <c r="H81" s="50"/>
-      <c r="I81" s="50"/>
-      <c r="J81" s="50"/>
+      <c r="A81" s="48"/>
+      <c r="B81" s="48"/>
+      <c r="C81" s="48"/>
+      <c r="D81" s="48"/>
+      <c r="E81" s="48"/>
+      <c r="F81" s="48"/>
+      <c r="G81" s="48"/>
+      <c r="H81" s="48"/>
+      <c r="I81" s="48"/>
+      <c r="J81" s="48"/>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="47"/>
-      <c r="C82" s="48"/>
-      <c r="D82" s="48"/>
-      <c r="E82" s="48"/>
-      <c r="F82" s="48"/>
-      <c r="G82" s="48"/>
-      <c r="H82" s="48"/>
-      <c r="I82" s="48"/>
-      <c r="J82" s="49"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="46"/>
+      <c r="D82" s="46"/>
+      <c r="E82" s="46"/>
+      <c r="F82" s="46"/>
+      <c r="G82" s="46"/>
+      <c r="H82" s="46"/>
+      <c r="I82" s="46"/>
+      <c r="J82" s="50"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3319,30 +3426,30 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A89" s="50"/>
-      <c r="B89" s="50"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
-      <c r="E89" s="50"/>
-      <c r="F89" s="50"/>
-      <c r="G89" s="50"/>
-      <c r="H89" s="50"/>
-      <c r="I89" s="50"/>
-      <c r="J89" s="50"/>
+      <c r="A89" s="48"/>
+      <c r="B89" s="48"/>
+      <c r="C89" s="48"/>
+      <c r="D89" s="48"/>
+      <c r="E89" s="48"/>
+      <c r="F89" s="48"/>
+      <c r="G89" s="48"/>
+      <c r="H89" s="48"/>
+      <c r="I89" s="48"/>
+      <c r="J89" s="48"/>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="47"/>
-      <c r="C90" s="48"/>
-      <c r="D90" s="48"/>
-      <c r="E90" s="48"/>
-      <c r="F90" s="48"/>
-      <c r="G90" s="48"/>
-      <c r="H90" s="48"/>
-      <c r="I90" s="48"/>
-      <c r="J90" s="49"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="46"/>
+      <c r="D90" s="46"/>
+      <c r="E90" s="46"/>
+      <c r="F90" s="46"/>
+      <c r="G90" s="46"/>
+      <c r="H90" s="46"/>
+      <c r="I90" s="46"/>
+      <c r="J90" s="50"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3439,30 +3546,30 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A97" s="50"/>
-      <c r="B97" s="50"/>
-      <c r="C97" s="50"/>
-      <c r="D97" s="50"/>
-      <c r="E97" s="50"/>
-      <c r="F97" s="50"/>
-      <c r="G97" s="50"/>
-      <c r="H97" s="50"/>
-      <c r="I97" s="50"/>
-      <c r="J97" s="50"/>
+      <c r="A97" s="48"/>
+      <c r="B97" s="48"/>
+      <c r="C97" s="48"/>
+      <c r="D97" s="48"/>
+      <c r="E97" s="48"/>
+      <c r="F97" s="48"/>
+      <c r="G97" s="48"/>
+      <c r="H97" s="48"/>
+      <c r="I97" s="48"/>
+      <c r="J97" s="48"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="47"/>
-      <c r="C98" s="48"/>
-      <c r="D98" s="48"/>
-      <c r="E98" s="48"/>
-      <c r="F98" s="48"/>
-      <c r="G98" s="48"/>
-      <c r="H98" s="48"/>
-      <c r="I98" s="48"/>
-      <c r="J98" s="49"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="46"/>
+      <c r="D98" s="46"/>
+      <c r="E98" s="46"/>
+      <c r="F98" s="46"/>
+      <c r="G98" s="46"/>
+      <c r="H98" s="46"/>
+      <c r="I98" s="46"/>
+      <c r="J98" s="50"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -3559,30 +3666,30 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A105" s="50"/>
-      <c r="B105" s="50"/>
-      <c r="C105" s="50"/>
-      <c r="D105" s="50"/>
-      <c r="E105" s="50"/>
-      <c r="F105" s="50"/>
-      <c r="G105" s="50"/>
-      <c r="H105" s="50"/>
-      <c r="I105" s="50"/>
-      <c r="J105" s="50"/>
+      <c r="A105" s="48"/>
+      <c r="B105" s="48"/>
+      <c r="C105" s="48"/>
+      <c r="D105" s="48"/>
+      <c r="E105" s="48"/>
+      <c r="F105" s="48"/>
+      <c r="G105" s="48"/>
+      <c r="H105" s="48"/>
+      <c r="I105" s="48"/>
+      <c r="J105" s="48"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="47"/>
-      <c r="C106" s="48"/>
-      <c r="D106" s="48"/>
-      <c r="E106" s="48"/>
-      <c r="F106" s="48"/>
-      <c r="G106" s="48"/>
-      <c r="H106" s="48"/>
-      <c r="I106" s="48"/>
-      <c r="J106" s="49"/>
+      <c r="B106" s="49"/>
+      <c r="C106" s="46"/>
+      <c r="D106" s="46"/>
+      <c r="E106" s="46"/>
+      <c r="F106" s="46"/>
+      <c r="G106" s="46"/>
+      <c r="H106" s="46"/>
+      <c r="I106" s="46"/>
+      <c r="J106" s="50"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -3679,30 +3786,30 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A113" s="50"/>
-      <c r="B113" s="50"/>
-      <c r="C113" s="50"/>
-      <c r="D113" s="50"/>
-      <c r="E113" s="50"/>
-      <c r="F113" s="50"/>
-      <c r="G113" s="50"/>
-      <c r="H113" s="50"/>
-      <c r="I113" s="50"/>
-      <c r="J113" s="50"/>
+      <c r="A113" s="48"/>
+      <c r="B113" s="48"/>
+      <c r="C113" s="48"/>
+      <c r="D113" s="48"/>
+      <c r="E113" s="48"/>
+      <c r="F113" s="48"/>
+      <c r="G113" s="48"/>
+      <c r="H113" s="48"/>
+      <c r="I113" s="48"/>
+      <c r="J113" s="48"/>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="47"/>
-      <c r="C114" s="48"/>
-      <c r="D114" s="48"/>
-      <c r="E114" s="48"/>
-      <c r="F114" s="48"/>
-      <c r="G114" s="48"/>
-      <c r="H114" s="48"/>
-      <c r="I114" s="48"/>
-      <c r="J114" s="49"/>
+      <c r="B114" s="49"/>
+      <c r="C114" s="46"/>
+      <c r="D114" s="46"/>
+      <c r="E114" s="46"/>
+      <c r="F114" s="46"/>
+      <c r="G114" s="46"/>
+      <c r="H114" s="46"/>
+      <c r="I114" s="46"/>
+      <c r="J114" s="50"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -3799,30 +3906,30 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A121" s="50"/>
-      <c r="B121" s="50"/>
-      <c r="C121" s="50"/>
-      <c r="D121" s="50"/>
-      <c r="E121" s="50"/>
-      <c r="F121" s="50"/>
-      <c r="G121" s="50"/>
-      <c r="H121" s="50"/>
-      <c r="I121" s="50"/>
-      <c r="J121" s="50"/>
+      <c r="A121" s="48"/>
+      <c r="B121" s="48"/>
+      <c r="C121" s="48"/>
+      <c r="D121" s="48"/>
+      <c r="E121" s="48"/>
+      <c r="F121" s="48"/>
+      <c r="G121" s="48"/>
+      <c r="H121" s="48"/>
+      <c r="I121" s="48"/>
+      <c r="J121" s="48"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="47"/>
-      <c r="C122" s="48"/>
-      <c r="D122" s="48"/>
-      <c r="E122" s="48"/>
-      <c r="F122" s="48"/>
-      <c r="G122" s="48"/>
-      <c r="H122" s="48"/>
-      <c r="I122" s="48"/>
-      <c r="J122" s="49"/>
+      <c r="B122" s="49"/>
+      <c r="C122" s="46"/>
+      <c r="D122" s="46"/>
+      <c r="E122" s="46"/>
+      <c r="F122" s="46"/>
+      <c r="G122" s="46"/>
+      <c r="H122" s="46"/>
+      <c r="I122" s="46"/>
+      <c r="J122" s="50"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -3919,30 +4026,30 @@
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A129" s="50"/>
-      <c r="B129" s="50"/>
-      <c r="C129" s="50"/>
-      <c r="D129" s="50"/>
-      <c r="E129" s="50"/>
-      <c r="F129" s="50"/>
-      <c r="G129" s="50"/>
-      <c r="H129" s="50"/>
-      <c r="I129" s="50"/>
-      <c r="J129" s="50"/>
+      <c r="A129" s="48"/>
+      <c r="B129" s="48"/>
+      <c r="C129" s="48"/>
+      <c r="D129" s="48"/>
+      <c r="E129" s="48"/>
+      <c r="F129" s="48"/>
+      <c r="G129" s="48"/>
+      <c r="H129" s="48"/>
+      <c r="I129" s="48"/>
+      <c r="J129" s="48"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="47"/>
-      <c r="C130" s="48"/>
-      <c r="D130" s="48"/>
-      <c r="E130" s="48"/>
-      <c r="F130" s="48"/>
-      <c r="G130" s="48"/>
-      <c r="H130" s="48"/>
-      <c r="I130" s="48"/>
-      <c r="J130" s="49"/>
+      <c r="B130" s="49"/>
+      <c r="C130" s="46"/>
+      <c r="D130" s="46"/>
+      <c r="E130" s="46"/>
+      <c r="F130" s="46"/>
+      <c r="G130" s="46"/>
+      <c r="H130" s="46"/>
+      <c r="I130" s="46"/>
+      <c r="J130" s="50"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -4039,30 +4146,30 @@
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A137" s="50"/>
-      <c r="B137" s="50"/>
-      <c r="C137" s="50"/>
-      <c r="D137" s="50"/>
-      <c r="E137" s="50"/>
-      <c r="F137" s="50"/>
-      <c r="G137" s="50"/>
-      <c r="H137" s="50"/>
-      <c r="I137" s="50"/>
-      <c r="J137" s="50"/>
+      <c r="A137" s="48"/>
+      <c r="B137" s="48"/>
+      <c r="C137" s="48"/>
+      <c r="D137" s="48"/>
+      <c r="E137" s="48"/>
+      <c r="F137" s="48"/>
+      <c r="G137" s="48"/>
+      <c r="H137" s="48"/>
+      <c r="I137" s="48"/>
+      <c r="J137" s="48"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="47"/>
-      <c r="C138" s="48"/>
-      <c r="D138" s="48"/>
-      <c r="E138" s="48"/>
-      <c r="F138" s="48"/>
-      <c r="G138" s="48"/>
-      <c r="H138" s="48"/>
-      <c r="I138" s="48"/>
-      <c r="J138" s="49"/>
+      <c r="B138" s="49"/>
+      <c r="C138" s="46"/>
+      <c r="D138" s="46"/>
+      <c r="E138" s="46"/>
+      <c r="F138" s="46"/>
+      <c r="G138" s="46"/>
+      <c r="H138" s="46"/>
+      <c r="I138" s="46"/>
+      <c r="J138" s="50"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -4159,30 +4266,30 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A145" s="50"/>
-      <c r="B145" s="50"/>
-      <c r="C145" s="50"/>
-      <c r="D145" s="50"/>
-      <c r="E145" s="50"/>
-      <c r="F145" s="50"/>
-      <c r="G145" s="50"/>
-      <c r="H145" s="50"/>
-      <c r="I145" s="50"/>
-      <c r="J145" s="50"/>
+      <c r="A145" s="48"/>
+      <c r="B145" s="48"/>
+      <c r="C145" s="48"/>
+      <c r="D145" s="48"/>
+      <c r="E145" s="48"/>
+      <c r="F145" s="48"/>
+      <c r="G145" s="48"/>
+      <c r="H145" s="48"/>
+      <c r="I145" s="48"/>
+      <c r="J145" s="48"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="47"/>
-      <c r="C146" s="48"/>
-      <c r="D146" s="48"/>
-      <c r="E146" s="48"/>
-      <c r="F146" s="48"/>
-      <c r="G146" s="48"/>
-      <c r="H146" s="48"/>
-      <c r="I146" s="48"/>
-      <c r="J146" s="49"/>
+      <c r="B146" s="49"/>
+      <c r="C146" s="46"/>
+      <c r="D146" s="46"/>
+      <c r="E146" s="46"/>
+      <c r="F146" s="46"/>
+      <c r="G146" s="46"/>
+      <c r="H146" s="46"/>
+      <c r="I146" s="46"/>
+      <c r="J146" s="50"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -4279,30 +4386,30 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A153" s="50"/>
-      <c r="B153" s="50"/>
-      <c r="C153" s="50"/>
-      <c r="D153" s="50"/>
-      <c r="E153" s="50"/>
-      <c r="F153" s="50"/>
-      <c r="G153" s="50"/>
-      <c r="H153" s="50"/>
-      <c r="I153" s="50"/>
-      <c r="J153" s="50"/>
+      <c r="A153" s="48"/>
+      <c r="B153" s="48"/>
+      <c r="C153" s="48"/>
+      <c r="D153" s="48"/>
+      <c r="E153" s="48"/>
+      <c r="F153" s="48"/>
+      <c r="G153" s="48"/>
+      <c r="H153" s="48"/>
+      <c r="I153" s="48"/>
+      <c r="J153" s="48"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="47"/>
-      <c r="C154" s="48"/>
-      <c r="D154" s="48"/>
-      <c r="E154" s="48"/>
-      <c r="F154" s="48"/>
-      <c r="G154" s="48"/>
-      <c r="H154" s="48"/>
-      <c r="I154" s="48"/>
-      <c r="J154" s="49"/>
+      <c r="B154" s="49"/>
+      <c r="C154" s="46"/>
+      <c r="D154" s="46"/>
+      <c r="E154" s="46"/>
+      <c r="F154" s="46"/>
+      <c r="G154" s="46"/>
+      <c r="H154" s="46"/>
+      <c r="I154" s="46"/>
+      <c r="J154" s="50"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -4399,30 +4506,30 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A161" s="50"/>
-      <c r="B161" s="50"/>
-      <c r="C161" s="50"/>
-      <c r="D161" s="50"/>
-      <c r="E161" s="50"/>
-      <c r="F161" s="50"/>
-      <c r="G161" s="50"/>
-      <c r="H161" s="50"/>
-      <c r="I161" s="50"/>
-      <c r="J161" s="50"/>
+      <c r="A161" s="48"/>
+      <c r="B161" s="48"/>
+      <c r="C161" s="48"/>
+      <c r="D161" s="48"/>
+      <c r="E161" s="48"/>
+      <c r="F161" s="48"/>
+      <c r="G161" s="48"/>
+      <c r="H161" s="48"/>
+      <c r="I161" s="48"/>
+      <c r="J161" s="48"/>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="47"/>
-      <c r="C162" s="48"/>
-      <c r="D162" s="48"/>
-      <c r="E162" s="48"/>
-      <c r="F162" s="48"/>
-      <c r="G162" s="48"/>
-      <c r="H162" s="48"/>
-      <c r="I162" s="48"/>
-      <c r="J162" s="49"/>
+      <c r="B162" s="49"/>
+      <c r="C162" s="46"/>
+      <c r="D162" s="46"/>
+      <c r="E162" s="46"/>
+      <c r="F162" s="46"/>
+      <c r="G162" s="46"/>
+      <c r="H162" s="46"/>
+      <c r="I162" s="46"/>
+      <c r="J162" s="50"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -4519,30 +4626,30 @@
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A169" s="50"/>
-      <c r="B169" s="50"/>
-      <c r="C169" s="50"/>
-      <c r="D169" s="50"/>
-      <c r="E169" s="50"/>
-      <c r="F169" s="50"/>
-      <c r="G169" s="50"/>
-      <c r="H169" s="50"/>
-      <c r="I169" s="50"/>
-      <c r="J169" s="50"/>
+      <c r="A169" s="48"/>
+      <c r="B169" s="48"/>
+      <c r="C169" s="48"/>
+      <c r="D169" s="48"/>
+      <c r="E169" s="48"/>
+      <c r="F169" s="48"/>
+      <c r="G169" s="48"/>
+      <c r="H169" s="48"/>
+      <c r="I169" s="48"/>
+      <c r="J169" s="48"/>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="47"/>
-      <c r="C170" s="48"/>
-      <c r="D170" s="48"/>
-      <c r="E170" s="48"/>
-      <c r="F170" s="48"/>
-      <c r="G170" s="48"/>
-      <c r="H170" s="48"/>
-      <c r="I170" s="48"/>
-      <c r="J170" s="49"/>
+      <c r="B170" s="49"/>
+      <c r="C170" s="46"/>
+      <c r="D170" s="46"/>
+      <c r="E170" s="46"/>
+      <c r="F170" s="46"/>
+      <c r="G170" s="46"/>
+      <c r="H170" s="46"/>
+      <c r="I170" s="46"/>
+      <c r="J170" s="50"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -4639,63 +4746,31 @@
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="48"/>
-      <c r="B177" s="48"/>
-      <c r="C177" s="48"/>
-      <c r="D177" s="48"/>
-      <c r="E177" s="48"/>
-      <c r="F177" s="48"/>
-      <c r="G177" s="48"/>
-      <c r="H177" s="48"/>
-      <c r="I177" s="48"/>
-      <c r="J177" s="48"/>
+      <c r="A177" s="46"/>
+      <c r="B177" s="46"/>
+      <c r="C177" s="46"/>
+      <c r="D177" s="46"/>
+      <c r="E177" s="46"/>
+      <c r="F177" s="46"/>
+      <c r="G177" s="46"/>
+      <c r="H177" s="46"/>
+      <c r="I177" s="46"/>
+      <c r="J177" s="46"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="51"/>
-      <c r="B178" s="51"/>
-      <c r="C178" s="51"/>
-      <c r="D178" s="51"/>
-      <c r="E178" s="51"/>
-      <c r="F178" s="51"/>
-      <c r="G178" s="51"/>
-      <c r="H178" s="51"/>
-      <c r="I178" s="51"/>
-      <c r="J178" s="51"/>
+      <c r="A178" s="47"/>
+      <c r="B178" s="47"/>
+      <c r="C178" s="47"/>
+      <c r="D178" s="47"/>
+      <c r="E178" s="47"/>
+      <c r="F178" s="47"/>
+      <c r="G178" s="47"/>
+      <c r="H178" s="47"/>
+      <c r="I178" s="47"/>
+      <c r="J178" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="B154:J154"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="B162:J162"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="B170:J170"/>
-    <mergeCell ref="B146:J146"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B114:J114"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="B122:J122"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="B130:J130"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="B138:J138"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="B98:J98"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A97:J97"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="B2:J2"/>
@@ -4709,6 +4784,38 @@
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B98:J98"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="B82:J82"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="B146:J146"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="B114:J114"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="B122:J122"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="B130:J130"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="B138:J138"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="B154:J154"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="B162:J162"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="B170:J170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
StartScene & Canvas update + Uren reg
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -724,6 +724,12 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -737,12 +743,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1037,7 +1037,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L119" sqref="L119"/>
+      <selection pane="bottomLeft" activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1097,29 +1097,29 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="71"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="73"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.9928057553956835</v>
+        <v>0.99303135888501737</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>35</v>
@@ -1163,11 +1163,11 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.83812949640287771</v>
+        <v>0.83972125435540068</v>
       </c>
       <c r="O3" s="54" t="s">
         <v>34</v>
@@ -1211,11 +1211,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.9928057553956835</v>
+        <v>0.99303135888501737</v>
       </c>
       <c r="O4" s="55" t="s">
         <v>36</v>
@@ -1259,11 +1259,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.93525179856115104</v>
+        <v>0.91986062717770034</v>
       </c>
       <c r="O5" s="56" t="s">
         <v>37</v>
@@ -1293,11 +1293,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.79136690647482011</v>
+        <v>0.78397212543554007</v>
       </c>
       <c r="O6" s="57" t="s">
         <v>38</v>
@@ -1341,11 +1341,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.67266187050359716</v>
+        <v>0.68292682926829273</v>
       </c>
       <c r="O7" s="58" t="s">
         <v>39</v>
@@ -1395,11 +1395,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.97482014388489213</v>
+        <v>0.97560975609756095</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>40</v>
@@ -1409,30 +1409,30 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A9" s="69"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="71"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="73"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1639,30 +1639,30 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="69"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="71"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="73"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1867,30 +1867,30 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="69"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="70"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="71"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="73"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -2095,30 +2095,30 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="69"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
+      <c r="A33" s="71"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="70"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="71"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="73"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2325,30 +2325,30 @@
       <c r="L40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A41" s="69"/>
-      <c r="B41" s="69"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="69"/>
-      <c r="J41" s="69"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="70"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="67"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="67"/>
-      <c r="H42" s="67"/>
-      <c r="I42" s="67"/>
-      <c r="J42" s="71"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="73"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2557,30 +2557,30 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="69"/>
-      <c r="B49" s="69"/>
-      <c r="C49" s="69"/>
-      <c r="D49" s="69"/>
-      <c r="E49" s="69"/>
-      <c r="F49" s="69"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="69"/>
-      <c r="I49" s="69"/>
-      <c r="J49" s="69"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="71"/>
+      <c r="I49" s="71"/>
+      <c r="J49" s="71"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="70"/>
-      <c r="C50" s="67"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="67"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="67"/>
-      <c r="J50" s="71"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="69"/>
+      <c r="J50" s="73"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2785,30 +2785,30 @@
       <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="69"/>
-      <c r="B57" s="69"/>
-      <c r="C57" s="69"/>
-      <c r="D57" s="69"/>
-      <c r="E57" s="69"/>
-      <c r="F57" s="69"/>
-      <c r="G57" s="69"/>
-      <c r="H57" s="69"/>
-      <c r="I57" s="69"/>
-      <c r="J57" s="69"/>
+      <c r="A57" s="71"/>
+      <c r="B57" s="71"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="71"/>
+      <c r="E57" s="71"/>
+      <c r="F57" s="71"/>
+      <c r="G57" s="71"/>
+      <c r="H57" s="71"/>
+      <c r="I57" s="71"/>
+      <c r="J57" s="71"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="70"/>
-      <c r="C58" s="67"/>
-      <c r="D58" s="67"/>
-      <c r="E58" s="67"/>
-      <c r="F58" s="67"/>
-      <c r="G58" s="67"/>
-      <c r="H58" s="67"/>
-      <c r="I58" s="67"/>
-      <c r="J58" s="71"/>
+      <c r="B58" s="72"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="69"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="69"/>
+      <c r="G58" s="69"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="69"/>
+      <c r="J58" s="73"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -3017,30 +3017,30 @@
       <c r="L64" s="8"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A65" s="69"/>
-      <c r="B65" s="69"/>
-      <c r="C65" s="69"/>
-      <c r="D65" s="69"/>
-      <c r="E65" s="69"/>
-      <c r="F65" s="69"/>
-      <c r="G65" s="69"/>
-      <c r="H65" s="69"/>
-      <c r="I65" s="69"/>
-      <c r="J65" s="69"/>
+      <c r="A65" s="71"/>
+      <c r="B65" s="71"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71"/>
+      <c r="J65" s="71"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="70"/>
-      <c r="C66" s="67"/>
-      <c r="D66" s="67"/>
-      <c r="E66" s="67"/>
-      <c r="F66" s="67"/>
-      <c r="G66" s="67"/>
-      <c r="H66" s="67"/>
-      <c r="I66" s="67"/>
-      <c r="J66" s="71"/>
+      <c r="B66" s="72"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="69"/>
+      <c r="E66" s="69"/>
+      <c r="F66" s="69"/>
+      <c r="G66" s="69"/>
+      <c r="H66" s="69"/>
+      <c r="I66" s="69"/>
+      <c r="J66" s="73"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -3175,30 +3175,30 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A73" s="69"/>
-      <c r="B73" s="69"/>
-      <c r="C73" s="69"/>
-      <c r="D73" s="69"/>
-      <c r="E73" s="69"/>
-      <c r="F73" s="69"/>
-      <c r="G73" s="69"/>
-      <c r="H73" s="69"/>
-      <c r="I73" s="69"/>
-      <c r="J73" s="69"/>
+      <c r="A73" s="71"/>
+      <c r="B73" s="71"/>
+      <c r="C73" s="71"/>
+      <c r="D73" s="71"/>
+      <c r="E73" s="71"/>
+      <c r="F73" s="71"/>
+      <c r="G73" s="71"/>
+      <c r="H73" s="71"/>
+      <c r="I73" s="71"/>
+      <c r="J73" s="71"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="70"/>
-      <c r="C74" s="67"/>
-      <c r="D74" s="67"/>
-      <c r="E74" s="67"/>
-      <c r="F74" s="67"/>
-      <c r="G74" s="67"/>
-      <c r="H74" s="67"/>
-      <c r="I74" s="67"/>
-      <c r="J74" s="71"/>
+      <c r="B74" s="72"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="69"/>
+      <c r="F74" s="69"/>
+      <c r="G74" s="69"/>
+      <c r="H74" s="69"/>
+      <c r="I74" s="69"/>
+      <c r="J74" s="73"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3389,30 +3389,30 @@
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A81" s="69"/>
-      <c r="B81" s="69"/>
-      <c r="C81" s="69"/>
-      <c r="D81" s="69"/>
-      <c r="E81" s="69"/>
-      <c r="F81" s="69"/>
-      <c r="G81" s="69"/>
-      <c r="H81" s="69"/>
-      <c r="I81" s="69"/>
-      <c r="J81" s="69"/>
+      <c r="A81" s="71"/>
+      <c r="B81" s="71"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="71"/>
+      <c r="E81" s="71"/>
+      <c r="F81" s="71"/>
+      <c r="G81" s="71"/>
+      <c r="H81" s="71"/>
+      <c r="I81" s="71"/>
+      <c r="J81" s="71"/>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="70"/>
-      <c r="C82" s="67"/>
-      <c r="D82" s="67"/>
-      <c r="E82" s="67"/>
-      <c r="F82" s="67"/>
-      <c r="G82" s="67"/>
-      <c r="H82" s="67"/>
-      <c r="I82" s="67"/>
-      <c r="J82" s="71"/>
+      <c r="B82" s="72"/>
+      <c r="C82" s="69"/>
+      <c r="D82" s="69"/>
+      <c r="E82" s="69"/>
+      <c r="F82" s="69"/>
+      <c r="G82" s="69"/>
+      <c r="H82" s="69"/>
+      <c r="I82" s="69"/>
+      <c r="J82" s="73"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3619,30 +3619,30 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A89" s="69"/>
-      <c r="B89" s="69"/>
-      <c r="C89" s="69"/>
-      <c r="D89" s="69"/>
-      <c r="E89" s="69"/>
-      <c r="F89" s="69"/>
-      <c r="G89" s="69"/>
-      <c r="H89" s="69"/>
-      <c r="I89" s="69"/>
-      <c r="J89" s="69"/>
+      <c r="A89" s="71"/>
+      <c r="B89" s="71"/>
+      <c r="C89" s="71"/>
+      <c r="D89" s="71"/>
+      <c r="E89" s="71"/>
+      <c r="F89" s="71"/>
+      <c r="G89" s="71"/>
+      <c r="H89" s="71"/>
+      <c r="I89" s="71"/>
+      <c r="J89" s="71"/>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="70"/>
-      <c r="C90" s="67"/>
-      <c r="D90" s="67"/>
-      <c r="E90" s="67"/>
-      <c r="F90" s="67"/>
-      <c r="G90" s="67"/>
-      <c r="H90" s="67"/>
-      <c r="I90" s="67"/>
-      <c r="J90" s="71"/>
+      <c r="B90" s="72"/>
+      <c r="C90" s="69"/>
+      <c r="D90" s="69"/>
+      <c r="E90" s="69"/>
+      <c r="F90" s="69"/>
+      <c r="G90" s="69"/>
+      <c r="H90" s="69"/>
+      <c r="I90" s="69"/>
+      <c r="J90" s="73"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3847,30 +3847,30 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A97" s="69"/>
-      <c r="B97" s="69"/>
-      <c r="C97" s="69"/>
-      <c r="D97" s="69"/>
-      <c r="E97" s="69"/>
-      <c r="F97" s="69"/>
-      <c r="G97" s="69"/>
-      <c r="H97" s="69"/>
-      <c r="I97" s="69"/>
-      <c r="J97" s="69"/>
+      <c r="A97" s="71"/>
+      <c r="B97" s="71"/>
+      <c r="C97" s="71"/>
+      <c r="D97" s="71"/>
+      <c r="E97" s="71"/>
+      <c r="F97" s="71"/>
+      <c r="G97" s="71"/>
+      <c r="H97" s="71"/>
+      <c r="I97" s="71"/>
+      <c r="J97" s="71"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="70"/>
-      <c r="C98" s="67"/>
-      <c r="D98" s="67"/>
-      <c r="E98" s="67"/>
-      <c r="F98" s="67"/>
-      <c r="G98" s="67"/>
-      <c r="H98" s="67"/>
-      <c r="I98" s="67"/>
-      <c r="J98" s="71"/>
+      <c r="B98" s="72"/>
+      <c r="C98" s="69"/>
+      <c r="D98" s="69"/>
+      <c r="E98" s="69"/>
+      <c r="F98" s="69"/>
+      <c r="G98" s="69"/>
+      <c r="H98" s="69"/>
+      <c r="I98" s="69"/>
+      <c r="J98" s="73"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -4077,30 +4077,30 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A105" s="69"/>
-      <c r="B105" s="69"/>
-      <c r="C105" s="69"/>
-      <c r="D105" s="69"/>
-      <c r="E105" s="69"/>
-      <c r="F105" s="69"/>
-      <c r="G105" s="69"/>
-      <c r="H105" s="69"/>
-      <c r="I105" s="69"/>
-      <c r="J105" s="69"/>
+      <c r="A105" s="71"/>
+      <c r="B105" s="71"/>
+      <c r="C105" s="71"/>
+      <c r="D105" s="71"/>
+      <c r="E105" s="71"/>
+      <c r="F105" s="71"/>
+      <c r="G105" s="71"/>
+      <c r="H105" s="71"/>
+      <c r="I105" s="71"/>
+      <c r="J105" s="71"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="70"/>
-      <c r="C106" s="67"/>
-      <c r="D106" s="67"/>
-      <c r="E106" s="67"/>
-      <c r="F106" s="67"/>
-      <c r="G106" s="67"/>
-      <c r="H106" s="67"/>
-      <c r="I106" s="67"/>
-      <c r="J106" s="71"/>
+      <c r="B106" s="72"/>
+      <c r="C106" s="69"/>
+      <c r="D106" s="69"/>
+      <c r="E106" s="69"/>
+      <c r="F106" s="69"/>
+      <c r="G106" s="69"/>
+      <c r="H106" s="69"/>
+      <c r="I106" s="69"/>
+      <c r="J106" s="73"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -4307,30 +4307,30 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A113" s="69"/>
-      <c r="B113" s="69"/>
-      <c r="C113" s="69"/>
-      <c r="D113" s="69"/>
-      <c r="E113" s="69"/>
-      <c r="F113" s="69"/>
-      <c r="G113" s="69"/>
-      <c r="H113" s="69"/>
-      <c r="I113" s="69"/>
-      <c r="J113" s="69"/>
+      <c r="A113" s="71"/>
+      <c r="B113" s="71"/>
+      <c r="C113" s="71"/>
+      <c r="D113" s="71"/>
+      <c r="E113" s="71"/>
+      <c r="F113" s="71"/>
+      <c r="G113" s="71"/>
+      <c r="H113" s="71"/>
+      <c r="I113" s="71"/>
+      <c r="J113" s="71"/>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="70"/>
-      <c r="C114" s="67"/>
-      <c r="D114" s="67"/>
-      <c r="E114" s="67"/>
-      <c r="F114" s="67"/>
-      <c r="G114" s="67"/>
-      <c r="H114" s="67"/>
-      <c r="I114" s="67"/>
-      <c r="J114" s="71"/>
+      <c r="B114" s="72"/>
+      <c r="C114" s="69"/>
+      <c r="D114" s="69"/>
+      <c r="E114" s="69"/>
+      <c r="F114" s="69"/>
+      <c r="G114" s="69"/>
+      <c r="H114" s="69"/>
+      <c r="I114" s="69"/>
+      <c r="J114" s="73"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -4452,7 +4452,7 @@
       <c r="G118" s="6">
         <v>2</v>
       </c>
-      <c r="H118" s="72">
+      <c r="H118" s="67">
         <v>2</v>
       </c>
       <c r="I118" s="6">
@@ -4484,7 +4484,7 @@
       <c r="G119" s="7">
         <v>4</v>
       </c>
-      <c r="H119" s="73">
+      <c r="H119" s="68">
         <v>4</v>
       </c>
       <c r="I119" s="7">
@@ -4535,30 +4535,30 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A121" s="69"/>
-      <c r="B121" s="69"/>
-      <c r="C121" s="69"/>
-      <c r="D121" s="69"/>
-      <c r="E121" s="69"/>
-      <c r="F121" s="69"/>
-      <c r="G121" s="69"/>
-      <c r="H121" s="69"/>
-      <c r="I121" s="69"/>
-      <c r="J121" s="69"/>
+      <c r="A121" s="71"/>
+      <c r="B121" s="71"/>
+      <c r="C121" s="71"/>
+      <c r="D121" s="71"/>
+      <c r="E121" s="71"/>
+      <c r="F121" s="71"/>
+      <c r="G121" s="71"/>
+      <c r="H121" s="71"/>
+      <c r="I121" s="71"/>
+      <c r="J121" s="71"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="70"/>
-      <c r="C122" s="67"/>
-      <c r="D122" s="67"/>
-      <c r="E122" s="67"/>
-      <c r="F122" s="67"/>
-      <c r="G122" s="67"/>
-      <c r="H122" s="67"/>
-      <c r="I122" s="67"/>
-      <c r="J122" s="71"/>
+      <c r="B122" s="72"/>
+      <c r="C122" s="69"/>
+      <c r="D122" s="69"/>
+      <c r="E122" s="69"/>
+      <c r="F122" s="69"/>
+      <c r="G122" s="69"/>
+      <c r="H122" s="69"/>
+      <c r="I122" s="69"/>
+      <c r="J122" s="73"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -4566,8 +4566,30 @@
       <c r="A123" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B123" s="8"/>
-      <c r="H123" s="72"/>
+      <c r="B123" s="8">
+        <v>4</v>
+      </c>
+      <c r="C123" s="6">
+        <v>4</v>
+      </c>
+      <c r="D123" s="6">
+        <v>4</v>
+      </c>
+      <c r="E123" s="6">
+        <v>4</v>
+      </c>
+      <c r="F123" s="6">
+        <v>4</v>
+      </c>
+      <c r="G123" s="28">
+        <v>0</v>
+      </c>
+      <c r="H123" s="67">
+        <v>4</v>
+      </c>
+      <c r="I123" s="6">
+        <v>4</v>
+      </c>
       <c r="J123" s="1"/>
       <c r="K123" s="23"/>
       <c r="L123" s="8"/>
@@ -4576,8 +4598,28 @@
       <c r="A124" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B124" s="8"/>
-      <c r="H124" s="72"/>
+      <c r="B124" s="8">
+        <v>5</v>
+      </c>
+      <c r="C124" s="6">
+        <v>5</v>
+      </c>
+      <c r="D124" s="30">
+        <v>4</v>
+      </c>
+      <c r="E124" s="6">
+        <v>5</v>
+      </c>
+      <c r="F124" s="62"/>
+      <c r="G124" s="6">
+        <v>5</v>
+      </c>
+      <c r="H124" s="67">
+        <v>5</v>
+      </c>
+      <c r="I124" s="6">
+        <v>5</v>
+      </c>
       <c r="J124" s="1"/>
       <c r="K124" s="23"/>
       <c r="L124" s="8"/>
@@ -4587,7 +4629,7 @@
         <v>2</v>
       </c>
       <c r="B125" s="8"/>
-      <c r="H125" s="72"/>
+      <c r="H125" s="67"/>
       <c r="J125" s="1"/>
       <c r="K125" s="23"/>
       <c r="L125" s="8"/>
@@ -4597,7 +4639,7 @@
         <v>3</v>
       </c>
       <c r="B126" s="8"/>
-      <c r="H126" s="72"/>
+      <c r="H126" s="67"/>
       <c r="J126" s="1"/>
       <c r="K126" s="23"/>
       <c r="L126" s="8"/>
@@ -4612,7 +4654,7 @@
       <c r="E127" s="7"/>
       <c r="F127" s="7"/>
       <c r="G127" s="65"/>
-      <c r="H127" s="73"/>
+      <c r="H127" s="68"/>
       <c r="I127" s="7"/>
       <c r="J127" s="2" t="s">
         <v>65</v>
@@ -4626,65 +4668,65 @@
       </c>
       <c r="B128" s="34">
         <f>B123+B124+B125+B126+B127</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C128" s="35">
         <f t="shared" ref="C128:I128" si="15">SUM(C123:C127)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D128" s="35">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E128" s="35">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F128" s="35">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G128" s="35">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H128" s="35">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I128" s="35">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J128" s="36"/>
       <c r="K128" s="23"/>
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A129" s="69"/>
-      <c r="B129" s="69"/>
-      <c r="C129" s="69"/>
-      <c r="D129" s="69"/>
-      <c r="E129" s="69"/>
-      <c r="F129" s="69"/>
-      <c r="G129" s="69"/>
-      <c r="H129" s="69"/>
-      <c r="I129" s="69"/>
-      <c r="J129" s="69"/>
+      <c r="A129" s="71"/>
+      <c r="B129" s="71"/>
+      <c r="C129" s="71"/>
+      <c r="D129" s="71"/>
+      <c r="E129" s="71"/>
+      <c r="F129" s="71"/>
+      <c r="G129" s="71"/>
+      <c r="H129" s="71"/>
+      <c r="I129" s="71"/>
+      <c r="J129" s="71"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="70"/>
-      <c r="C130" s="67"/>
-      <c r="D130" s="67"/>
-      <c r="E130" s="67"/>
-      <c r="F130" s="67"/>
-      <c r="G130" s="67"/>
-      <c r="H130" s="67"/>
-      <c r="I130" s="67"/>
-      <c r="J130" s="71"/>
+      <c r="B130" s="72"/>
+      <c r="C130" s="69"/>
+      <c r="D130" s="69"/>
+      <c r="E130" s="69"/>
+      <c r="F130" s="69"/>
+      <c r="G130" s="69"/>
+      <c r="H130" s="69"/>
+      <c r="I130" s="69"/>
+      <c r="J130" s="73"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -4693,7 +4735,7 @@
         <v>0</v>
       </c>
       <c r="B131" s="8"/>
-      <c r="H131" s="72"/>
+      <c r="H131" s="67"/>
       <c r="J131" s="1"/>
       <c r="K131" s="23"/>
       <c r="L131" s="8"/>
@@ -4703,7 +4745,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="8"/>
-      <c r="H132" s="72"/>
+      <c r="H132" s="67"/>
       <c r="J132" s="1"/>
       <c r="K132" s="23"/>
       <c r="L132" s="8"/>
@@ -4713,7 +4755,7 @@
         <v>2</v>
       </c>
       <c r="B133" s="8"/>
-      <c r="H133" s="72"/>
+      <c r="H133" s="67"/>
       <c r="J133" s="1"/>
       <c r="K133" s="23"/>
       <c r="L133" s="8"/>
@@ -4723,7 +4765,7 @@
         <v>3</v>
       </c>
       <c r="B134" s="8"/>
-      <c r="H134" s="72"/>
+      <c r="H134" s="67"/>
       <c r="J134" s="1"/>
       <c r="K134" s="23"/>
       <c r="L134" s="8"/>
@@ -4738,7 +4780,7 @@
       <c r="E135" s="7"/>
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
-      <c r="H135" s="73"/>
+      <c r="H135" s="68"/>
       <c r="I135" s="7"/>
       <c r="J135" s="2"/>
       <c r="K135" s="23"/>
@@ -4785,30 +4827,30 @@
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A137" s="69"/>
-      <c r="B137" s="69"/>
-      <c r="C137" s="69"/>
-      <c r="D137" s="69"/>
-      <c r="E137" s="69"/>
-      <c r="F137" s="69"/>
-      <c r="G137" s="69"/>
-      <c r="H137" s="69"/>
-      <c r="I137" s="69"/>
-      <c r="J137" s="69"/>
+      <c r="A137" s="71"/>
+      <c r="B137" s="71"/>
+      <c r="C137" s="71"/>
+      <c r="D137" s="71"/>
+      <c r="E137" s="71"/>
+      <c r="F137" s="71"/>
+      <c r="G137" s="71"/>
+      <c r="H137" s="71"/>
+      <c r="I137" s="71"/>
+      <c r="J137" s="71"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="70"/>
-      <c r="C138" s="67"/>
-      <c r="D138" s="67"/>
-      <c r="E138" s="67"/>
-      <c r="F138" s="67"/>
-      <c r="G138" s="67"/>
-      <c r="H138" s="67"/>
-      <c r="I138" s="67"/>
-      <c r="J138" s="71"/>
+      <c r="B138" s="72"/>
+      <c r="C138" s="69"/>
+      <c r="D138" s="69"/>
+      <c r="E138" s="69"/>
+      <c r="F138" s="69"/>
+      <c r="G138" s="69"/>
+      <c r="H138" s="69"/>
+      <c r="I138" s="69"/>
+      <c r="J138" s="73"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -4943,30 +4985,30 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A145" s="69"/>
-      <c r="B145" s="69"/>
-      <c r="C145" s="69"/>
-      <c r="D145" s="69"/>
-      <c r="E145" s="69"/>
-      <c r="F145" s="69"/>
-      <c r="G145" s="69"/>
-      <c r="H145" s="69"/>
-      <c r="I145" s="69"/>
-      <c r="J145" s="69"/>
+      <c r="A145" s="71"/>
+      <c r="B145" s="71"/>
+      <c r="C145" s="71"/>
+      <c r="D145" s="71"/>
+      <c r="E145" s="71"/>
+      <c r="F145" s="71"/>
+      <c r="G145" s="71"/>
+      <c r="H145" s="71"/>
+      <c r="I145" s="71"/>
+      <c r="J145" s="71"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="70"/>
-      <c r="C146" s="67"/>
-      <c r="D146" s="67"/>
-      <c r="E146" s="67"/>
-      <c r="F146" s="67"/>
-      <c r="G146" s="67"/>
-      <c r="H146" s="67"/>
-      <c r="I146" s="67"/>
-      <c r="J146" s="71"/>
+      <c r="B146" s="72"/>
+      <c r="C146" s="69"/>
+      <c r="D146" s="69"/>
+      <c r="E146" s="69"/>
+      <c r="F146" s="69"/>
+      <c r="G146" s="69"/>
+      <c r="H146" s="69"/>
+      <c r="I146" s="69"/>
+      <c r="J146" s="73"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -4975,7 +5017,7 @@
         <v>0</v>
       </c>
       <c r="B147" s="8"/>
-      <c r="H147" s="72"/>
+      <c r="H147" s="67"/>
       <c r="J147" s="1"/>
       <c r="K147" s="23"/>
       <c r="L147" s="8"/>
@@ -4985,7 +5027,7 @@
         <v>1</v>
       </c>
       <c r="B148" s="8"/>
-      <c r="H148" s="72"/>
+      <c r="H148" s="67"/>
       <c r="J148" s="1"/>
       <c r="K148" s="23"/>
       <c r="L148" s="8"/>
@@ -4995,7 +5037,7 @@
         <v>2</v>
       </c>
       <c r="B149" s="8"/>
-      <c r="H149" s="72"/>
+      <c r="H149" s="67"/>
       <c r="J149" s="1"/>
       <c r="K149" s="23"/>
       <c r="L149" s="8"/>
@@ -5005,7 +5047,7 @@
         <v>3</v>
       </c>
       <c r="B150" s="8"/>
-      <c r="H150" s="72"/>
+      <c r="H150" s="67"/>
       <c r="J150" s="1"/>
       <c r="K150" s="23"/>
       <c r="L150" s="8"/>
@@ -5020,7 +5062,7 @@
       <c r="E151" s="7"/>
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
-      <c r="H151" s="73"/>
+      <c r="H151" s="68"/>
       <c r="I151" s="7"/>
       <c r="J151" s="2"/>
       <c r="K151" s="23"/>
@@ -5067,30 +5109,30 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A153" s="69"/>
-      <c r="B153" s="69"/>
-      <c r="C153" s="69"/>
-      <c r="D153" s="69"/>
-      <c r="E153" s="69"/>
-      <c r="F153" s="69"/>
-      <c r="G153" s="69"/>
-      <c r="H153" s="69"/>
-      <c r="I153" s="69"/>
-      <c r="J153" s="69"/>
+      <c r="A153" s="71"/>
+      <c r="B153" s="71"/>
+      <c r="C153" s="71"/>
+      <c r="D153" s="71"/>
+      <c r="E153" s="71"/>
+      <c r="F153" s="71"/>
+      <c r="G153" s="71"/>
+      <c r="H153" s="71"/>
+      <c r="I153" s="71"/>
+      <c r="J153" s="71"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="70"/>
-      <c r="C154" s="67"/>
-      <c r="D154" s="67"/>
-      <c r="E154" s="67"/>
-      <c r="F154" s="67"/>
-      <c r="G154" s="67"/>
-      <c r="H154" s="67"/>
-      <c r="I154" s="67"/>
-      <c r="J154" s="71"/>
+      <c r="B154" s="72"/>
+      <c r="C154" s="69"/>
+      <c r="D154" s="69"/>
+      <c r="E154" s="69"/>
+      <c r="F154" s="69"/>
+      <c r="G154" s="69"/>
+      <c r="H154" s="69"/>
+      <c r="I154" s="69"/>
+      <c r="J154" s="73"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -5099,7 +5141,7 @@
         <v>0</v>
       </c>
       <c r="B155" s="8"/>
-      <c r="H155" s="72"/>
+      <c r="H155" s="67"/>
       <c r="J155" s="1"/>
       <c r="K155" s="23"/>
       <c r="L155" s="8"/>
@@ -5109,7 +5151,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="8"/>
-      <c r="H156" s="72"/>
+      <c r="H156" s="67"/>
       <c r="J156" s="1"/>
       <c r="K156" s="23"/>
       <c r="L156" s="8"/>
@@ -5119,7 +5161,7 @@
         <v>2</v>
       </c>
       <c r="B157" s="8"/>
-      <c r="H157" s="72"/>
+      <c r="H157" s="67"/>
       <c r="J157" s="1"/>
       <c r="K157" s="23"/>
       <c r="L157" s="8"/>
@@ -5129,7 +5171,7 @@
         <v>3</v>
       </c>
       <c r="B158" s="8"/>
-      <c r="H158" s="72"/>
+      <c r="H158" s="67"/>
       <c r="J158" s="1"/>
       <c r="K158" s="23"/>
       <c r="L158" s="8"/>
@@ -5144,7 +5186,7 @@
       <c r="E159" s="7"/>
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
-      <c r="H159" s="73"/>
+      <c r="H159" s="68"/>
       <c r="I159" s="7"/>
       <c r="J159" s="2"/>
       <c r="K159" s="23"/>
@@ -5191,30 +5233,30 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A161" s="69"/>
-      <c r="B161" s="69"/>
-      <c r="C161" s="69"/>
-      <c r="D161" s="69"/>
-      <c r="E161" s="69"/>
-      <c r="F161" s="69"/>
-      <c r="G161" s="69"/>
-      <c r="H161" s="69"/>
-      <c r="I161" s="69"/>
-      <c r="J161" s="69"/>
+      <c r="A161" s="71"/>
+      <c r="B161" s="71"/>
+      <c r="C161" s="71"/>
+      <c r="D161" s="71"/>
+      <c r="E161" s="71"/>
+      <c r="F161" s="71"/>
+      <c r="G161" s="71"/>
+      <c r="H161" s="71"/>
+      <c r="I161" s="71"/>
+      <c r="J161" s="71"/>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="70"/>
-      <c r="C162" s="67"/>
-      <c r="D162" s="67"/>
-      <c r="E162" s="67"/>
-      <c r="F162" s="67"/>
-      <c r="G162" s="67"/>
-      <c r="H162" s="67"/>
-      <c r="I162" s="67"/>
-      <c r="J162" s="71"/>
+      <c r="B162" s="72"/>
+      <c r="C162" s="69"/>
+      <c r="D162" s="69"/>
+      <c r="E162" s="69"/>
+      <c r="F162" s="69"/>
+      <c r="G162" s="69"/>
+      <c r="H162" s="69"/>
+      <c r="I162" s="69"/>
+      <c r="J162" s="73"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -5223,7 +5265,7 @@
         <v>0</v>
       </c>
       <c r="B163" s="8"/>
-      <c r="H163" s="72"/>
+      <c r="H163" s="67"/>
       <c r="J163" s="1"/>
       <c r="K163" s="23"/>
       <c r="L163" s="8"/>
@@ -5233,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="B164" s="8"/>
-      <c r="H164" s="72"/>
+      <c r="H164" s="67"/>
       <c r="J164" s="1"/>
       <c r="K164" s="23"/>
       <c r="L164" s="8"/>
@@ -5243,7 +5285,7 @@
         <v>2</v>
       </c>
       <c r="B165" s="8"/>
-      <c r="H165" s="72"/>
+      <c r="H165" s="67"/>
       <c r="J165" s="1"/>
       <c r="K165" s="23"/>
       <c r="L165" s="8"/>
@@ -5253,7 +5295,7 @@
         <v>3</v>
       </c>
       <c r="B166" s="8"/>
-      <c r="H166" s="72"/>
+      <c r="H166" s="67"/>
       <c r="J166" s="1"/>
       <c r="K166" s="23"/>
       <c r="L166" s="8"/>
@@ -5268,7 +5310,7 @@
       <c r="E167" s="7"/>
       <c r="F167" s="7"/>
       <c r="G167" s="7"/>
-      <c r="H167" s="73"/>
+      <c r="H167" s="68"/>
       <c r="I167" s="7"/>
       <c r="J167" s="2"/>
       <c r="K167" s="23"/>
@@ -5315,30 +5357,30 @@
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A169" s="69"/>
-      <c r="B169" s="69"/>
-      <c r="C169" s="69"/>
-      <c r="D169" s="69"/>
-      <c r="E169" s="69"/>
-      <c r="F169" s="69"/>
-      <c r="G169" s="69"/>
-      <c r="H169" s="69"/>
-      <c r="I169" s="69"/>
-      <c r="J169" s="69"/>
+      <c r="A169" s="71"/>
+      <c r="B169" s="71"/>
+      <c r="C169" s="71"/>
+      <c r="D169" s="71"/>
+      <c r="E169" s="71"/>
+      <c r="F169" s="71"/>
+      <c r="G169" s="71"/>
+      <c r="H169" s="71"/>
+      <c r="I169" s="71"/>
+      <c r="J169" s="71"/>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="70"/>
-      <c r="C170" s="67"/>
-      <c r="D170" s="67"/>
-      <c r="E170" s="67"/>
-      <c r="F170" s="67"/>
-      <c r="G170" s="67"/>
-      <c r="H170" s="67"/>
-      <c r="I170" s="67"/>
-      <c r="J170" s="71"/>
+      <c r="B170" s="72"/>
+      <c r="C170" s="69"/>
+      <c r="D170" s="69"/>
+      <c r="E170" s="69"/>
+      <c r="F170" s="69"/>
+      <c r="G170" s="69"/>
+      <c r="H170" s="69"/>
+      <c r="I170" s="69"/>
+      <c r="J170" s="73"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -5347,7 +5389,7 @@
         <v>0</v>
       </c>
       <c r="B171" s="8"/>
-      <c r="H171" s="72"/>
+      <c r="H171" s="67"/>
       <c r="J171" s="1"/>
       <c r="K171" s="23"/>
       <c r="L171" s="8"/>
@@ -5357,7 +5399,7 @@
         <v>1</v>
       </c>
       <c r="B172" s="8"/>
-      <c r="H172" s="72"/>
+      <c r="H172" s="67"/>
       <c r="J172" s="1"/>
       <c r="K172" s="23"/>
       <c r="L172" s="8"/>
@@ -5367,7 +5409,7 @@
         <v>2</v>
       </c>
       <c r="B173" s="8"/>
-      <c r="H173" s="72"/>
+      <c r="H173" s="67"/>
       <c r="J173" s="1"/>
       <c r="K173" s="23"/>
       <c r="L173" s="8"/>
@@ -5377,7 +5419,7 @@
         <v>3</v>
       </c>
       <c r="B174" s="8"/>
-      <c r="H174" s="72"/>
+      <c r="H174" s="67"/>
       <c r="J174" s="1"/>
       <c r="K174" s="23"/>
       <c r="L174" s="8"/>
@@ -5392,7 +5434,7 @@
       <c r="E175" s="7"/>
       <c r="F175" s="7"/>
       <c r="G175" s="7"/>
-      <c r="H175" s="73"/>
+      <c r="H175" s="68"/>
       <c r="I175" s="7"/>
       <c r="J175" s="2"/>
       <c r="K175" s="23"/>
@@ -5439,28 +5481,28 @@
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="67"/>
-      <c r="B177" s="67"/>
-      <c r="C177" s="67"/>
-      <c r="D177" s="67"/>
-      <c r="E177" s="67"/>
-      <c r="F177" s="67"/>
-      <c r="G177" s="67"/>
-      <c r="H177" s="67"/>
-      <c r="I177" s="67"/>
-      <c r="J177" s="67"/>
+      <c r="A177" s="69"/>
+      <c r="B177" s="69"/>
+      <c r="C177" s="69"/>
+      <c r="D177" s="69"/>
+      <c r="E177" s="69"/>
+      <c r="F177" s="69"/>
+      <c r="G177" s="69"/>
+      <c r="H177" s="69"/>
+      <c r="I177" s="69"/>
+      <c r="J177" s="69"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="68"/>
-      <c r="B178" s="68"/>
-      <c r="C178" s="68"/>
-      <c r="D178" s="68"/>
-      <c r="E178" s="68"/>
-      <c r="F178" s="68"/>
-      <c r="G178" s="68"/>
-      <c r="H178" s="68"/>
-      <c r="I178" s="68"/>
-      <c r="J178" s="68"/>
+      <c r="A178" s="70"/>
+      <c r="B178" s="70"/>
+      <c r="C178" s="70"/>
+      <c r="D178" s="70"/>
+      <c r="E178" s="70"/>
+      <c r="F178" s="70"/>
+      <c r="G178" s="70"/>
+      <c r="H178" s="70"/>
+      <c r="I178" s="70"/>
+      <c r="J178" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="45">

</xml_diff>

<commit_message>
Animaties + uren reg
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="66">
   <si>
     <t>Maandag</t>
   </si>
@@ -730,19 +730,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1025,7 +1025,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1036,8 +1036,8 @@
   <dimension ref="A1:P178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J125" sqref="J125"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L126" sqref="L126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1097,29 +1097,29 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="73"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.99303135888501737</v>
+        <v>0.9932659932659933</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>35</v>
@@ -1163,11 +1163,11 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.83972125435540068</v>
+        <v>0.84175084175084181</v>
       </c>
       <c r="O3" s="54" t="s">
         <v>34</v>
@@ -1211,11 +1211,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.99303135888501737</v>
+        <v>0.9932659932659933</v>
       </c>
       <c r="O4" s="55" t="s">
         <v>36</v>
@@ -1259,11 +1259,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.93031358885017423</v>
+        <v>0.92592592592592593</v>
       </c>
       <c r="O5" s="56" t="s">
         <v>37</v>
@@ -1293,11 +1293,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.78397212543554007</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="O6" s="57" t="s">
         <v>38</v>
@@ -1341,11 +1341,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.68292682926829273</v>
+        <v>0.69360269360269355</v>
       </c>
       <c r="O7" s="58" t="s">
         <v>39</v>
@@ -1395,11 +1395,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.97560975609756095</v>
+        <v>0.97643097643097643</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>40</v>
@@ -1409,30 +1409,30 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A9" s="72"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="71"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="73"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1639,30 +1639,30 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="72"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="71"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="73"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1867,30 +1867,30 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="72"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="71"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="73"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -2095,30 +2095,30 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="72"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
+      <c r="A33" s="71"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="69"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="71"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="73"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2325,30 +2325,30 @@
       <c r="L40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A41" s="72"/>
-      <c r="B41" s="72"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="72"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="72"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="69"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
-      <c r="J42" s="71"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="73"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2557,30 +2557,30 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="72"/>
-      <c r="B49" s="72"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="72"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="72"/>
-      <c r="G49" s="72"/>
-      <c r="H49" s="72"/>
-      <c r="I49" s="72"/>
-      <c r="J49" s="72"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="71"/>
+      <c r="I49" s="71"/>
+      <c r="J49" s="71"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="69"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
-      <c r="F50" s="70"/>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="71"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="69"/>
+      <c r="J50" s="73"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2785,30 +2785,30 @@
       <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="72"/>
-      <c r="B57" s="72"/>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
-      <c r="E57" s="72"/>
-      <c r="F57" s="72"/>
-      <c r="G57" s="72"/>
-      <c r="H57" s="72"/>
-      <c r="I57" s="72"/>
-      <c r="J57" s="72"/>
+      <c r="A57" s="71"/>
+      <c r="B57" s="71"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="71"/>
+      <c r="E57" s="71"/>
+      <c r="F57" s="71"/>
+      <c r="G57" s="71"/>
+      <c r="H57" s="71"/>
+      <c r="I57" s="71"/>
+      <c r="J57" s="71"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="69"/>
-      <c r="C58" s="70"/>
-      <c r="D58" s="70"/>
-      <c r="E58" s="70"/>
-      <c r="F58" s="70"/>
-      <c r="G58" s="70"/>
-      <c r="H58" s="70"/>
-      <c r="I58" s="70"/>
-      <c r="J58" s="71"/>
+      <c r="B58" s="72"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="69"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="69"/>
+      <c r="G58" s="69"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="69"/>
+      <c r="J58" s="73"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -3017,30 +3017,30 @@
       <c r="L64" s="8"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A65" s="72"/>
-      <c r="B65" s="72"/>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="72"/>
-      <c r="H65" s="72"/>
-      <c r="I65" s="72"/>
-      <c r="J65" s="72"/>
+      <c r="A65" s="71"/>
+      <c r="B65" s="71"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71"/>
+      <c r="J65" s="71"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="69"/>
-      <c r="C66" s="70"/>
-      <c r="D66" s="70"/>
-      <c r="E66" s="70"/>
-      <c r="F66" s="70"/>
-      <c r="G66" s="70"/>
-      <c r="H66" s="70"/>
-      <c r="I66" s="70"/>
-      <c r="J66" s="71"/>
+      <c r="B66" s="72"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="69"/>
+      <c r="E66" s="69"/>
+      <c r="F66" s="69"/>
+      <c r="G66" s="69"/>
+      <c r="H66" s="69"/>
+      <c r="I66" s="69"/>
+      <c r="J66" s="73"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -3175,30 +3175,30 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A73" s="72"/>
-      <c r="B73" s="72"/>
-      <c r="C73" s="72"/>
-      <c r="D73" s="72"/>
-      <c r="E73" s="72"/>
-      <c r="F73" s="72"/>
-      <c r="G73" s="72"/>
-      <c r="H73" s="72"/>
-      <c r="I73" s="72"/>
-      <c r="J73" s="72"/>
+      <c r="A73" s="71"/>
+      <c r="B73" s="71"/>
+      <c r="C73" s="71"/>
+      <c r="D73" s="71"/>
+      <c r="E73" s="71"/>
+      <c r="F73" s="71"/>
+      <c r="G73" s="71"/>
+      <c r="H73" s="71"/>
+      <c r="I73" s="71"/>
+      <c r="J73" s="71"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="69"/>
-      <c r="C74" s="70"/>
-      <c r="D74" s="70"/>
-      <c r="E74" s="70"/>
-      <c r="F74" s="70"/>
-      <c r="G74" s="70"/>
-      <c r="H74" s="70"/>
-      <c r="I74" s="70"/>
-      <c r="J74" s="71"/>
+      <c r="B74" s="72"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="69"/>
+      <c r="F74" s="69"/>
+      <c r="G74" s="69"/>
+      <c r="H74" s="69"/>
+      <c r="I74" s="69"/>
+      <c r="J74" s="73"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3389,30 +3389,30 @@
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A81" s="72"/>
-      <c r="B81" s="72"/>
-      <c r="C81" s="72"/>
-      <c r="D81" s="72"/>
-      <c r="E81" s="72"/>
-      <c r="F81" s="72"/>
-      <c r="G81" s="72"/>
-      <c r="H81" s="72"/>
-      <c r="I81" s="72"/>
-      <c r="J81" s="72"/>
+      <c r="A81" s="71"/>
+      <c r="B81" s="71"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="71"/>
+      <c r="E81" s="71"/>
+      <c r="F81" s="71"/>
+      <c r="G81" s="71"/>
+      <c r="H81" s="71"/>
+      <c r="I81" s="71"/>
+      <c r="J81" s="71"/>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="69"/>
-      <c r="C82" s="70"/>
-      <c r="D82" s="70"/>
-      <c r="E82" s="70"/>
-      <c r="F82" s="70"/>
-      <c r="G82" s="70"/>
-      <c r="H82" s="70"/>
-      <c r="I82" s="70"/>
-      <c r="J82" s="71"/>
+      <c r="B82" s="72"/>
+      <c r="C82" s="69"/>
+      <c r="D82" s="69"/>
+      <c r="E82" s="69"/>
+      <c r="F82" s="69"/>
+      <c r="G82" s="69"/>
+      <c r="H82" s="69"/>
+      <c r="I82" s="69"/>
+      <c r="J82" s="73"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3619,30 +3619,30 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A89" s="72"/>
-      <c r="B89" s="72"/>
-      <c r="C89" s="72"/>
-      <c r="D89" s="72"/>
-      <c r="E89" s="72"/>
-      <c r="F89" s="72"/>
-      <c r="G89" s="72"/>
-      <c r="H89" s="72"/>
-      <c r="I89" s="72"/>
-      <c r="J89" s="72"/>
+      <c r="A89" s="71"/>
+      <c r="B89" s="71"/>
+      <c r="C89" s="71"/>
+      <c r="D89" s="71"/>
+      <c r="E89" s="71"/>
+      <c r="F89" s="71"/>
+      <c r="G89" s="71"/>
+      <c r="H89" s="71"/>
+      <c r="I89" s="71"/>
+      <c r="J89" s="71"/>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="69"/>
-      <c r="C90" s="70"/>
-      <c r="D90" s="70"/>
-      <c r="E90" s="70"/>
-      <c r="F90" s="70"/>
-      <c r="G90" s="70"/>
-      <c r="H90" s="70"/>
-      <c r="I90" s="70"/>
-      <c r="J90" s="71"/>
+      <c r="B90" s="72"/>
+      <c r="C90" s="69"/>
+      <c r="D90" s="69"/>
+      <c r="E90" s="69"/>
+      <c r="F90" s="69"/>
+      <c r="G90" s="69"/>
+      <c r="H90" s="69"/>
+      <c r="I90" s="69"/>
+      <c r="J90" s="73"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3847,30 +3847,30 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A97" s="72"/>
-      <c r="B97" s="72"/>
-      <c r="C97" s="72"/>
-      <c r="D97" s="72"/>
-      <c r="E97" s="72"/>
-      <c r="F97" s="72"/>
-      <c r="G97" s="72"/>
-      <c r="H97" s="72"/>
-      <c r="I97" s="72"/>
-      <c r="J97" s="72"/>
+      <c r="A97" s="71"/>
+      <c r="B97" s="71"/>
+      <c r="C97" s="71"/>
+      <c r="D97" s="71"/>
+      <c r="E97" s="71"/>
+      <c r="F97" s="71"/>
+      <c r="G97" s="71"/>
+      <c r="H97" s="71"/>
+      <c r="I97" s="71"/>
+      <c r="J97" s="71"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="69"/>
-      <c r="C98" s="70"/>
-      <c r="D98" s="70"/>
-      <c r="E98" s="70"/>
-      <c r="F98" s="70"/>
-      <c r="G98" s="70"/>
-      <c r="H98" s="70"/>
-      <c r="I98" s="70"/>
-      <c r="J98" s="71"/>
+      <c r="B98" s="72"/>
+      <c r="C98" s="69"/>
+      <c r="D98" s="69"/>
+      <c r="E98" s="69"/>
+      <c r="F98" s="69"/>
+      <c r="G98" s="69"/>
+      <c r="H98" s="69"/>
+      <c r="I98" s="69"/>
+      <c r="J98" s="73"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -4077,30 +4077,30 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A105" s="72"/>
-      <c r="B105" s="72"/>
-      <c r="C105" s="72"/>
-      <c r="D105" s="72"/>
-      <c r="E105" s="72"/>
-      <c r="F105" s="72"/>
-      <c r="G105" s="72"/>
-      <c r="H105" s="72"/>
-      <c r="I105" s="72"/>
-      <c r="J105" s="72"/>
+      <c r="A105" s="71"/>
+      <c r="B105" s="71"/>
+      <c r="C105" s="71"/>
+      <c r="D105" s="71"/>
+      <c r="E105" s="71"/>
+      <c r="F105" s="71"/>
+      <c r="G105" s="71"/>
+      <c r="H105" s="71"/>
+      <c r="I105" s="71"/>
+      <c r="J105" s="71"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="69"/>
-      <c r="C106" s="70"/>
-      <c r="D106" s="70"/>
-      <c r="E106" s="70"/>
-      <c r="F106" s="70"/>
-      <c r="G106" s="70"/>
-      <c r="H106" s="70"/>
-      <c r="I106" s="70"/>
-      <c r="J106" s="71"/>
+      <c r="B106" s="72"/>
+      <c r="C106" s="69"/>
+      <c r="D106" s="69"/>
+      <c r="E106" s="69"/>
+      <c r="F106" s="69"/>
+      <c r="G106" s="69"/>
+      <c r="H106" s="69"/>
+      <c r="I106" s="69"/>
+      <c r="J106" s="73"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -4307,30 +4307,30 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A113" s="72"/>
-      <c r="B113" s="72"/>
-      <c r="C113" s="72"/>
-      <c r="D113" s="72"/>
-      <c r="E113" s="72"/>
-      <c r="F113" s="72"/>
-      <c r="G113" s="72"/>
-      <c r="H113" s="72"/>
-      <c r="I113" s="72"/>
-      <c r="J113" s="72"/>
+      <c r="A113" s="71"/>
+      <c r="B113" s="71"/>
+      <c r="C113" s="71"/>
+      <c r="D113" s="71"/>
+      <c r="E113" s="71"/>
+      <c r="F113" s="71"/>
+      <c r="G113" s="71"/>
+      <c r="H113" s="71"/>
+      <c r="I113" s="71"/>
+      <c r="J113" s="71"/>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="69"/>
-      <c r="C114" s="70"/>
-      <c r="D114" s="70"/>
-      <c r="E114" s="70"/>
-      <c r="F114" s="70"/>
-      <c r="G114" s="70"/>
-      <c r="H114" s="70"/>
-      <c r="I114" s="70"/>
-      <c r="J114" s="71"/>
+      <c r="B114" s="72"/>
+      <c r="C114" s="69"/>
+      <c r="D114" s="69"/>
+      <c r="E114" s="69"/>
+      <c r="F114" s="69"/>
+      <c r="G114" s="69"/>
+      <c r="H114" s="69"/>
+      <c r="I114" s="69"/>
+      <c r="J114" s="73"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -4535,30 +4535,30 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A121" s="72"/>
-      <c r="B121" s="72"/>
-      <c r="C121" s="72"/>
-      <c r="D121" s="72"/>
-      <c r="E121" s="72"/>
-      <c r="F121" s="72"/>
-      <c r="G121" s="72"/>
-      <c r="H121" s="72"/>
-      <c r="I121" s="72"/>
-      <c r="J121" s="72"/>
+      <c r="A121" s="71"/>
+      <c r="B121" s="71"/>
+      <c r="C121" s="71"/>
+      <c r="D121" s="71"/>
+      <c r="E121" s="71"/>
+      <c r="F121" s="71"/>
+      <c r="G121" s="71"/>
+      <c r="H121" s="71"/>
+      <c r="I121" s="71"/>
+      <c r="J121" s="71"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="69"/>
-      <c r="C122" s="70"/>
-      <c r="D122" s="70"/>
-      <c r="E122" s="70"/>
-      <c r="F122" s="70"/>
-      <c r="G122" s="70"/>
-      <c r="H122" s="70"/>
-      <c r="I122" s="70"/>
-      <c r="J122" s="71"/>
+      <c r="B122" s="72"/>
+      <c r="C122" s="69"/>
+      <c r="D122" s="69"/>
+      <c r="E122" s="69"/>
+      <c r="F122" s="69"/>
+      <c r="G122" s="69"/>
+      <c r="H122" s="69"/>
+      <c r="I122" s="69"/>
+      <c r="J122" s="73"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -4627,12 +4627,20 @@
       <c r="L124" s="8"/>
     </row>
     <row r="125" spans="1:12">
-      <c r="A125" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B125" s="8"/>
-      <c r="H125" s="67"/>
-      <c r="J125" s="1"/>
+      <c r="A125" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B125" s="20"/>
+      <c r="C125" s="21"/>
+      <c r="D125" s="21"/>
+      <c r="E125" s="21"/>
+      <c r="F125" s="21"/>
+      <c r="G125" s="21"/>
+      <c r="H125" s="21"/>
+      <c r="I125" s="21"/>
+      <c r="J125" s="22" t="s">
+        <v>41</v>
+      </c>
       <c r="K125" s="23"/>
       <c r="L125" s="8"/>
     </row>
@@ -4640,8 +4648,30 @@
       <c r="A126" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B126" s="8"/>
-      <c r="H126" s="67"/>
+      <c r="B126" s="8">
+        <v>2</v>
+      </c>
+      <c r="C126" s="6">
+        <v>2</v>
+      </c>
+      <c r="D126" s="6">
+        <v>2</v>
+      </c>
+      <c r="E126" s="6">
+        <v>2</v>
+      </c>
+      <c r="F126" s="6">
+        <v>2</v>
+      </c>
+      <c r="G126" s="6">
+        <v>2</v>
+      </c>
+      <c r="H126" s="67">
+        <v>2</v>
+      </c>
+      <c r="I126" s="6">
+        <v>2</v>
+      </c>
       <c r="J126" s="1"/>
       <c r="K126" s="23"/>
       <c r="L126" s="8"/>
@@ -4650,14 +4680,30 @@
       <c r="A127" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B127" s="7"/>
-      <c r="C127" s="7"/>
-      <c r="D127" s="7"/>
-      <c r="E127" s="7"/>
-      <c r="F127" s="7"/>
-      <c r="G127" s="65"/>
-      <c r="H127" s="68"/>
-      <c r="I127" s="7"/>
+      <c r="B127" s="7">
+        <v>4</v>
+      </c>
+      <c r="C127" s="7">
+        <v>4</v>
+      </c>
+      <c r="D127" s="7">
+        <v>4</v>
+      </c>
+      <c r="E127" s="7">
+        <v>4</v>
+      </c>
+      <c r="F127" s="31">
+        <v>2</v>
+      </c>
+      <c r="G127" s="65">
+        <v>0</v>
+      </c>
+      <c r="H127" s="68">
+        <v>4</v>
+      </c>
+      <c r="I127" s="7">
+        <v>4</v>
+      </c>
       <c r="J127" s="2" t="s">
         <v>65</v>
       </c>
@@ -4670,65 +4716,65 @@
       </c>
       <c r="B128" s="34">
         <f>B123+B124+B125+B126+B127</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C128" s="35">
         <f t="shared" ref="C128:I128" si="15">SUM(C123:C127)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D128" s="35">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E128" s="35">
         <f t="shared" si="15"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F128" s="35">
         <f t="shared" si="15"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G128" s="35">
         <f t="shared" si="15"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H128" s="35">
         <f t="shared" si="15"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I128" s="35">
         <f t="shared" si="15"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J128" s="36"/>
       <c r="K128" s="23"/>
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A129" s="72"/>
-      <c r="B129" s="72"/>
-      <c r="C129" s="72"/>
-      <c r="D129" s="72"/>
-      <c r="E129" s="72"/>
-      <c r="F129" s="72"/>
-      <c r="G129" s="72"/>
-      <c r="H129" s="72"/>
-      <c r="I129" s="72"/>
-      <c r="J129" s="72"/>
+      <c r="A129" s="71"/>
+      <c r="B129" s="71"/>
+      <c r="C129" s="71"/>
+      <c r="D129" s="71"/>
+      <c r="E129" s="71"/>
+      <c r="F129" s="71"/>
+      <c r="G129" s="71"/>
+      <c r="H129" s="71"/>
+      <c r="I129" s="71"/>
+      <c r="J129" s="71"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="69"/>
-      <c r="C130" s="70"/>
-      <c r="D130" s="70"/>
-      <c r="E130" s="70"/>
-      <c r="F130" s="70"/>
-      <c r="G130" s="70"/>
-      <c r="H130" s="70"/>
-      <c r="I130" s="70"/>
-      <c r="J130" s="71"/>
+      <c r="B130" s="72"/>
+      <c r="C130" s="69"/>
+      <c r="D130" s="69"/>
+      <c r="E130" s="69"/>
+      <c r="F130" s="69"/>
+      <c r="G130" s="69"/>
+      <c r="H130" s="69"/>
+      <c r="I130" s="69"/>
+      <c r="J130" s="73"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -4736,8 +4782,30 @@
       <c r="A131" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B131" s="8"/>
-      <c r="H131" s="67"/>
+      <c r="B131" s="8">
+        <v>4</v>
+      </c>
+      <c r="C131" s="6">
+        <v>4</v>
+      </c>
+      <c r="D131" s="30">
+        <v>3</v>
+      </c>
+      <c r="E131" s="6">
+        <v>4</v>
+      </c>
+      <c r="F131" s="6">
+        <v>4</v>
+      </c>
+      <c r="G131" s="6">
+        <v>4</v>
+      </c>
+      <c r="H131" s="67">
+        <v>4</v>
+      </c>
+      <c r="I131" s="6">
+        <v>4</v>
+      </c>
       <c r="J131" s="1"/>
       <c r="K131" s="23"/>
       <c r="L131" s="8"/>
@@ -4794,65 +4862,65 @@
       </c>
       <c r="B136" s="34">
         <f>B131+B132+B133+B134+B135</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C136" s="35">
         <f t="shared" ref="C136:I136" si="16">SUM(C131:C135)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D136" s="35">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E136" s="35">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F136" s="35">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G136" s="35">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H136" s="35">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I136" s="35">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J136" s="36"/>
       <c r="K136" s="23"/>
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A137" s="72"/>
-      <c r="B137" s="72"/>
-      <c r="C137" s="72"/>
-      <c r="D137" s="72"/>
-      <c r="E137" s="72"/>
-      <c r="F137" s="72"/>
-      <c r="G137" s="72"/>
-      <c r="H137" s="72"/>
-      <c r="I137" s="72"/>
-      <c r="J137" s="72"/>
+      <c r="A137" s="71"/>
+      <c r="B137" s="71"/>
+      <c r="C137" s="71"/>
+      <c r="D137" s="71"/>
+      <c r="E137" s="71"/>
+      <c r="F137" s="71"/>
+      <c r="G137" s="71"/>
+      <c r="H137" s="71"/>
+      <c r="I137" s="71"/>
+      <c r="J137" s="71"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="69"/>
-      <c r="C138" s="70"/>
-      <c r="D138" s="70"/>
-      <c r="E138" s="70"/>
-      <c r="F138" s="70"/>
-      <c r="G138" s="70"/>
-      <c r="H138" s="70"/>
-      <c r="I138" s="70"/>
-      <c r="J138" s="71"/>
+      <c r="B138" s="72"/>
+      <c r="C138" s="69"/>
+      <c r="D138" s="69"/>
+      <c r="E138" s="69"/>
+      <c r="F138" s="69"/>
+      <c r="G138" s="69"/>
+      <c r="H138" s="69"/>
+      <c r="I138" s="69"/>
+      <c r="J138" s="73"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -4987,30 +5055,30 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A145" s="72"/>
-      <c r="B145" s="72"/>
-      <c r="C145" s="72"/>
-      <c r="D145" s="72"/>
-      <c r="E145" s="72"/>
-      <c r="F145" s="72"/>
-      <c r="G145" s="72"/>
-      <c r="H145" s="72"/>
-      <c r="I145" s="72"/>
-      <c r="J145" s="72"/>
+      <c r="A145" s="71"/>
+      <c r="B145" s="71"/>
+      <c r="C145" s="71"/>
+      <c r="D145" s="71"/>
+      <c r="E145" s="71"/>
+      <c r="F145" s="71"/>
+      <c r="G145" s="71"/>
+      <c r="H145" s="71"/>
+      <c r="I145" s="71"/>
+      <c r="J145" s="71"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="69"/>
-      <c r="C146" s="70"/>
-      <c r="D146" s="70"/>
-      <c r="E146" s="70"/>
-      <c r="F146" s="70"/>
-      <c r="G146" s="70"/>
-      <c r="H146" s="70"/>
-      <c r="I146" s="70"/>
-      <c r="J146" s="71"/>
+      <c r="B146" s="72"/>
+      <c r="C146" s="69"/>
+      <c r="D146" s="69"/>
+      <c r="E146" s="69"/>
+      <c r="F146" s="69"/>
+      <c r="G146" s="69"/>
+      <c r="H146" s="69"/>
+      <c r="I146" s="69"/>
+      <c r="J146" s="73"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -5111,30 +5179,30 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A153" s="72"/>
-      <c r="B153" s="72"/>
-      <c r="C153" s="72"/>
-      <c r="D153" s="72"/>
-      <c r="E153" s="72"/>
-      <c r="F153" s="72"/>
-      <c r="G153" s="72"/>
-      <c r="H153" s="72"/>
-      <c r="I153" s="72"/>
-      <c r="J153" s="72"/>
+      <c r="A153" s="71"/>
+      <c r="B153" s="71"/>
+      <c r="C153" s="71"/>
+      <c r="D153" s="71"/>
+      <c r="E153" s="71"/>
+      <c r="F153" s="71"/>
+      <c r="G153" s="71"/>
+      <c r="H153" s="71"/>
+      <c r="I153" s="71"/>
+      <c r="J153" s="71"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="69"/>
-      <c r="C154" s="70"/>
-      <c r="D154" s="70"/>
-      <c r="E154" s="70"/>
-      <c r="F154" s="70"/>
-      <c r="G154" s="70"/>
-      <c r="H154" s="70"/>
-      <c r="I154" s="70"/>
-      <c r="J154" s="71"/>
+      <c r="B154" s="72"/>
+      <c r="C154" s="69"/>
+      <c r="D154" s="69"/>
+      <c r="E154" s="69"/>
+      <c r="F154" s="69"/>
+      <c r="G154" s="69"/>
+      <c r="H154" s="69"/>
+      <c r="I154" s="69"/>
+      <c r="J154" s="73"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -5235,30 +5303,30 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A161" s="72"/>
-      <c r="B161" s="72"/>
-      <c r="C161" s="72"/>
-      <c r="D161" s="72"/>
-      <c r="E161" s="72"/>
-      <c r="F161" s="72"/>
-      <c r="G161" s="72"/>
-      <c r="H161" s="72"/>
-      <c r="I161" s="72"/>
-      <c r="J161" s="72"/>
+      <c r="A161" s="71"/>
+      <c r="B161" s="71"/>
+      <c r="C161" s="71"/>
+      <c r="D161" s="71"/>
+      <c r="E161" s="71"/>
+      <c r="F161" s="71"/>
+      <c r="G161" s="71"/>
+      <c r="H161" s="71"/>
+      <c r="I161" s="71"/>
+      <c r="J161" s="71"/>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="69"/>
-      <c r="C162" s="70"/>
-      <c r="D162" s="70"/>
-      <c r="E162" s="70"/>
-      <c r="F162" s="70"/>
-      <c r="G162" s="70"/>
-      <c r="H162" s="70"/>
-      <c r="I162" s="70"/>
-      <c r="J162" s="71"/>
+      <c r="B162" s="72"/>
+      <c r="C162" s="69"/>
+      <c r="D162" s="69"/>
+      <c r="E162" s="69"/>
+      <c r="F162" s="69"/>
+      <c r="G162" s="69"/>
+      <c r="H162" s="69"/>
+      <c r="I162" s="69"/>
+      <c r="J162" s="73"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -5359,30 +5427,30 @@
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A169" s="72"/>
-      <c r="B169" s="72"/>
-      <c r="C169" s="72"/>
-      <c r="D169" s="72"/>
-      <c r="E169" s="72"/>
-      <c r="F169" s="72"/>
-      <c r="G169" s="72"/>
-      <c r="H169" s="72"/>
-      <c r="I169" s="72"/>
-      <c r="J169" s="72"/>
+      <c r="A169" s="71"/>
+      <c r="B169" s="71"/>
+      <c r="C169" s="71"/>
+      <c r="D169" s="71"/>
+      <c r="E169" s="71"/>
+      <c r="F169" s="71"/>
+      <c r="G169" s="71"/>
+      <c r="H169" s="71"/>
+      <c r="I169" s="71"/>
+      <c r="J169" s="71"/>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="69"/>
-      <c r="C170" s="70"/>
-      <c r="D170" s="70"/>
-      <c r="E170" s="70"/>
-      <c r="F170" s="70"/>
-      <c r="G170" s="70"/>
-      <c r="H170" s="70"/>
-      <c r="I170" s="70"/>
-      <c r="J170" s="71"/>
+      <c r="B170" s="72"/>
+      <c r="C170" s="69"/>
+      <c r="D170" s="69"/>
+      <c r="E170" s="69"/>
+      <c r="F170" s="69"/>
+      <c r="G170" s="69"/>
+      <c r="H170" s="69"/>
+      <c r="I170" s="69"/>
+      <c r="J170" s="73"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -5483,63 +5551,31 @@
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="70"/>
-      <c r="B177" s="70"/>
-      <c r="C177" s="70"/>
-      <c r="D177" s="70"/>
-      <c r="E177" s="70"/>
-      <c r="F177" s="70"/>
-      <c r="G177" s="70"/>
-      <c r="H177" s="70"/>
-      <c r="I177" s="70"/>
-      <c r="J177" s="70"/>
+      <c r="A177" s="69"/>
+      <c r="B177" s="69"/>
+      <c r="C177" s="69"/>
+      <c r="D177" s="69"/>
+      <c r="E177" s="69"/>
+      <c r="F177" s="69"/>
+      <c r="G177" s="69"/>
+      <c r="H177" s="69"/>
+      <c r="I177" s="69"/>
+      <c r="J177" s="69"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="73"/>
-      <c r="B178" s="73"/>
-      <c r="C178" s="73"/>
-      <c r="D178" s="73"/>
-      <c r="E178" s="73"/>
-      <c r="F178" s="73"/>
-      <c r="G178" s="73"/>
-      <c r="H178" s="73"/>
-      <c r="I178" s="73"/>
-      <c r="J178" s="73"/>
+      <c r="A178" s="70"/>
+      <c r="B178" s="70"/>
+      <c r="C178" s="70"/>
+      <c r="D178" s="70"/>
+      <c r="E178" s="70"/>
+      <c r="F178" s="70"/>
+      <c r="G178" s="70"/>
+      <c r="H178" s="70"/>
+      <c r="I178" s="70"/>
+      <c r="J178" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="B154:J154"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="B162:J162"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="B170:J170"/>
-    <mergeCell ref="B146:J146"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B114:J114"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="B122:J122"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="B130:J130"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="B138:J138"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="B98:J98"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A97:J97"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="B2:J2"/>
@@ -5553,6 +5589,38 @@
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B98:J98"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="B82:J82"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="B146:J146"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="B114:J114"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="B122:J122"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="B130:J130"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="B138:J138"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="B154:J154"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="B162:J162"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="B170:J170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Explosion particle + uren reg
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carloakuma\Desktop\Gamelab1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="66">
   <si>
     <t>Maandag</t>
   </si>
@@ -222,19 +217,13 @@
   </si>
   <si>
     <t>Danial gamejam</t>
-  </si>
-  <si>
-    <t>Chantal Ziek</t>
-  </si>
-  <si>
-    <t>Chantal ZIek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -741,6 +730,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -824,7 +816,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -859,7 +851,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1036,36 +1028,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K118" sqref="K118"/>
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L144" sqref="L144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="6" customWidth="1"/>
-    <col min="3" max="9" width="10.88671875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="42.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="42.42578125" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="12" width="22" style="6" customWidth="1"/>
-    <col min="13" max="13" width="24.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="17" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" style="6" customWidth="1"/>
-    <col min="16" max="16" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1">
       <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
@@ -1104,33 +1096,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="74"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.94855305466237938</v>
+        <v>0.96540880503144655</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>35</v>
@@ -1139,7 +1131,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1174,11 +1166,11 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.84887459807073951</v>
+        <v>0.84905660377358494</v>
       </c>
       <c r="O3" s="54" t="s">
         <v>34</v>
@@ -1187,7 +1179,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1222,11 +1214,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.99035369774919613</v>
+        <v>0.99056603773584906</v>
       </c>
       <c r="O4" s="55" t="s">
         <v>36</v>
@@ -1235,7 +1227,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1270,11 +1262,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.92926045016077174</v>
+        <v>0.9308176100628931</v>
       </c>
       <c r="O5" s="56" t="s">
         <v>37</v>
@@ -1283,7 +1275,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
@@ -1304,11 +1296,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.76848874598070738</v>
+        <v>0.77358490566037741</v>
       </c>
       <c r="O6" s="57" t="s">
         <v>38</v>
@@ -1317,7 +1309,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1352,11 +1344,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.707395498392283</v>
+        <v>0.71383647798742134</v>
       </c>
       <c r="O7" s="58" t="s">
         <v>39</v>
@@ -1365,7 +1357,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1">
       <c r="A8" s="33" t="s">
         <v>11</v>
       </c>
@@ -1406,11 +1398,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.96784565916398713</v>
+        <v>0.96855345911949686</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>40</v>
@@ -1419,35 +1411,35 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="71"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A9" s="72"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="73"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="74"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1473,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -1513,7 +1505,7 @@
       <c r="K12" s="23"/>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1545,7 +1537,7 @@
       <c r="K13" s="23"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -1577,7 +1569,7 @@
       <c r="K14" s="23"/>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="15.75" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1609,7 +1601,7 @@
       <c r="K15" s="23"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="15.75" thickBot="1">
       <c r="A16" s="33" t="s">
         <v>6</v>
       </c>
@@ -1649,35 +1641,35 @@
       <c r="K16" s="23"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="71"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A17" s="72"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="72"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="72"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="73"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="74"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
@@ -1709,7 +1701,7 @@
       <c r="K19" s="23"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" s="4" t="s">
         <v>1</v>
       </c>
@@ -1741,7 +1733,7 @@
       <c r="K20" s="23"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" s="4" t="s">
         <v>2</v>
       </c>
@@ -1773,7 +1765,7 @@
       <c r="K21" s="23"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
@@ -1805,7 +1797,7 @@
       <c r="K22" s="23"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="15.75" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
@@ -1837,7 +1829,7 @@
       <c r="K23" s="23"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1">
       <c r="A24" s="33" t="s">
         <v>6</v>
       </c>
@@ -1877,35 +1869,35 @@
       <c r="K24" s="23"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="71"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A25" s="72"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="72"/>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="73"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="74"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27" s="4" t="s">
         <v>0</v>
       </c>
@@ -1937,7 +1929,7 @@
       <c r="K27" s="23"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28" s="4" t="s">
         <v>1</v>
       </c>
@@ -1969,7 +1961,7 @@
       <c r="K28" s="23"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" s="4" t="s">
         <v>2</v>
       </c>
@@ -2001,7 +1993,7 @@
       <c r="K29" s="23"/>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30" s="4" t="s">
         <v>3</v>
       </c>
@@ -2033,7 +2025,7 @@
       <c r="K30" s="23"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="15.75" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>4</v>
       </c>
@@ -2065,7 +2057,7 @@
       <c r="K31" s="23"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="15.75" thickBot="1">
       <c r="A32" s="33" t="s">
         <v>6</v>
       </c>
@@ -2105,35 +2097,35 @@
       <c r="K32" s="23"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="71"/>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="71"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A33" s="72"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="72"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="73"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="74"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" s="4" t="s">
         <v>0</v>
       </c>
@@ -2165,7 +2157,7 @@
       <c r="K35" s="23"/>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" s="4" t="s">
         <v>1</v>
       </c>
@@ -2197,7 +2189,7 @@
       <c r="K36" s="23"/>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="A37" s="4" t="s">
         <v>2</v>
       </c>
@@ -2231,7 +2223,7 @@
       <c r="K37" s="23"/>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -2263,7 +2255,7 @@
       <c r="K38" s="23"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="15.75" thickBot="1">
       <c r="A39" s="5" t="s">
         <v>4</v>
       </c>
@@ -2295,7 +2287,7 @@
       <c r="K39" s="23"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="15.75" thickBot="1">
       <c r="A40" s="33" t="s">
         <v>6</v>
       </c>
@@ -2335,35 +2327,35 @@
       <c r="K40" s="23"/>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="71"/>
-      <c r="B41" s="71"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="71"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A41" s="72"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="72"/>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="72"/>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="73"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="70"/>
+      <c r="J42" s="74"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12">
       <c r="A43" s="4" t="s">
         <v>0</v>
       </c>
@@ -2397,7 +2389,7 @@
       <c r="K43" s="23"/>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12">
       <c r="A44" s="4" t="s">
         <v>1</v>
       </c>
@@ -2431,7 +2423,7 @@
       <c r="K44" s="23"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12">
       <c r="A45" s="4" t="s">
         <v>2</v>
       </c>
@@ -2463,7 +2455,7 @@
       <c r="K45" s="23"/>
       <c r="L45" s="8"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12">
       <c r="A46" s="4" t="s">
         <v>3</v>
       </c>
@@ -2495,7 +2487,7 @@
       <c r="K46" s="23"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="15.75" thickBot="1">
       <c r="A47" s="5" t="s">
         <v>4</v>
       </c>
@@ -2527,7 +2519,7 @@
       <c r="K47" s="23"/>
       <c r="L47" s="8"/>
     </row>
-    <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" ht="15.75" thickBot="1">
       <c r="A48" s="33" t="s">
         <v>6</v>
       </c>
@@ -2567,35 +2559,35 @@
       <c r="K48" s="23"/>
       <c r="L48" s="8"/>
     </row>
-    <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="71"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="71"/>
-      <c r="D49" s="71"/>
-      <c r="E49" s="71"/>
-      <c r="F49" s="71"/>
-      <c r="G49" s="71"/>
-      <c r="H49" s="71"/>
-      <c r="I49" s="71"/>
-      <c r="J49" s="71"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A49" s="72"/>
+      <c r="B49" s="72"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="72"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="72"/>
+      <c r="H49" s="72"/>
+      <c r="I49" s="72"/>
+      <c r="J49" s="72"/>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="72"/>
-      <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="69"/>
-      <c r="J50" s="73"/>
+      <c r="B50" s="73"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="70"/>
+      <c r="E50" s="70"/>
+      <c r="F50" s="70"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="74"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12">
       <c r="A51" s="4" t="s">
         <v>0</v>
       </c>
@@ -2627,7 +2619,7 @@
       <c r="K51" s="23"/>
       <c r="L51" s="8"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12">
       <c r="A52" s="4" t="s">
         <v>1</v>
       </c>
@@ -2659,7 +2651,7 @@
       <c r="K52" s="23"/>
       <c r="L52" s="8"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12">
       <c r="A53" s="4" t="s">
         <v>2</v>
       </c>
@@ -2691,7 +2683,7 @@
       <c r="K53" s="23"/>
       <c r="L53" s="8"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12">
       <c r="A54" s="4" t="s">
         <v>3</v>
       </c>
@@ -2723,7 +2715,7 @@
       <c r="K54" s="23"/>
       <c r="L54" s="8"/>
     </row>
-    <row r="55" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" ht="15.75" thickBot="1">
       <c r="A55" s="5" t="s">
         <v>4</v>
       </c>
@@ -2755,7 +2747,7 @@
       <c r="K55" s="23"/>
       <c r="L55" s="8"/>
     </row>
-    <row r="56" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" ht="15.75" thickBot="1">
       <c r="A56" s="33" t="s">
         <v>6</v>
       </c>
@@ -2795,35 +2787,35 @@
       <c r="K56" s="23"/>
       <c r="L56" s="8"/>
     </row>
-    <row r="57" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="71"/>
-      <c r="B57" s="71"/>
-      <c r="C57" s="71"/>
-      <c r="D57" s="71"/>
-      <c r="E57" s="71"/>
-      <c r="F57" s="71"/>
-      <c r="G57" s="71"/>
-      <c r="H57" s="71"/>
-      <c r="I57" s="71"/>
-      <c r="J57" s="71"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A57" s="72"/>
+      <c r="B57" s="72"/>
+      <c r="C57" s="72"/>
+      <c r="D57" s="72"/>
+      <c r="E57" s="72"/>
+      <c r="F57" s="72"/>
+      <c r="G57" s="72"/>
+      <c r="H57" s="72"/>
+      <c r="I57" s="72"/>
+      <c r="J57" s="72"/>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="72"/>
-      <c r="C58" s="69"/>
-      <c r="D58" s="69"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="69"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="69"/>
-      <c r="I58" s="69"/>
-      <c r="J58" s="73"/>
+      <c r="B58" s="73"/>
+      <c r="C58" s="70"/>
+      <c r="D58" s="70"/>
+      <c r="E58" s="70"/>
+      <c r="F58" s="70"/>
+      <c r="G58" s="70"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="70"/>
+      <c r="J58" s="74"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12">
       <c r="A59" s="4" t="s">
         <v>0</v>
       </c>
@@ -2855,7 +2847,7 @@
       <c r="K59" s="23"/>
       <c r="L59" s="8"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12">
       <c r="A60" s="4" t="s">
         <v>1</v>
       </c>
@@ -2887,7 +2879,7 @@
       <c r="K60" s="23"/>
       <c r="L60" s="8"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12">
       <c r="A61" s="4" t="s">
         <v>2</v>
       </c>
@@ -2919,7 +2911,7 @@
       <c r="K61" s="23"/>
       <c r="L61" s="8"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12">
       <c r="A62" s="4" t="s">
         <v>3</v>
       </c>
@@ -2953,7 +2945,7 @@
       <c r="K62" s="23"/>
       <c r="L62" s="8"/>
     </row>
-    <row r="63" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" ht="15.75" thickBot="1">
       <c r="A63" s="5" t="s">
         <v>4</v>
       </c>
@@ -2987,7 +2979,7 @@
       <c r="K63" s="23"/>
       <c r="L63" s="8"/>
     </row>
-    <row r="64" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" ht="15.75" thickBot="1">
       <c r="A64" s="33" t="s">
         <v>6</v>
       </c>
@@ -3027,35 +3019,35 @@
       <c r="K64" s="23"/>
       <c r="L64" s="8"/>
     </row>
-    <row r="65" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="71"/>
-      <c r="B65" s="71"/>
-      <c r="C65" s="71"/>
-      <c r="D65" s="71"/>
-      <c r="E65" s="71"/>
-      <c r="F65" s="71"/>
-      <c r="G65" s="71"/>
-      <c r="H65" s="71"/>
-      <c r="I65" s="71"/>
-      <c r="J65" s="71"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A65" s="72"/>
+      <c r="B65" s="72"/>
+      <c r="C65" s="72"/>
+      <c r="D65" s="72"/>
+      <c r="E65" s="72"/>
+      <c r="F65" s="72"/>
+      <c r="G65" s="72"/>
+      <c r="H65" s="72"/>
+      <c r="I65" s="72"/>
+      <c r="J65" s="72"/>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="72"/>
-      <c r="C66" s="69"/>
-      <c r="D66" s="69"/>
-      <c r="E66" s="69"/>
-      <c r="F66" s="69"/>
-      <c r="G66" s="69"/>
-      <c r="H66" s="69"/>
-      <c r="I66" s="69"/>
-      <c r="J66" s="73"/>
+      <c r="B66" s="73"/>
+      <c r="C66" s="70"/>
+      <c r="D66" s="70"/>
+      <c r="E66" s="70"/>
+      <c r="F66" s="70"/>
+      <c r="G66" s="70"/>
+      <c r="H66" s="70"/>
+      <c r="I66" s="70"/>
+      <c r="J66" s="74"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12">
       <c r="A67" s="19" t="s">
         <v>0</v>
       </c>
@@ -3073,7 +3065,7 @@
       <c r="K67" s="23"/>
       <c r="L67" s="8"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12">
       <c r="A68" s="19" t="s">
         <v>1</v>
       </c>
@@ -3091,7 +3083,7 @@
       <c r="K68" s="23"/>
       <c r="L68" s="43"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12">
       <c r="A69" s="19" t="s">
         <v>2</v>
       </c>
@@ -3109,7 +3101,7 @@
       <c r="K69" s="23"/>
       <c r="L69" s="8"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12">
       <c r="A70" s="19" t="s">
         <v>3</v>
       </c>
@@ -3127,7 +3119,7 @@
       <c r="K70" s="23"/>
       <c r="L70" s="8"/>
     </row>
-    <row r="71" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" ht="15.75" thickBot="1">
       <c r="A71" s="41" t="s">
         <v>4</v>
       </c>
@@ -3145,7 +3137,7 @@
       <c r="K71" s="23"/>
       <c r="L71" s="8"/>
     </row>
-    <row r="72" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" ht="15.75" thickBot="1">
       <c r="A72" s="33" t="s">
         <v>6</v>
       </c>
@@ -3185,35 +3177,35 @@
       <c r="K72" s="23"/>
       <c r="L72" s="8"/>
     </row>
-    <row r="73" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="71"/>
-      <c r="B73" s="71"/>
-      <c r="C73" s="71"/>
-      <c r="D73" s="71"/>
-      <c r="E73" s="71"/>
-      <c r="F73" s="71"/>
-      <c r="G73" s="71"/>
-      <c r="H73" s="71"/>
-      <c r="I73" s="71"/>
-      <c r="J73" s="71"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A73" s="72"/>
+      <c r="B73" s="72"/>
+      <c r="C73" s="72"/>
+      <c r="D73" s="72"/>
+      <c r="E73" s="72"/>
+      <c r="F73" s="72"/>
+      <c r="G73" s="72"/>
+      <c r="H73" s="72"/>
+      <c r="I73" s="72"/>
+      <c r="J73" s="72"/>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="72"/>
-      <c r="C74" s="69"/>
-      <c r="D74" s="69"/>
-      <c r="E74" s="69"/>
-      <c r="F74" s="69"/>
-      <c r="G74" s="69"/>
-      <c r="H74" s="69"/>
-      <c r="I74" s="69"/>
-      <c r="J74" s="73"/>
+      <c r="B74" s="73"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="70"/>
+      <c r="E74" s="70"/>
+      <c r="F74" s="70"/>
+      <c r="G74" s="70"/>
+      <c r="H74" s="70"/>
+      <c r="I74" s="70"/>
+      <c r="J74" s="74"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12">
       <c r="A75" s="19" t="s">
         <v>0</v>
       </c>
@@ -3231,7 +3223,7 @@
       <c r="K75" s="23"/>
       <c r="L75" s="8"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12">
       <c r="A76" s="4" t="s">
         <v>1</v>
       </c>
@@ -3263,7 +3255,7 @@
       <c r="K76" s="23"/>
       <c r="L76" s="8"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12">
       <c r="A77" s="4" t="s">
         <v>2</v>
       </c>
@@ -3295,7 +3287,7 @@
       <c r="K77" s="23"/>
       <c r="L77" s="8"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12">
       <c r="A78" s="4" t="s">
         <v>3</v>
       </c>
@@ -3327,7 +3319,7 @@
       <c r="K78" s="23"/>
       <c r="L78" s="8"/>
     </row>
-    <row r="79" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" ht="15.75" thickBot="1">
       <c r="A79" s="5" t="s">
         <v>4</v>
       </c>
@@ -3359,7 +3351,7 @@
       <c r="K79" s="23"/>
       <c r="L79" s="8"/>
     </row>
-    <row r="80" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" ht="15.75" thickBot="1">
       <c r="A80" s="33" t="s">
         <v>6</v>
       </c>
@@ -3399,35 +3391,35 @@
       <c r="K80" s="23"/>
       <c r="L80" s="8"/>
     </row>
-    <row r="81" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="71"/>
-      <c r="B81" s="71"/>
-      <c r="C81" s="71"/>
-      <c r="D81" s="71"/>
-      <c r="E81" s="71"/>
-      <c r="F81" s="71"/>
-      <c r="G81" s="71"/>
-      <c r="H81" s="71"/>
-      <c r="I81" s="71"/>
-      <c r="J81" s="71"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A81" s="72"/>
+      <c r="B81" s="72"/>
+      <c r="C81" s="72"/>
+      <c r="D81" s="72"/>
+      <c r="E81" s="72"/>
+      <c r="F81" s="72"/>
+      <c r="G81" s="72"/>
+      <c r="H81" s="72"/>
+      <c r="I81" s="72"/>
+      <c r="J81" s="72"/>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="72"/>
-      <c r="C82" s="69"/>
-      <c r="D82" s="69"/>
-      <c r="E82" s="69"/>
-      <c r="F82" s="69"/>
-      <c r="G82" s="69"/>
-      <c r="H82" s="69"/>
-      <c r="I82" s="69"/>
-      <c r="J82" s="73"/>
+      <c r="B82" s="73"/>
+      <c r="C82" s="70"/>
+      <c r="D82" s="70"/>
+      <c r="E82" s="70"/>
+      <c r="F82" s="70"/>
+      <c r="G82" s="70"/>
+      <c r="H82" s="70"/>
+      <c r="I82" s="70"/>
+      <c r="J82" s="74"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12">
       <c r="A83" s="4" t="s">
         <v>0</v>
       </c>
@@ -3459,7 +3451,7 @@
       <c r="K83" s="23"/>
       <c r="L83" s="8"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12">
       <c r="A84" s="4" t="s">
         <v>1</v>
       </c>
@@ -3491,7 +3483,7 @@
       <c r="K84" s="23"/>
       <c r="L84" s="8"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12">
       <c r="A85" s="4" t="s">
         <v>2</v>
       </c>
@@ -3525,7 +3517,7 @@
       <c r="K85" s="23"/>
       <c r="L85" s="8"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12">
       <c r="A86" s="4" t="s">
         <v>3</v>
       </c>
@@ -3557,7 +3549,7 @@
       <c r="K86" s="23"/>
       <c r="L86" s="8"/>
     </row>
-    <row r="87" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" ht="15.75" thickBot="1">
       <c r="A87" s="5" t="s">
         <v>4</v>
       </c>
@@ -3589,7 +3581,7 @@
       <c r="K87" s="23"/>
       <c r="L87" s="8"/>
     </row>
-    <row r="88" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" ht="15.75" thickBot="1">
       <c r="A88" s="33" t="s">
         <v>6</v>
       </c>
@@ -3629,35 +3621,35 @@
       <c r="K88" s="23"/>
       <c r="L88" s="8"/>
     </row>
-    <row r="89" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="71"/>
-      <c r="B89" s="71"/>
-      <c r="C89" s="71"/>
-      <c r="D89" s="71"/>
-      <c r="E89" s="71"/>
-      <c r="F89" s="71"/>
-      <c r="G89" s="71"/>
-      <c r="H89" s="71"/>
-      <c r="I89" s="71"/>
-      <c r="J89" s="71"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A89" s="72"/>
+      <c r="B89" s="72"/>
+      <c r="C89" s="72"/>
+      <c r="D89" s="72"/>
+      <c r="E89" s="72"/>
+      <c r="F89" s="72"/>
+      <c r="G89" s="72"/>
+      <c r="H89" s="72"/>
+      <c r="I89" s="72"/>
+      <c r="J89" s="72"/>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="72"/>
-      <c r="C90" s="69"/>
-      <c r="D90" s="69"/>
-      <c r="E90" s="69"/>
-      <c r="F90" s="69"/>
-      <c r="G90" s="69"/>
-      <c r="H90" s="69"/>
-      <c r="I90" s="69"/>
-      <c r="J90" s="73"/>
+      <c r="B90" s="73"/>
+      <c r="C90" s="70"/>
+      <c r="D90" s="70"/>
+      <c r="E90" s="70"/>
+      <c r="F90" s="70"/>
+      <c r="G90" s="70"/>
+      <c r="H90" s="70"/>
+      <c r="I90" s="70"/>
+      <c r="J90" s="74"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12">
       <c r="A91" s="4" t="s">
         <v>0</v>
       </c>
@@ -3689,7 +3681,7 @@
       <c r="K91" s="23"/>
       <c r="L91" s="8"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12">
       <c r="A92" s="4" t="s">
         <v>1</v>
       </c>
@@ -3721,7 +3713,7 @@
       <c r="K92" s="23"/>
       <c r="L92" s="8"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12">
       <c r="A93" s="4" t="s">
         <v>2</v>
       </c>
@@ -3753,7 +3745,7 @@
       <c r="K93" s="23"/>
       <c r="L93" s="8"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12">
       <c r="A94" s="4" t="s">
         <v>3</v>
       </c>
@@ -3785,7 +3777,7 @@
       <c r="K94" s="23"/>
       <c r="L94" s="8"/>
     </row>
-    <row r="95" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" ht="15.75" thickBot="1">
       <c r="A95" s="5" t="s">
         <v>4</v>
       </c>
@@ -3817,7 +3809,7 @@
       <c r="K95" s="23"/>
       <c r="L95" s="8"/>
     </row>
-    <row r="96" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" ht="15.75" thickBot="1">
       <c r="A96" s="33" t="s">
         <v>6</v>
       </c>
@@ -3857,35 +3849,35 @@
       <c r="K96" s="23"/>
       <c r="L96" s="8"/>
     </row>
-    <row r="97" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="71"/>
-      <c r="B97" s="71"/>
-      <c r="C97" s="71"/>
-      <c r="D97" s="71"/>
-      <c r="E97" s="71"/>
-      <c r="F97" s="71"/>
-      <c r="G97" s="71"/>
-      <c r="H97" s="71"/>
-      <c r="I97" s="71"/>
-      <c r="J97" s="71"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A97" s="72"/>
+      <c r="B97" s="72"/>
+      <c r="C97" s="72"/>
+      <c r="D97" s="72"/>
+      <c r="E97" s="72"/>
+      <c r="F97" s="72"/>
+      <c r="G97" s="72"/>
+      <c r="H97" s="72"/>
+      <c r="I97" s="72"/>
+      <c r="J97" s="72"/>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="72"/>
-      <c r="C98" s="69"/>
-      <c r="D98" s="69"/>
-      <c r="E98" s="69"/>
-      <c r="F98" s="69"/>
-      <c r="G98" s="69"/>
-      <c r="H98" s="69"/>
-      <c r="I98" s="69"/>
-      <c r="J98" s="73"/>
+      <c r="B98" s="73"/>
+      <c r="C98" s="70"/>
+      <c r="D98" s="70"/>
+      <c r="E98" s="70"/>
+      <c r="F98" s="70"/>
+      <c r="G98" s="70"/>
+      <c r="H98" s="70"/>
+      <c r="I98" s="70"/>
+      <c r="J98" s="74"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12">
       <c r="A99" s="4" t="s">
         <v>0</v>
       </c>
@@ -3919,7 +3911,7 @@
       <c r="K99" s="23"/>
       <c r="L99" s="8"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12">
       <c r="A100" s="4" t="s">
         <v>1</v>
       </c>
@@ -3951,7 +3943,7 @@
       <c r="K100" s="23"/>
       <c r="L100" s="8"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12">
       <c r="A101" s="4" t="s">
         <v>2</v>
       </c>
@@ -3983,7 +3975,7 @@
       <c r="K101" s="23"/>
       <c r="L101" s="8"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12">
       <c r="A102" s="4" t="s">
         <v>3</v>
       </c>
@@ -4015,7 +4007,7 @@
       <c r="K102" s="23"/>
       <c r="L102" s="8"/>
     </row>
-    <row r="103" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" ht="15.75" thickBot="1">
       <c r="A103" s="5" t="s">
         <v>4</v>
       </c>
@@ -4047,7 +4039,7 @@
       <c r="K103" s="23"/>
       <c r="L103" s="8"/>
     </row>
-    <row r="104" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" ht="15.75" thickBot="1">
       <c r="A104" s="33" t="s">
         <v>6</v>
       </c>
@@ -4087,35 +4079,35 @@
       <c r="K104" s="23"/>
       <c r="L104" s="8"/>
     </row>
-    <row r="105" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="71"/>
-      <c r="B105" s="71"/>
-      <c r="C105" s="71"/>
-      <c r="D105" s="71"/>
-      <c r="E105" s="71"/>
-      <c r="F105" s="71"/>
-      <c r="G105" s="71"/>
-      <c r="H105" s="71"/>
-      <c r="I105" s="71"/>
-      <c r="J105" s="71"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A105" s="72"/>
+      <c r="B105" s="72"/>
+      <c r="C105" s="72"/>
+      <c r="D105" s="72"/>
+      <c r="E105" s="72"/>
+      <c r="F105" s="72"/>
+      <c r="G105" s="72"/>
+      <c r="H105" s="72"/>
+      <c r="I105" s="72"/>
+      <c r="J105" s="72"/>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="72"/>
-      <c r="C106" s="69"/>
-      <c r="D106" s="69"/>
-      <c r="E106" s="69"/>
-      <c r="F106" s="69"/>
-      <c r="G106" s="69"/>
-      <c r="H106" s="69"/>
-      <c r="I106" s="69"/>
-      <c r="J106" s="73"/>
+      <c r="B106" s="73"/>
+      <c r="C106" s="70"/>
+      <c r="D106" s="70"/>
+      <c r="E106" s="70"/>
+      <c r="F106" s="70"/>
+      <c r="G106" s="70"/>
+      <c r="H106" s="70"/>
+      <c r="I106" s="70"/>
+      <c r="J106" s="74"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12">
       <c r="A107" s="4" t="s">
         <v>0</v>
       </c>
@@ -4147,7 +4139,7 @@
       <c r="K107" s="23"/>
       <c r="L107" s="8"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12">
       <c r="A108" s="4" t="s">
         <v>1</v>
       </c>
@@ -4181,7 +4173,7 @@
       <c r="K108" s="23"/>
       <c r="L108" s="8"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12">
       <c r="A109" s="4" t="s">
         <v>2</v>
       </c>
@@ -4213,7 +4205,7 @@
       <c r="K109" s="23"/>
       <c r="L109" s="8"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12">
       <c r="A110" s="4" t="s">
         <v>3</v>
       </c>
@@ -4245,7 +4237,7 @@
       <c r="K110" s="23"/>
       <c r="L110" s="8"/>
     </row>
-    <row r="111" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" ht="15.75" thickBot="1">
       <c r="A111" s="5" t="s">
         <v>4</v>
       </c>
@@ -4277,7 +4269,7 @@
       <c r="K111" s="23"/>
       <c r="L111" s="8"/>
     </row>
-    <row r="112" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" ht="15.75" thickBot="1">
       <c r="A112" s="33" t="s">
         <v>6</v>
       </c>
@@ -4317,35 +4309,35 @@
       <c r="K112" s="23"/>
       <c r="L112" s="8"/>
     </row>
-    <row r="113" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="71"/>
-      <c r="B113" s="71"/>
-      <c r="C113" s="71"/>
-      <c r="D113" s="71"/>
-      <c r="E113" s="71"/>
-      <c r="F113" s="71"/>
-      <c r="G113" s="71"/>
-      <c r="H113" s="71"/>
-      <c r="I113" s="71"/>
-      <c r="J113" s="71"/>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A113" s="72"/>
+      <c r="B113" s="72"/>
+      <c r="C113" s="72"/>
+      <c r="D113" s="72"/>
+      <c r="E113" s="72"/>
+      <c r="F113" s="72"/>
+      <c r="G113" s="72"/>
+      <c r="H113" s="72"/>
+      <c r="I113" s="72"/>
+      <c r="J113" s="72"/>
+    </row>
+    <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="72"/>
-      <c r="C114" s="69"/>
-      <c r="D114" s="69"/>
-      <c r="E114" s="69"/>
-      <c r="F114" s="69"/>
-      <c r="G114" s="69"/>
-      <c r="H114" s="69"/>
-      <c r="I114" s="69"/>
-      <c r="J114" s="73"/>
+      <c r="B114" s="73"/>
+      <c r="C114" s="70"/>
+      <c r="D114" s="70"/>
+      <c r="E114" s="70"/>
+      <c r="F114" s="70"/>
+      <c r="G114" s="70"/>
+      <c r="H114" s="70"/>
+      <c r="I114" s="70"/>
+      <c r="J114" s="74"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12">
       <c r="A115" s="4" t="s">
         <v>0</v>
       </c>
@@ -4377,7 +4369,7 @@
       <c r="K115" s="23"/>
       <c r="L115" s="8"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12">
       <c r="A116" s="4" t="s">
         <v>1</v>
       </c>
@@ -4409,7 +4401,7 @@
       <c r="K116" s="23"/>
       <c r="L116" s="8"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12">
       <c r="A117" s="4" t="s">
         <v>2</v>
       </c>
@@ -4441,7 +4433,7 @@
       <c r="K117" s="23"/>
       <c r="L117" s="8"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12">
       <c r="A118" s="4" t="s">
         <v>3</v>
       </c>
@@ -4473,7 +4465,7 @@
       <c r="K118" s="23"/>
       <c r="L118" s="8"/>
     </row>
-    <row r="119" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" ht="15.75" thickBot="1">
       <c r="A119" s="5" t="s">
         <v>4</v>
       </c>
@@ -4505,7 +4497,7 @@
       <c r="K119" s="23"/>
       <c r="L119" s="8"/>
     </row>
-    <row r="120" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" ht="15.75" thickBot="1">
       <c r="A120" s="33" t="s">
         <v>6</v>
       </c>
@@ -4545,35 +4537,35 @@
       <c r="K120" s="23"/>
       <c r="L120" s="8"/>
     </row>
-    <row r="121" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="71"/>
-      <c r="B121" s="71"/>
-      <c r="C121" s="71"/>
-      <c r="D121" s="71"/>
-      <c r="E121" s="71"/>
-      <c r="F121" s="71"/>
-      <c r="G121" s="71"/>
-      <c r="H121" s="71"/>
-      <c r="I121" s="71"/>
-      <c r="J121" s="71"/>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A121" s="72"/>
+      <c r="B121" s="72"/>
+      <c r="C121" s="72"/>
+      <c r="D121" s="72"/>
+      <c r="E121" s="72"/>
+      <c r="F121" s="72"/>
+      <c r="G121" s="72"/>
+      <c r="H121" s="72"/>
+      <c r="I121" s="72"/>
+      <c r="J121" s="72"/>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="72"/>
-      <c r="C122" s="69"/>
-      <c r="D122" s="69"/>
-      <c r="E122" s="69"/>
-      <c r="F122" s="69"/>
-      <c r="G122" s="69"/>
-      <c r="H122" s="69"/>
-      <c r="I122" s="69"/>
-      <c r="J122" s="73"/>
+      <c r="B122" s="73"/>
+      <c r="C122" s="70"/>
+      <c r="D122" s="70"/>
+      <c r="E122" s="70"/>
+      <c r="F122" s="70"/>
+      <c r="G122" s="70"/>
+      <c r="H122" s="70"/>
+      <c r="I122" s="70"/>
+      <c r="J122" s="74"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12">
       <c r="A123" s="4" t="s">
         <v>0</v>
       </c>
@@ -4605,7 +4597,7 @@
       <c r="K123" s="23"/>
       <c r="L123" s="8"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12">
       <c r="A124" s="4" t="s">
         <v>1</v>
       </c>
@@ -4637,7 +4629,7 @@
       <c r="K124" s="23"/>
       <c r="L124" s="8"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12">
       <c r="A125" s="19" t="s">
         <v>2</v>
       </c>
@@ -4655,7 +4647,7 @@
       <c r="K125" s="23"/>
       <c r="L125" s="8"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12">
       <c r="A126" s="4" t="s">
         <v>3</v>
       </c>
@@ -4687,7 +4679,7 @@
       <c r="K126" s="23"/>
       <c r="L126" s="8"/>
     </row>
-    <row r="127" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" ht="15.75" thickBot="1">
       <c r="A127" s="5" t="s">
         <v>4</v>
       </c>
@@ -4721,7 +4713,7 @@
       <c r="K127" s="23"/>
       <c r="L127" s="8"/>
     </row>
-    <row r="128" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" ht="15.75" thickBot="1">
       <c r="A128" s="33" t="s">
         <v>6</v>
       </c>
@@ -4761,35 +4753,35 @@
       <c r="K128" s="23"/>
       <c r="L128" s="8"/>
     </row>
-    <row r="129" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="71"/>
-      <c r="B129" s="71"/>
-      <c r="C129" s="71"/>
-      <c r="D129" s="71"/>
-      <c r="E129" s="71"/>
-      <c r="F129" s="71"/>
-      <c r="G129" s="71"/>
-      <c r="H129" s="71"/>
-      <c r="I129" s="71"/>
-      <c r="J129" s="71"/>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A129" s="72"/>
+      <c r="B129" s="72"/>
+      <c r="C129" s="72"/>
+      <c r="D129" s="72"/>
+      <c r="E129" s="72"/>
+      <c r="F129" s="72"/>
+      <c r="G129" s="72"/>
+      <c r="H129" s="72"/>
+      <c r="I129" s="72"/>
+      <c r="J129" s="72"/>
+    </row>
+    <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="72"/>
-      <c r="C130" s="69"/>
-      <c r="D130" s="69"/>
-      <c r="E130" s="69"/>
-      <c r="F130" s="69"/>
-      <c r="G130" s="69"/>
-      <c r="H130" s="69"/>
-      <c r="I130" s="69"/>
-      <c r="J130" s="73"/>
+      <c r="B130" s="73"/>
+      <c r="C130" s="70"/>
+      <c r="D130" s="70"/>
+      <c r="E130" s="70"/>
+      <c r="F130" s="70"/>
+      <c r="G130" s="70"/>
+      <c r="H130" s="70"/>
+      <c r="I130" s="70"/>
+      <c r="J130" s="74"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12">
       <c r="A131" s="4" t="s">
         <v>0</v>
       </c>
@@ -4821,41 +4813,39 @@
       <c r="K131" s="23"/>
       <c r="L131" s="8"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12">
       <c r="A132" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B132" s="8">
         <v>5</v>
       </c>
-      <c r="C132" s="28">
-        <v>0</v>
-      </c>
-      <c r="D132" s="6">
-        <v>5</v>
-      </c>
-      <c r="E132" s="6">
-        <v>5</v>
-      </c>
-      <c r="F132" s="6">
-        <v>5</v>
-      </c>
-      <c r="G132" s="6">
+      <c r="C132" s="69">
+        <v>5</v>
+      </c>
+      <c r="D132" s="30">
+        <v>4</v>
+      </c>
+      <c r="E132" s="69">
+        <v>5</v>
+      </c>
+      <c r="F132" s="69">
+        <v>5</v>
+      </c>
+      <c r="G132" s="28">
         <v>0</v>
       </c>
       <c r="H132" s="67">
         <v>5</v>
       </c>
-      <c r="I132" s="6">
-        <v>5</v>
-      </c>
-      <c r="J132" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="I132" s="69">
+        <v>5</v>
+      </c>
+      <c r="J132" s="1"/>
       <c r="K132" s="23"/>
       <c r="L132" s="8"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12">
       <c r="A133" s="4" t="s">
         <v>2</v>
       </c>
@@ -4868,28 +4858,26 @@
       <c r="D133" s="6">
         <v>3</v>
       </c>
-      <c r="E133" s="6">
+      <c r="E133" s="30">
         <v>2</v>
       </c>
       <c r="F133" s="6">
         <v>3</v>
       </c>
-      <c r="G133" s="6">
+      <c r="G133" s="30">
         <v>2</v>
       </c>
       <c r="H133" s="67">
         <v>3</v>
       </c>
-      <c r="I133" s="6">
-        <v>0</v>
-      </c>
-      <c r="J133" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="I133" s="28">
+        <v>0</v>
+      </c>
+      <c r="J133" s="1"/>
       <c r="K133" s="23"/>
       <c r="L133" s="8"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12">
       <c r="A134" s="4" t="s">
         <v>3</v>
       </c>
@@ -4917,13 +4905,11 @@
       <c r="I134" s="6">
         <v>2</v>
       </c>
-      <c r="J134" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="J134" s="1"/>
       <c r="K134" s="23"/>
       <c r="L134" s="8"/>
     </row>
-    <row r="135" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" ht="15.75" thickBot="1">
       <c r="A135" s="5" t="s">
         <v>4</v>
       </c>
@@ -4951,13 +4937,11 @@
       <c r="I135" s="7">
         <v>4</v>
       </c>
-      <c r="J135" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="J135" s="2"/>
       <c r="K135" s="23"/>
       <c r="L135" s="8"/>
     </row>
-    <row r="136" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" ht="15.75" thickBot="1">
       <c r="A136" s="33" t="s">
         <v>6</v>
       </c>
@@ -4967,11 +4951,11 @@
       </c>
       <c r="C136" s="35">
         <f t="shared" ref="C136:I136" si="16">SUM(C131:C135)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D136" s="35">
         <f t="shared" si="16"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E136" s="35">
         <f t="shared" si="16"/>
@@ -4997,35 +4981,35 @@
       <c r="K136" s="23"/>
       <c r="L136" s="8"/>
     </row>
-    <row r="137" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="71"/>
-      <c r="B137" s="71"/>
-      <c r="C137" s="71"/>
-      <c r="D137" s="71"/>
-      <c r="E137" s="71"/>
-      <c r="F137" s="71"/>
-      <c r="G137" s="71"/>
-      <c r="H137" s="71"/>
-      <c r="I137" s="71"/>
-      <c r="J137" s="71"/>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A137" s="72"/>
+      <c r="B137" s="72"/>
+      <c r="C137" s="72"/>
+      <c r="D137" s="72"/>
+      <c r="E137" s="72"/>
+      <c r="F137" s="72"/>
+      <c r="G137" s="72"/>
+      <c r="H137" s="72"/>
+      <c r="I137" s="72"/>
+      <c r="J137" s="72"/>
+    </row>
+    <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="72"/>
-      <c r="C138" s="69"/>
-      <c r="D138" s="69"/>
-      <c r="E138" s="69"/>
-      <c r="F138" s="69"/>
-      <c r="G138" s="69"/>
-      <c r="H138" s="69"/>
-      <c r="I138" s="69"/>
-      <c r="J138" s="73"/>
+      <c r="B138" s="73"/>
+      <c r="C138" s="70"/>
+      <c r="D138" s="70"/>
+      <c r="E138" s="70"/>
+      <c r="F138" s="70"/>
+      <c r="G138" s="70"/>
+      <c r="H138" s="70"/>
+      <c r="I138" s="70"/>
+      <c r="J138" s="74"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12">
       <c r="A139" s="19" t="s">
         <v>0</v>
       </c>
@@ -5043,7 +5027,7 @@
       <c r="K139" s="23"/>
       <c r="L139" s="8"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12">
       <c r="A140" s="19" t="s">
         <v>1</v>
       </c>
@@ -5061,7 +5045,7 @@
       <c r="K140" s="23"/>
       <c r="L140" s="8"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12">
       <c r="A141" s="19" t="s">
         <v>2</v>
       </c>
@@ -5077,11 +5061,9 @@
         <v>51</v>
       </c>
       <c r="K141" s="23"/>
-      <c r="L141" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L141" s="8"/>
+    </row>
+    <row r="142" spans="1:12">
       <c r="A142" s="19" t="s">
         <v>3</v>
       </c>
@@ -5099,7 +5081,7 @@
       <c r="K142" s="23"/>
       <c r="L142" s="8"/>
     </row>
-    <row r="143" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" ht="15.75" thickBot="1">
       <c r="A143" s="41" t="s">
         <v>4</v>
       </c>
@@ -5117,7 +5099,7 @@
       <c r="K143" s="23"/>
       <c r="L143" s="8"/>
     </row>
-    <row r="144" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" ht="15.75" thickBot="1">
       <c r="A144" s="33" t="s">
         <v>6</v>
       </c>
@@ -5157,55 +5139,99 @@
       <c r="K144" s="23"/>
       <c r="L144" s="8"/>
     </row>
-    <row r="145" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="71"/>
-      <c r="B145" s="71"/>
-      <c r="C145" s="71"/>
-      <c r="D145" s="71"/>
-      <c r="E145" s="71"/>
-      <c r="F145" s="71"/>
-      <c r="G145" s="71"/>
-      <c r="H145" s="71"/>
-      <c r="I145" s="71"/>
-      <c r="J145" s="71"/>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A145" s="72"/>
+      <c r="B145" s="72"/>
+      <c r="C145" s="72"/>
+      <c r="D145" s="72"/>
+      <c r="E145" s="72"/>
+      <c r="F145" s="72"/>
+      <c r="G145" s="72"/>
+      <c r="H145" s="72"/>
+      <c r="I145" s="72"/>
+      <c r="J145" s="72"/>
+    </row>
+    <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="72"/>
-      <c r="C146" s="69"/>
-      <c r="D146" s="69"/>
-      <c r="E146" s="69"/>
-      <c r="F146" s="69"/>
-      <c r="G146" s="69"/>
-      <c r="H146" s="69"/>
-      <c r="I146" s="69"/>
-      <c r="J146" s="73"/>
+      <c r="B146" s="73"/>
+      <c r="C146" s="70"/>
+      <c r="D146" s="70"/>
+      <c r="E146" s="70"/>
+      <c r="F146" s="70"/>
+      <c r="G146" s="70"/>
+      <c r="H146" s="70"/>
+      <c r="I146" s="70"/>
+      <c r="J146" s="74"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12">
       <c r="A147" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B147" s="8"/>
-      <c r="H147" s="67"/>
+      <c r="B147" s="8">
+        <v>2</v>
+      </c>
+      <c r="C147" s="6">
+        <v>2</v>
+      </c>
+      <c r="D147" s="6">
+        <v>2</v>
+      </c>
+      <c r="E147" s="6">
+        <v>2</v>
+      </c>
+      <c r="F147" s="6">
+        <v>2</v>
+      </c>
+      <c r="G147" s="6">
+        <v>2</v>
+      </c>
+      <c r="H147" s="67">
+        <v>2</v>
+      </c>
+      <c r="I147" s="6">
+        <v>2</v>
+      </c>
       <c r="J147" s="1"/>
       <c r="K147" s="23"/>
       <c r="L147" s="8"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12">
       <c r="A148" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B148" s="8"/>
-      <c r="H148" s="67"/>
+      <c r="B148" s="8">
+        <v>5</v>
+      </c>
+      <c r="C148" s="6">
+        <v>5</v>
+      </c>
+      <c r="D148" s="6">
+        <v>5</v>
+      </c>
+      <c r="E148" s="6">
+        <v>5</v>
+      </c>
+      <c r="F148" s="6">
+        <v>5</v>
+      </c>
+      <c r="G148" s="6">
+        <v>5</v>
+      </c>
+      <c r="H148" s="67">
+        <v>5</v>
+      </c>
+      <c r="I148" s="6">
+        <v>5</v>
+      </c>
       <c r="J148" s="1"/>
       <c r="K148" s="23"/>
       <c r="L148" s="8"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12">
       <c r="A149" s="4" t="s">
         <v>2</v>
       </c>
@@ -5215,7 +5241,7 @@
       <c r="K149" s="23"/>
       <c r="L149" s="8"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12">
       <c r="A150" s="4" t="s">
         <v>3</v>
       </c>
@@ -5225,7 +5251,7 @@
       <c r="K150" s="23"/>
       <c r="L150" s="8"/>
     </row>
-    <row r="151" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" ht="15.75" thickBot="1">
       <c r="A151" s="5" t="s">
         <v>4</v>
       </c>
@@ -5241,75 +5267,75 @@
       <c r="K151" s="23"/>
       <c r="L151" s="8"/>
     </row>
-    <row r="152" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" ht="15.75" thickBot="1">
       <c r="A152" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B152" s="34">
         <f>B147+B148+B149+B150+B151</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C152" s="35">
         <f t="shared" ref="C152:I152" si="18">SUM(C147:C151)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D152" s="35">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E152" s="35">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F152" s="35">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G152" s="35">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H152" s="35">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I152" s="35">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J152" s="36"/>
       <c r="K152" s="23"/>
       <c r="L152" s="8"/>
     </row>
-    <row r="153" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="71"/>
-      <c r="B153" s="71"/>
-      <c r="C153" s="71"/>
-      <c r="D153" s="71"/>
-      <c r="E153" s="71"/>
-      <c r="F153" s="71"/>
-      <c r="G153" s="71"/>
-      <c r="H153" s="71"/>
-      <c r="I153" s="71"/>
-      <c r="J153" s="71"/>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A153" s="72"/>
+      <c r="B153" s="72"/>
+      <c r="C153" s="72"/>
+      <c r="D153" s="72"/>
+      <c r="E153" s="72"/>
+      <c r="F153" s="72"/>
+      <c r="G153" s="72"/>
+      <c r="H153" s="72"/>
+      <c r="I153" s="72"/>
+      <c r="J153" s="72"/>
+    </row>
+    <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="72"/>
-      <c r="C154" s="69"/>
-      <c r="D154" s="69"/>
-      <c r="E154" s="69"/>
-      <c r="F154" s="69"/>
-      <c r="G154" s="69"/>
-      <c r="H154" s="69"/>
-      <c r="I154" s="69"/>
-      <c r="J154" s="73"/>
+      <c r="B154" s="73"/>
+      <c r="C154" s="70"/>
+      <c r="D154" s="70"/>
+      <c r="E154" s="70"/>
+      <c r="F154" s="70"/>
+      <c r="G154" s="70"/>
+      <c r="H154" s="70"/>
+      <c r="I154" s="70"/>
+      <c r="J154" s="74"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12">
       <c r="A155" s="4" t="s">
         <v>0</v>
       </c>
@@ -5319,7 +5345,7 @@
       <c r="K155" s="23"/>
       <c r="L155" s="8"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12">
       <c r="A156" s="4" t="s">
         <v>1</v>
       </c>
@@ -5329,7 +5355,7 @@
       <c r="K156" s="23"/>
       <c r="L156" s="8"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12">
       <c r="A157" s="4" t="s">
         <v>2</v>
       </c>
@@ -5339,7 +5365,7 @@
       <c r="K157" s="23"/>
       <c r="L157" s="8"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12">
       <c r="A158" s="4" t="s">
         <v>3</v>
       </c>
@@ -5349,7 +5375,7 @@
       <c r="K158" s="23"/>
       <c r="L158" s="8"/>
     </row>
-    <row r="159" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" ht="15.75" thickBot="1">
       <c r="A159" s="5" t="s">
         <v>4</v>
       </c>
@@ -5365,7 +5391,7 @@
       <c r="K159" s="23"/>
       <c r="L159" s="8"/>
     </row>
-    <row r="160" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" ht="15.75" thickBot="1">
       <c r="A160" s="33" t="s">
         <v>6</v>
       </c>
@@ -5405,35 +5431,35 @@
       <c r="K160" s="23"/>
       <c r="L160" s="8"/>
     </row>
-    <row r="161" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="71"/>
-      <c r="B161" s="71"/>
-      <c r="C161" s="71"/>
-      <c r="D161" s="71"/>
-      <c r="E161" s="71"/>
-      <c r="F161" s="71"/>
-      <c r="G161" s="71"/>
-      <c r="H161" s="71"/>
-      <c r="I161" s="71"/>
-      <c r="J161" s="71"/>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A161" s="72"/>
+      <c r="B161" s="72"/>
+      <c r="C161" s="72"/>
+      <c r="D161" s="72"/>
+      <c r="E161" s="72"/>
+      <c r="F161" s="72"/>
+      <c r="G161" s="72"/>
+      <c r="H161" s="72"/>
+      <c r="I161" s="72"/>
+      <c r="J161" s="72"/>
+    </row>
+    <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="72"/>
-      <c r="C162" s="69"/>
-      <c r="D162" s="69"/>
-      <c r="E162" s="69"/>
-      <c r="F162" s="69"/>
-      <c r="G162" s="69"/>
-      <c r="H162" s="69"/>
-      <c r="I162" s="69"/>
-      <c r="J162" s="73"/>
+      <c r="B162" s="73"/>
+      <c r="C162" s="70"/>
+      <c r="D162" s="70"/>
+      <c r="E162" s="70"/>
+      <c r="F162" s="70"/>
+      <c r="G162" s="70"/>
+      <c r="H162" s="70"/>
+      <c r="I162" s="70"/>
+      <c r="J162" s="74"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12">
       <c r="A163" s="4" t="s">
         <v>0</v>
       </c>
@@ -5443,7 +5469,7 @@
       <c r="K163" s="23"/>
       <c r="L163" s="8"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12">
       <c r="A164" s="4" t="s">
         <v>1</v>
       </c>
@@ -5453,7 +5479,7 @@
       <c r="K164" s="23"/>
       <c r="L164" s="8"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12">
       <c r="A165" s="4" t="s">
         <v>2</v>
       </c>
@@ -5463,7 +5489,7 @@
       <c r="K165" s="23"/>
       <c r="L165" s="8"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12">
       <c r="A166" s="4" t="s">
         <v>3</v>
       </c>
@@ -5473,7 +5499,7 @@
       <c r="K166" s="23"/>
       <c r="L166" s="8"/>
     </row>
-    <row r="167" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" ht="15.75" thickBot="1">
       <c r="A167" s="5" t="s">
         <v>4</v>
       </c>
@@ -5489,7 +5515,7 @@
       <c r="K167" s="23"/>
       <c r="L167" s="8"/>
     </row>
-    <row r="168" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" ht="15.75" thickBot="1">
       <c r="A168" s="33" t="s">
         <v>6</v>
       </c>
@@ -5529,35 +5555,35 @@
       <c r="K168" s="23"/>
       <c r="L168" s="8"/>
     </row>
-    <row r="169" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="71"/>
-      <c r="B169" s="71"/>
-      <c r="C169" s="71"/>
-      <c r="D169" s="71"/>
-      <c r="E169" s="71"/>
-      <c r="F169" s="71"/>
-      <c r="G169" s="71"/>
-      <c r="H169" s="71"/>
-      <c r="I169" s="71"/>
-      <c r="J169" s="71"/>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A169" s="72"/>
+      <c r="B169" s="72"/>
+      <c r="C169" s="72"/>
+      <c r="D169" s="72"/>
+      <c r="E169" s="72"/>
+      <c r="F169" s="72"/>
+      <c r="G169" s="72"/>
+      <c r="H169" s="72"/>
+      <c r="I169" s="72"/>
+      <c r="J169" s="72"/>
+    </row>
+    <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="72"/>
-      <c r="C170" s="69"/>
-      <c r="D170" s="69"/>
-      <c r="E170" s="69"/>
-      <c r="F170" s="69"/>
-      <c r="G170" s="69"/>
-      <c r="H170" s="69"/>
-      <c r="I170" s="69"/>
-      <c r="J170" s="73"/>
+      <c r="B170" s="73"/>
+      <c r="C170" s="70"/>
+      <c r="D170" s="70"/>
+      <c r="E170" s="70"/>
+      <c r="F170" s="70"/>
+      <c r="G170" s="70"/>
+      <c r="H170" s="70"/>
+      <c r="I170" s="70"/>
+      <c r="J170" s="74"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12">
       <c r="A171" s="4" t="s">
         <v>0</v>
       </c>
@@ -5567,7 +5593,7 @@
       <c r="K171" s="23"/>
       <c r="L171" s="8"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12">
       <c r="A172" s="4" t="s">
         <v>1</v>
       </c>
@@ -5577,7 +5603,7 @@
       <c r="K172" s="23"/>
       <c r="L172" s="8"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12">
       <c r="A173" s="4" t="s">
         <v>2</v>
       </c>
@@ -5587,7 +5613,7 @@
       <c r="K173" s="23"/>
       <c r="L173" s="8"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12">
       <c r="A174" s="4" t="s">
         <v>3</v>
       </c>
@@ -5597,7 +5623,7 @@
       <c r="K174" s="23"/>
       <c r="L174" s="8"/>
     </row>
-    <row r="175" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" ht="15.75" thickBot="1">
       <c r="A175" s="5" t="s">
         <v>4</v>
       </c>
@@ -5613,7 +5639,7 @@
       <c r="K175" s="23"/>
       <c r="L175" s="8"/>
     </row>
-    <row r="176" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" ht="15.75" thickBot="1">
       <c r="A176" s="33" t="s">
         <v>6</v>
       </c>
@@ -5653,29 +5679,29 @@
       <c r="K176" s="23"/>
       <c r="L176" s="8"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A177" s="69"/>
-      <c r="B177" s="69"/>
-      <c r="C177" s="69"/>
-      <c r="D177" s="69"/>
-      <c r="E177" s="69"/>
-      <c r="F177" s="69"/>
-      <c r="G177" s="69"/>
-      <c r="H177" s="69"/>
-      <c r="I177" s="69"/>
-      <c r="J177" s="69"/>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A178" s="70"/>
-      <c r="B178" s="70"/>
-      <c r="C178" s="70"/>
-      <c r="D178" s="70"/>
-      <c r="E178" s="70"/>
-      <c r="F178" s="70"/>
-      <c r="G178" s="70"/>
-      <c r="H178" s="70"/>
-      <c r="I178" s="70"/>
-      <c r="J178" s="70"/>
+    <row r="177" spans="1:10">
+      <c r="A177" s="70"/>
+      <c r="B177" s="70"/>
+      <c r="C177" s="70"/>
+      <c r="D177" s="70"/>
+      <c r="E177" s="70"/>
+      <c r="F177" s="70"/>
+      <c r="G177" s="70"/>
+      <c r="H177" s="70"/>
+      <c r="I177" s="70"/>
+      <c r="J177" s="70"/>
+    </row>
+    <row r="178" spans="1:10">
+      <c r="A178" s="71"/>
+      <c r="B178" s="71"/>
+      <c r="C178" s="71"/>
+      <c r="D178" s="71"/>
+      <c r="E178" s="71"/>
+      <c r="F178" s="71"/>
+      <c r="G178" s="71"/>
+      <c r="H178" s="71"/>
+      <c r="I178" s="71"/>
+      <c r="J178" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="45">

</xml_diff>

<commit_message>
Uren reg, logo, hud imgs
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -739,22 +739,22 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1037,7 +1037,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1049,7 +1049,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M157" sqref="M157"/>
+      <selection pane="bottomLeft" activeCell="L154" sqref="L154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1109,7 +1109,7 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="71"/>
+      <c r="B2" s="75"/>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
       <c r="E2" s="72"/>
@@ -1117,21 +1117,21 @@
       <c r="G2" s="72"/>
       <c r="H2" s="72"/>
       <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
+      <c r="J2" s="76"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.96646341463414631</v>
+        <v>0.96696696696696693</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>35</v>
@@ -1175,11 +1175,11 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.84756097560975607</v>
+        <v>0.84684684684684686</v>
       </c>
       <c r="O3" s="54" t="s">
         <v>34</v>
@@ -1223,11 +1223,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.99085365853658536</v>
+        <v>0.99099099099099097</v>
       </c>
       <c r="O4" s="55" t="s">
         <v>36</v>
@@ -1271,11 +1271,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.92682926829268297</v>
+        <v>0.92792792792792789</v>
       </c>
       <c r="O5" s="56" t="s">
         <v>37</v>
@@ -1305,11 +1305,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.78048780487804881</v>
+        <v>0.78378378378378377</v>
       </c>
       <c r="O6" s="57" t="s">
         <v>38</v>
@@ -1353,11 +1353,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.71646341463414631</v>
+        <v>0.71771771771771775</v>
       </c>
       <c r="O7" s="58" t="s">
         <v>39</v>
@@ -1407,11 +1407,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.96951219512195119</v>
+        <v>0.96996996996996998</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>40</v>
@@ -1436,7 +1436,7 @@
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="71"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="72"/>
       <c r="D10" s="72"/>
       <c r="E10" s="72"/>
@@ -1444,7 +1444,7 @@
       <c r="G10" s="72"/>
       <c r="H10" s="72"/>
       <c r="I10" s="72"/>
-      <c r="J10" s="73"/>
+      <c r="J10" s="76"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1666,7 +1666,7 @@
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="71"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="72"/>
       <c r="D18" s="72"/>
       <c r="E18" s="72"/>
@@ -1674,7 +1674,7 @@
       <c r="G18" s="72"/>
       <c r="H18" s="72"/>
       <c r="I18" s="72"/>
-      <c r="J18" s="73"/>
+      <c r="J18" s="76"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1894,7 +1894,7 @@
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="71"/>
+      <c r="B26" s="75"/>
       <c r="C26" s="72"/>
       <c r="D26" s="72"/>
       <c r="E26" s="72"/>
@@ -1902,7 +1902,7 @@
       <c r="G26" s="72"/>
       <c r="H26" s="72"/>
       <c r="I26" s="72"/>
-      <c r="J26" s="73"/>
+      <c r="J26" s="76"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -2122,7 +2122,7 @@
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="71"/>
+      <c r="B34" s="75"/>
       <c r="C34" s="72"/>
       <c r="D34" s="72"/>
       <c r="E34" s="72"/>
@@ -2130,7 +2130,7 @@
       <c r="G34" s="72"/>
       <c r="H34" s="72"/>
       <c r="I34" s="72"/>
-      <c r="J34" s="73"/>
+      <c r="J34" s="76"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2352,7 +2352,7 @@
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="71"/>
+      <c r="B42" s="75"/>
       <c r="C42" s="72"/>
       <c r="D42" s="72"/>
       <c r="E42" s="72"/>
@@ -2360,7 +2360,7 @@
       <c r="G42" s="72"/>
       <c r="H42" s="72"/>
       <c r="I42" s="72"/>
-      <c r="J42" s="73"/>
+      <c r="J42" s="76"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2584,7 +2584,7 @@
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="71"/>
+      <c r="B50" s="75"/>
       <c r="C50" s="72"/>
       <c r="D50" s="72"/>
       <c r="E50" s="72"/>
@@ -2592,7 +2592,7 @@
       <c r="G50" s="72"/>
       <c r="H50" s="72"/>
       <c r="I50" s="72"/>
-      <c r="J50" s="73"/>
+      <c r="J50" s="76"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2812,7 +2812,7 @@
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="71"/>
+      <c r="B58" s="75"/>
       <c r="C58" s="72"/>
       <c r="D58" s="72"/>
       <c r="E58" s="72"/>
@@ -2820,7 +2820,7 @@
       <c r="G58" s="72"/>
       <c r="H58" s="72"/>
       <c r="I58" s="72"/>
-      <c r="J58" s="73"/>
+      <c r="J58" s="76"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -3044,7 +3044,7 @@
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="71"/>
+      <c r="B66" s="75"/>
       <c r="C66" s="72"/>
       <c r="D66" s="72"/>
       <c r="E66" s="72"/>
@@ -3052,7 +3052,7 @@
       <c r="G66" s="72"/>
       <c r="H66" s="72"/>
       <c r="I66" s="72"/>
-      <c r="J66" s="73"/>
+      <c r="J66" s="76"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -3202,7 +3202,7 @@
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="71"/>
+      <c r="B74" s="75"/>
       <c r="C74" s="72"/>
       <c r="D74" s="72"/>
       <c r="E74" s="72"/>
@@ -3210,7 +3210,7 @@
       <c r="G74" s="72"/>
       <c r="H74" s="72"/>
       <c r="I74" s="72"/>
-      <c r="J74" s="73"/>
+      <c r="J74" s="76"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3416,7 +3416,7 @@
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="71"/>
+      <c r="B82" s="75"/>
       <c r="C82" s="72"/>
       <c r="D82" s="72"/>
       <c r="E82" s="72"/>
@@ -3424,7 +3424,7 @@
       <c r="G82" s="72"/>
       <c r="H82" s="72"/>
       <c r="I82" s="72"/>
-      <c r="J82" s="73"/>
+      <c r="J82" s="76"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3646,7 +3646,7 @@
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="71"/>
+      <c r="B90" s="75"/>
       <c r="C90" s="72"/>
       <c r="D90" s="72"/>
       <c r="E90" s="72"/>
@@ -3654,7 +3654,7 @@
       <c r="G90" s="72"/>
       <c r="H90" s="72"/>
       <c r="I90" s="72"/>
-      <c r="J90" s="73"/>
+      <c r="J90" s="76"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3874,7 +3874,7 @@
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="71"/>
+      <c r="B98" s="75"/>
       <c r="C98" s="72"/>
       <c r="D98" s="72"/>
       <c r="E98" s="72"/>
@@ -3882,7 +3882,7 @@
       <c r="G98" s="72"/>
       <c r="H98" s="72"/>
       <c r="I98" s="72"/>
-      <c r="J98" s="73"/>
+      <c r="J98" s="76"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -4104,7 +4104,7 @@
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="71"/>
+      <c r="B106" s="75"/>
       <c r="C106" s="72"/>
       <c r="D106" s="72"/>
       <c r="E106" s="72"/>
@@ -4112,7 +4112,7 @@
       <c r="G106" s="72"/>
       <c r="H106" s="72"/>
       <c r="I106" s="72"/>
-      <c r="J106" s="73"/>
+      <c r="J106" s="76"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -4334,7 +4334,7 @@
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="71"/>
+      <c r="B114" s="75"/>
       <c r="C114" s="72"/>
       <c r="D114" s="72"/>
       <c r="E114" s="72"/>
@@ -4342,7 +4342,7 @@
       <c r="G114" s="72"/>
       <c r="H114" s="72"/>
       <c r="I114" s="72"/>
-      <c r="J114" s="73"/>
+      <c r="J114" s="76"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -4562,7 +4562,7 @@
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="71"/>
+      <c r="B122" s="75"/>
       <c r="C122" s="72"/>
       <c r="D122" s="72"/>
       <c r="E122" s="72"/>
@@ -4570,7 +4570,7 @@
       <c r="G122" s="72"/>
       <c r="H122" s="72"/>
       <c r="I122" s="72"/>
-      <c r="J122" s="73"/>
+      <c r="J122" s="76"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -4778,7 +4778,7 @@
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="71"/>
+      <c r="B130" s="75"/>
       <c r="C130" s="72"/>
       <c r="D130" s="72"/>
       <c r="E130" s="72"/>
@@ -4786,7 +4786,7 @@
       <c r="G130" s="72"/>
       <c r="H130" s="72"/>
       <c r="I130" s="72"/>
-      <c r="J130" s="73"/>
+      <c r="J130" s="76"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -5006,7 +5006,7 @@
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="71"/>
+      <c r="B138" s="75"/>
       <c r="C138" s="72"/>
       <c r="D138" s="72"/>
       <c r="E138" s="72"/>
@@ -5014,7 +5014,7 @@
       <c r="G138" s="72"/>
       <c r="H138" s="72"/>
       <c r="I138" s="72"/>
-      <c r="J138" s="73"/>
+      <c r="J138" s="76"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -5164,7 +5164,7 @@
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="71"/>
+      <c r="B146" s="75"/>
       <c r="C146" s="72"/>
       <c r="D146" s="72"/>
       <c r="E146" s="72"/>
@@ -5172,7 +5172,7 @@
       <c r="G146" s="72"/>
       <c r="H146" s="72"/>
       <c r="I146" s="72"/>
-      <c r="J146" s="73"/>
+      <c r="J146" s="76"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -5378,7 +5378,7 @@
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="71"/>
+      <c r="B154" s="75"/>
       <c r="C154" s="72"/>
       <c r="D154" s="72"/>
       <c r="E154" s="72"/>
@@ -5386,7 +5386,7 @@
       <c r="G154" s="72"/>
       <c r="H154" s="72"/>
       <c r="I154" s="72"/>
-      <c r="J154" s="73"/>
+      <c r="J154" s="76"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -5412,7 +5412,7 @@
       <c r="G155" s="6">
         <v>4</v>
       </c>
-      <c r="H155" s="76">
+      <c r="H155" s="71">
         <v>3</v>
       </c>
       <c r="I155" s="6">
@@ -5426,8 +5426,30 @@
       <c r="A156" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B156" s="8"/>
-      <c r="H156" s="67"/>
+      <c r="B156" s="8">
+        <v>5</v>
+      </c>
+      <c r="C156" s="6">
+        <v>5</v>
+      </c>
+      <c r="D156" s="30">
+        <v>4</v>
+      </c>
+      <c r="E156" s="6">
+        <v>5</v>
+      </c>
+      <c r="F156" s="6">
+        <v>5</v>
+      </c>
+      <c r="G156" s="6">
+        <v>5</v>
+      </c>
+      <c r="H156" s="71">
+        <v>4</v>
+      </c>
+      <c r="I156" s="6">
+        <v>5</v>
+      </c>
       <c r="J156" s="1"/>
       <c r="K156" s="23"/>
       <c r="L156" s="8"/>
@@ -5474,35 +5496,35 @@
       </c>
       <c r="B160" s="34">
         <f>B155+B156+B157+B158+B159</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C160" s="35">
         <f t="shared" ref="C160:I160" si="19">SUM(C155:C159)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D160" s="35">
         <f t="shared" si="19"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E160" s="35">
         <f t="shared" si="19"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F160" s="35">
         <f t="shared" si="19"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G160" s="35">
         <f t="shared" si="19"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H160" s="35">
         <f t="shared" si="19"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I160" s="35">
         <f t="shared" si="19"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J160" s="36"/>
       <c r="K160" s="23"/>
@@ -5524,7 +5546,7 @@
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="71"/>
+      <c r="B162" s="75"/>
       <c r="C162" s="72"/>
       <c r="D162" s="72"/>
       <c r="E162" s="72"/>
@@ -5532,7 +5554,7 @@
       <c r="G162" s="72"/>
       <c r="H162" s="72"/>
       <c r="I162" s="72"/>
-      <c r="J162" s="73"/>
+      <c r="J162" s="76"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -5648,7 +5670,7 @@
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="71"/>
+      <c r="B170" s="75"/>
       <c r="C170" s="72"/>
       <c r="D170" s="72"/>
       <c r="E170" s="72"/>
@@ -5656,7 +5678,7 @@
       <c r="G170" s="72"/>
       <c r="H170" s="72"/>
       <c r="I170" s="72"/>
-      <c r="J170" s="73"/>
+      <c r="J170" s="76"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -5769,51 +5791,19 @@
       <c r="J177" s="72"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="75"/>
-      <c r="B178" s="75"/>
-      <c r="C178" s="75"/>
-      <c r="D178" s="75"/>
-      <c r="E178" s="75"/>
-      <c r="F178" s="75"/>
-      <c r="G178" s="75"/>
-      <c r="H178" s="75"/>
-      <c r="I178" s="75"/>
-      <c r="J178" s="75"/>
+      <c r="A178" s="73"/>
+      <c r="B178" s="73"/>
+      <c r="C178" s="73"/>
+      <c r="D178" s="73"/>
+      <c r="E178" s="73"/>
+      <c r="F178" s="73"/>
+      <c r="G178" s="73"/>
+      <c r="H178" s="73"/>
+      <c r="I178" s="73"/>
+      <c r="J178" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="B154:J154"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="B162:J162"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="B170:J170"/>
-    <mergeCell ref="B146:J146"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B114:J114"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="B122:J122"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="B130:J130"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="B138:J138"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="B98:J98"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A97:J97"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="B2:J2"/>
@@ -5827,6 +5817,38 @@
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B98:J98"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="B82:J82"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="B146:J146"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="B114:J114"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="B122:J122"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="B130:J130"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="B138:J138"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="B154:J154"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="B162:J162"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="B170:J170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uren reg, default ability script, ui stuff
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="67">
   <si>
     <t>Maandag</t>
   </si>
@@ -257,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,6 +363,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -757,6 +763,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -765,10 +777,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99CC"/>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FFD7AFFF"/>
-      <color rgb="FFFFCCFF"/>
-      <color rgb="FFFF99CC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1048,8 +1060,8 @@
   <dimension ref="A1:P178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L154" sqref="L154"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L157" sqref="L157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1123,15 +1135,15 @@
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.96696696696696693</v>
+        <v>0.96745562130177509</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>35</v>
@@ -1175,11 +1187,11 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.84684684684684686</v>
+        <v>0.84319526627218933</v>
       </c>
       <c r="O3" s="54" t="s">
         <v>34</v>
@@ -1223,11 +1235,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.99099099099099097</v>
+        <v>0.99112426035502954</v>
       </c>
       <c r="O4" s="55" t="s">
         <v>36</v>
@@ -1271,11 +1283,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.92792792792792789</v>
+        <v>0.92899408284023666</v>
       </c>
       <c r="O5" s="56" t="s">
         <v>37</v>
@@ -1305,11 +1317,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.78378378378378377</v>
+        <v>0.77810650887573962</v>
       </c>
       <c r="O6" s="57" t="s">
         <v>38</v>
@@ -1353,11 +1365,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.71771771771771775</v>
+        <v>0.71597633136094674</v>
       </c>
       <c r="O7" s="58" t="s">
         <v>39</v>
@@ -1407,11 +1419,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.96996996996996998</v>
+        <v>0.97041420118343191</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>40</v>
@@ -5458,8 +5470,30 @@
       <c r="A157" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B157" s="8"/>
-      <c r="H157" s="67"/>
+      <c r="B157" s="8">
+        <v>3</v>
+      </c>
+      <c r="C157" s="6">
+        <v>3</v>
+      </c>
+      <c r="D157" s="45">
+        <v>3</v>
+      </c>
+      <c r="E157" s="6">
+        <v>3</v>
+      </c>
+      <c r="F157" s="6">
+        <v>3</v>
+      </c>
+      <c r="G157" s="28">
+        <v>0</v>
+      </c>
+      <c r="H157" s="67">
+        <v>3</v>
+      </c>
+      <c r="I157" s="6">
+        <v>3</v>
+      </c>
       <c r="J157" s="1"/>
       <c r="K157" s="23"/>
       <c r="L157" s="8"/>
@@ -5468,25 +5502,47 @@
       <c r="A158" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B158" s="8"/>
-      <c r="H158" s="67"/>
+      <c r="B158" s="8">
+        <v>2</v>
+      </c>
+      <c r="C158" s="6">
+        <v>2</v>
+      </c>
+      <c r="D158" s="78"/>
+      <c r="E158" s="6">
+        <v>2</v>
+      </c>
+      <c r="F158" s="6">
+        <v>2</v>
+      </c>
+      <c r="G158" s="6">
+        <v>2</v>
+      </c>
+      <c r="H158" s="77">
+        <v>0</v>
+      </c>
+      <c r="I158" s="6">
+        <v>2</v>
+      </c>
       <c r="J158" s="1"/>
       <c r="K158" s="23"/>
       <c r="L158" s="8"/>
     </row>
     <row r="159" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A159" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B159" s="7"/>
-      <c r="C159" s="7"/>
-      <c r="D159" s="7"/>
-      <c r="E159" s="7"/>
-      <c r="F159" s="7"/>
-      <c r="G159" s="7"/>
-      <c r="H159" s="68"/>
-      <c r="I159" s="7"/>
-      <c r="J159" s="2"/>
+      <c r="A159" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B159" s="20"/>
+      <c r="C159" s="21"/>
+      <c r="D159" s="21"/>
+      <c r="E159" s="21"/>
+      <c r="F159" s="21"/>
+      <c r="G159" s="21"/>
+      <c r="H159" s="21"/>
+      <c r="I159" s="21"/>
+      <c r="J159" s="22" t="s">
+        <v>41</v>
+      </c>
       <c r="K159" s="23"/>
       <c r="L159" s="8"/>
     </row>
@@ -5496,35 +5552,35 @@
       </c>
       <c r="B160" s="34">
         <f>B155+B156+B157+B158+B159</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C160" s="35">
         <f t="shared" ref="C160:I160" si="19">SUM(C155:C159)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D160" s="35">
         <f t="shared" si="19"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E160" s="35">
         <f t="shared" si="19"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F160" s="35">
         <f t="shared" si="19"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G160" s="35">
         <f t="shared" si="19"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H160" s="35">
         <f t="shared" si="19"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I160" s="35">
         <f t="shared" si="19"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J160" s="36"/>
       <c r="K160" s="23"/>

</xml_diff>

<commit_message>
Uren reg + Fixed Dying
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -1052,7 +1052,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
+      <selection pane="bottomLeft" activeCell="K165" sqref="K165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1126,15 +1126,15 @@
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.96829971181556196</v>
+        <v>0.9683908045977011</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>35</v>
@@ -1178,11 +1178,11 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.82132564841498557</v>
+        <v>0.83620689655172409</v>
       </c>
       <c r="O3" s="54" t="s">
         <v>34</v>
@@ -1226,11 +1226,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.99135446685878958</v>
+        <v>0.99137931034482762</v>
       </c>
       <c r="O4" s="55" t="s">
         <v>36</v>
@@ -1274,11 +1274,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.93083573487031701</v>
+        <v>0.93103448275862066</v>
       </c>
       <c r="O5" s="56" t="s">
         <v>37</v>
@@ -1308,11 +1308,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.78386167146974062</v>
+        <v>0.78448275862068961</v>
       </c>
       <c r="O6" s="57" t="s">
         <v>38</v>
@@ -1356,11 +1356,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.72046109510086453</v>
+        <v>0.72126436781609193</v>
       </c>
       <c r="O7" s="58" t="s">
         <v>39</v>
@@ -1410,11 +1410,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.97118155619596547</v>
+        <v>0.97126436781609193</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>40</v>
@@ -5499,7 +5499,9 @@
       <c r="C158" s="6">
         <v>2</v>
       </c>
-      <c r="D158" s="61"/>
+      <c r="D158" s="61">
+        <v>1</v>
+      </c>
       <c r="E158" s="6">
         <v>2</v>
       </c>
@@ -5551,7 +5553,7 @@
       </c>
       <c r="D160" s="35">
         <f t="shared" si="19"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E160" s="35">
         <f t="shared" si="19"/>
@@ -5615,7 +5617,9 @@
       <c r="C163" s="6">
         <v>4</v>
       </c>
-      <c r="D163" s="61"/>
+      <c r="D163" s="61">
+        <v>2</v>
+      </c>
       <c r="E163" s="6">
         <v>4</v>
       </c>
@@ -5645,7 +5649,9 @@
       <c r="C164" s="6">
         <v>5</v>
       </c>
-      <c r="D164" s="61"/>
+      <c r="D164" s="61">
+        <v>2</v>
+      </c>
       <c r="E164" s="6">
         <v>5</v>
       </c>
@@ -5669,8 +5675,30 @@
       <c r="A165" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B165" s="8"/>
-      <c r="H165" s="67"/>
+      <c r="B165" s="8">
+        <v>1</v>
+      </c>
+      <c r="C165" s="6">
+        <v>1</v>
+      </c>
+      <c r="D165" s="6">
+        <v>1</v>
+      </c>
+      <c r="E165" s="6">
+        <v>1</v>
+      </c>
+      <c r="F165" s="6">
+        <v>1</v>
+      </c>
+      <c r="G165" s="6">
+        <v>1</v>
+      </c>
+      <c r="H165" s="67">
+        <v>1</v>
+      </c>
+      <c r="I165" s="6">
+        <v>1</v>
+      </c>
       <c r="J165" s="1"/>
       <c r="K165" s="23"/>
       <c r="L165" s="8"/>
@@ -5707,35 +5735,35 @@
       </c>
       <c r="B168" s="34">
         <f>B163+B164+B165+B166+B167</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C168" s="35">
         <f t="shared" ref="C168:I168" si="20">SUM(C163:C167)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D168" s="35">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E168" s="35">
         <f t="shared" si="20"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F168" s="35">
         <f t="shared" si="20"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G168" s="35">
         <f t="shared" si="20"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H168" s="35">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I168" s="35">
         <f t="shared" si="20"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J168" s="36"/>
       <c r="K168" s="23"/>

</xml_diff>

<commit_message>
Uren reg + script fix
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="67">
   <si>
     <t>Maandag</t>
   </si>
@@ -745,19 +745,19 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1040,7 +1040,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1051,8 +1051,8 @@
   <dimension ref="A1:P178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K165" sqref="K165"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L167" sqref="L167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1112,29 +1112,29 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="77"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="75"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.9683908045977011</v>
+        <v>0.96875</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>35</v>
@@ -1178,11 +1178,11 @@
       <c r="L3" s="8"/>
       <c r="M3" s="6">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.83620689655172409</v>
+        <v>0.83806818181818177</v>
       </c>
       <c r="O3" s="54" t="s">
         <v>34</v>
@@ -1226,11 +1226,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.99137931034482762</v>
+        <v>0.99147727272727271</v>
       </c>
       <c r="O4" s="55" t="s">
         <v>36</v>
@@ -1274,11 +1274,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.93103448275862066</v>
+        <v>0.93181818181818177</v>
       </c>
       <c r="O5" s="56" t="s">
         <v>37</v>
@@ -1308,11 +1308,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.78448275862068961</v>
+        <v>0.78693181818181823</v>
       </c>
       <c r="O6" s="57" t="s">
         <v>38</v>
@@ -1356,11 +1356,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.72126436781609193</v>
+        <v>0.72443181818181823</v>
       </c>
       <c r="O7" s="58" t="s">
         <v>39</v>
@@ -1410,11 +1410,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.97126436781609193</v>
+        <v>0.97159090909090906</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>40</v>
@@ -1424,30 +1424,30 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A9" s="75"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="77"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="75"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1654,30 +1654,30 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="75"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
+      <c r="A17" s="76"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="77"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="75"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1882,30 +1882,30 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="75"/>
+      <c r="A25" s="76"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="77"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="75"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -2110,30 +2110,30 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="75"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
+      <c r="A33" s="76"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="76"/>
+      <c r="J33" s="76"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="76"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="77"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="75"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2340,30 +2340,30 @@
       <c r="L40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A41" s="75"/>
-      <c r="B41" s="75"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="76"/>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="73"/>
-      <c r="J42" s="77"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="74"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="75"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2572,30 +2572,30 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="75"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="75"/>
-      <c r="I49" s="75"/>
-      <c r="J49" s="75"/>
+      <c r="A49" s="76"/>
+      <c r="B49" s="76"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
+      <c r="J49" s="76"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="76"/>
-      <c r="C50" s="73"/>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="73"/>
-      <c r="I50" s="73"/>
-      <c r="J50" s="77"/>
+      <c r="B50" s="73"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="75"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2800,30 +2800,30 @@
       <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="75"/>
-      <c r="B57" s="75"/>
-      <c r="C57" s="75"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="75"/>
-      <c r="I57" s="75"/>
-      <c r="J57" s="75"/>
+      <c r="A57" s="76"/>
+      <c r="B57" s="76"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="76"/>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="73"/>
-      <c r="G58" s="73"/>
-      <c r="H58" s="73"/>
-      <c r="I58" s="73"/>
-      <c r="J58" s="77"/>
+      <c r="B58" s="73"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="74"/>
+      <c r="I58" s="74"/>
+      <c r="J58" s="75"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -3032,30 +3032,30 @@
       <c r="L64" s="8"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A65" s="75"/>
-      <c r="B65" s="75"/>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="75"/>
-      <c r="H65" s="75"/>
-      <c r="I65" s="75"/>
-      <c r="J65" s="75"/>
+      <c r="A65" s="76"/>
+      <c r="B65" s="76"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="76"/>
+      <c r="G65" s="76"/>
+      <c r="H65" s="76"/>
+      <c r="I65" s="76"/>
+      <c r="J65" s="76"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="76"/>
-      <c r="C66" s="73"/>
-      <c r="D66" s="73"/>
-      <c r="E66" s="73"/>
-      <c r="F66" s="73"/>
-      <c r="G66" s="73"/>
-      <c r="H66" s="73"/>
-      <c r="I66" s="73"/>
-      <c r="J66" s="77"/>
+      <c r="B66" s="73"/>
+      <c r="C66" s="74"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
+      <c r="F66" s="74"/>
+      <c r="G66" s="74"/>
+      <c r="H66" s="74"/>
+      <c r="I66" s="74"/>
+      <c r="J66" s="75"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -3190,30 +3190,30 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A73" s="75"/>
-      <c r="B73" s="75"/>
-      <c r="C73" s="75"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
-      <c r="I73" s="75"/>
-      <c r="J73" s="75"/>
+      <c r="A73" s="76"/>
+      <c r="B73" s="76"/>
+      <c r="C73" s="76"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="76"/>
+      <c r="G73" s="76"/>
+      <c r="H73" s="76"/>
+      <c r="I73" s="76"/>
+      <c r="J73" s="76"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="76"/>
-      <c r="C74" s="73"/>
-      <c r="D74" s="73"/>
-      <c r="E74" s="73"/>
-      <c r="F74" s="73"/>
-      <c r="G74" s="73"/>
-      <c r="H74" s="73"/>
-      <c r="I74" s="73"/>
-      <c r="J74" s="77"/>
+      <c r="B74" s="73"/>
+      <c r="C74" s="74"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="74"/>
+      <c r="H74" s="74"/>
+      <c r="I74" s="74"/>
+      <c r="J74" s="75"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3404,30 +3404,30 @@
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A81" s="75"/>
-      <c r="B81" s="75"/>
-      <c r="C81" s="75"/>
-      <c r="D81" s="75"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="75"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
-      <c r="I81" s="75"/>
-      <c r="J81" s="75"/>
+      <c r="A81" s="76"/>
+      <c r="B81" s="76"/>
+      <c r="C81" s="76"/>
+      <c r="D81" s="76"/>
+      <c r="E81" s="76"/>
+      <c r="F81" s="76"/>
+      <c r="G81" s="76"/>
+      <c r="H81" s="76"/>
+      <c r="I81" s="76"/>
+      <c r="J81" s="76"/>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="76"/>
-      <c r="C82" s="73"/>
-      <c r="D82" s="73"/>
-      <c r="E82" s="73"/>
-      <c r="F82" s="73"/>
-      <c r="G82" s="73"/>
-      <c r="H82" s="73"/>
-      <c r="I82" s="73"/>
-      <c r="J82" s="77"/>
+      <c r="B82" s="73"/>
+      <c r="C82" s="74"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="74"/>
+      <c r="F82" s="74"/>
+      <c r="G82" s="74"/>
+      <c r="H82" s="74"/>
+      <c r="I82" s="74"/>
+      <c r="J82" s="75"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3634,30 +3634,30 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A89" s="75"/>
-      <c r="B89" s="75"/>
-      <c r="C89" s="75"/>
-      <c r="D89" s="75"/>
-      <c r="E89" s="75"/>
-      <c r="F89" s="75"/>
-      <c r="G89" s="75"/>
-      <c r="H89" s="75"/>
-      <c r="I89" s="75"/>
-      <c r="J89" s="75"/>
+      <c r="A89" s="76"/>
+      <c r="B89" s="76"/>
+      <c r="C89" s="76"/>
+      <c r="D89" s="76"/>
+      <c r="E89" s="76"/>
+      <c r="F89" s="76"/>
+      <c r="G89" s="76"/>
+      <c r="H89" s="76"/>
+      <c r="I89" s="76"/>
+      <c r="J89" s="76"/>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="76"/>
-      <c r="C90" s="73"/>
-      <c r="D90" s="73"/>
-      <c r="E90" s="73"/>
-      <c r="F90" s="73"/>
-      <c r="G90" s="73"/>
-      <c r="H90" s="73"/>
-      <c r="I90" s="73"/>
-      <c r="J90" s="77"/>
+      <c r="B90" s="73"/>
+      <c r="C90" s="74"/>
+      <c r="D90" s="74"/>
+      <c r="E90" s="74"/>
+      <c r="F90" s="74"/>
+      <c r="G90" s="74"/>
+      <c r="H90" s="74"/>
+      <c r="I90" s="74"/>
+      <c r="J90" s="75"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3862,30 +3862,30 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A97" s="75"/>
-      <c r="B97" s="75"/>
-      <c r="C97" s="75"/>
-      <c r="D97" s="75"/>
-      <c r="E97" s="75"/>
-      <c r="F97" s="75"/>
-      <c r="G97" s="75"/>
-      <c r="H97" s="75"/>
-      <c r="I97" s="75"/>
-      <c r="J97" s="75"/>
+      <c r="A97" s="76"/>
+      <c r="B97" s="76"/>
+      <c r="C97" s="76"/>
+      <c r="D97" s="76"/>
+      <c r="E97" s="76"/>
+      <c r="F97" s="76"/>
+      <c r="G97" s="76"/>
+      <c r="H97" s="76"/>
+      <c r="I97" s="76"/>
+      <c r="J97" s="76"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="76"/>
-      <c r="C98" s="73"/>
-      <c r="D98" s="73"/>
-      <c r="E98" s="73"/>
-      <c r="F98" s="73"/>
-      <c r="G98" s="73"/>
-      <c r="H98" s="73"/>
-      <c r="I98" s="73"/>
-      <c r="J98" s="77"/>
+      <c r="B98" s="73"/>
+      <c r="C98" s="74"/>
+      <c r="D98" s="74"/>
+      <c r="E98" s="74"/>
+      <c r="F98" s="74"/>
+      <c r="G98" s="74"/>
+      <c r="H98" s="74"/>
+      <c r="I98" s="74"/>
+      <c r="J98" s="75"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -4092,30 +4092,30 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A105" s="75"/>
-      <c r="B105" s="75"/>
-      <c r="C105" s="75"/>
-      <c r="D105" s="75"/>
-      <c r="E105" s="75"/>
-      <c r="F105" s="75"/>
-      <c r="G105" s="75"/>
-      <c r="H105" s="75"/>
-      <c r="I105" s="75"/>
-      <c r="J105" s="75"/>
+      <c r="A105" s="76"/>
+      <c r="B105" s="76"/>
+      <c r="C105" s="76"/>
+      <c r="D105" s="76"/>
+      <c r="E105" s="76"/>
+      <c r="F105" s="76"/>
+      <c r="G105" s="76"/>
+      <c r="H105" s="76"/>
+      <c r="I105" s="76"/>
+      <c r="J105" s="76"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="76"/>
-      <c r="C106" s="73"/>
-      <c r="D106" s="73"/>
-      <c r="E106" s="73"/>
-      <c r="F106" s="73"/>
-      <c r="G106" s="73"/>
-      <c r="H106" s="73"/>
-      <c r="I106" s="73"/>
-      <c r="J106" s="77"/>
+      <c r="B106" s="73"/>
+      <c r="C106" s="74"/>
+      <c r="D106" s="74"/>
+      <c r="E106" s="74"/>
+      <c r="F106" s="74"/>
+      <c r="G106" s="74"/>
+      <c r="H106" s="74"/>
+      <c r="I106" s="74"/>
+      <c r="J106" s="75"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -4322,30 +4322,30 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A113" s="75"/>
-      <c r="B113" s="75"/>
-      <c r="C113" s="75"/>
-      <c r="D113" s="75"/>
-      <c r="E113" s="75"/>
-      <c r="F113" s="75"/>
-      <c r="G113" s="75"/>
-      <c r="H113" s="75"/>
-      <c r="I113" s="75"/>
-      <c r="J113" s="75"/>
+      <c r="A113" s="76"/>
+      <c r="B113" s="76"/>
+      <c r="C113" s="76"/>
+      <c r="D113" s="76"/>
+      <c r="E113" s="76"/>
+      <c r="F113" s="76"/>
+      <c r="G113" s="76"/>
+      <c r="H113" s="76"/>
+      <c r="I113" s="76"/>
+      <c r="J113" s="76"/>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="76"/>
-      <c r="C114" s="73"/>
-      <c r="D114" s="73"/>
-      <c r="E114" s="73"/>
-      <c r="F114" s="73"/>
-      <c r="G114" s="73"/>
-      <c r="H114" s="73"/>
-      <c r="I114" s="73"/>
-      <c r="J114" s="77"/>
+      <c r="B114" s="73"/>
+      <c r="C114" s="74"/>
+      <c r="D114" s="74"/>
+      <c r="E114" s="74"/>
+      <c r="F114" s="74"/>
+      <c r="G114" s="74"/>
+      <c r="H114" s="74"/>
+      <c r="I114" s="74"/>
+      <c r="J114" s="75"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -4550,30 +4550,30 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A121" s="75"/>
-      <c r="B121" s="75"/>
-      <c r="C121" s="75"/>
-      <c r="D121" s="75"/>
-      <c r="E121" s="75"/>
-      <c r="F121" s="75"/>
-      <c r="G121" s="75"/>
-      <c r="H121" s="75"/>
-      <c r="I121" s="75"/>
-      <c r="J121" s="75"/>
+      <c r="A121" s="76"/>
+      <c r="B121" s="76"/>
+      <c r="C121" s="76"/>
+      <c r="D121" s="76"/>
+      <c r="E121" s="76"/>
+      <c r="F121" s="76"/>
+      <c r="G121" s="76"/>
+      <c r="H121" s="76"/>
+      <c r="I121" s="76"/>
+      <c r="J121" s="76"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="76"/>
-      <c r="C122" s="73"/>
-      <c r="D122" s="73"/>
-      <c r="E122" s="73"/>
-      <c r="F122" s="73"/>
-      <c r="G122" s="73"/>
-      <c r="H122" s="73"/>
-      <c r="I122" s="73"/>
-      <c r="J122" s="77"/>
+      <c r="B122" s="73"/>
+      <c r="C122" s="74"/>
+      <c r="D122" s="74"/>
+      <c r="E122" s="74"/>
+      <c r="F122" s="74"/>
+      <c r="G122" s="74"/>
+      <c r="H122" s="74"/>
+      <c r="I122" s="74"/>
+      <c r="J122" s="75"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -4766,30 +4766,30 @@
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A129" s="75"/>
-      <c r="B129" s="75"/>
-      <c r="C129" s="75"/>
-      <c r="D129" s="75"/>
-      <c r="E129" s="75"/>
-      <c r="F129" s="75"/>
-      <c r="G129" s="75"/>
-      <c r="H129" s="75"/>
-      <c r="I129" s="75"/>
-      <c r="J129" s="75"/>
+      <c r="A129" s="76"/>
+      <c r="B129" s="76"/>
+      <c r="C129" s="76"/>
+      <c r="D129" s="76"/>
+      <c r="E129" s="76"/>
+      <c r="F129" s="76"/>
+      <c r="G129" s="76"/>
+      <c r="H129" s="76"/>
+      <c r="I129" s="76"/>
+      <c r="J129" s="76"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="76"/>
-      <c r="C130" s="73"/>
-      <c r="D130" s="73"/>
-      <c r="E130" s="73"/>
-      <c r="F130" s="73"/>
-      <c r="G130" s="73"/>
-      <c r="H130" s="73"/>
-      <c r="I130" s="73"/>
-      <c r="J130" s="77"/>
+      <c r="B130" s="73"/>
+      <c r="C130" s="74"/>
+      <c r="D130" s="74"/>
+      <c r="E130" s="74"/>
+      <c r="F130" s="74"/>
+      <c r="G130" s="74"/>
+      <c r="H130" s="74"/>
+      <c r="I130" s="74"/>
+      <c r="J130" s="75"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -4994,30 +4994,30 @@
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A137" s="75"/>
-      <c r="B137" s="75"/>
-      <c r="C137" s="75"/>
-      <c r="D137" s="75"/>
-      <c r="E137" s="75"/>
-      <c r="F137" s="75"/>
-      <c r="G137" s="75"/>
-      <c r="H137" s="75"/>
-      <c r="I137" s="75"/>
-      <c r="J137" s="75"/>
+      <c r="A137" s="76"/>
+      <c r="B137" s="76"/>
+      <c r="C137" s="76"/>
+      <c r="D137" s="76"/>
+      <c r="E137" s="76"/>
+      <c r="F137" s="76"/>
+      <c r="G137" s="76"/>
+      <c r="H137" s="76"/>
+      <c r="I137" s="76"/>
+      <c r="J137" s="76"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="76"/>
-      <c r="C138" s="73"/>
-      <c r="D138" s="73"/>
-      <c r="E138" s="73"/>
-      <c r="F138" s="73"/>
-      <c r="G138" s="73"/>
-      <c r="H138" s="73"/>
-      <c r="I138" s="73"/>
-      <c r="J138" s="77"/>
+      <c r="B138" s="73"/>
+      <c r="C138" s="74"/>
+      <c r="D138" s="74"/>
+      <c r="E138" s="74"/>
+      <c r="F138" s="74"/>
+      <c r="G138" s="74"/>
+      <c r="H138" s="74"/>
+      <c r="I138" s="74"/>
+      <c r="J138" s="75"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -5152,30 +5152,30 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A145" s="75"/>
-      <c r="B145" s="75"/>
-      <c r="C145" s="75"/>
-      <c r="D145" s="75"/>
-      <c r="E145" s="75"/>
-      <c r="F145" s="75"/>
-      <c r="G145" s="75"/>
-      <c r="H145" s="75"/>
-      <c r="I145" s="75"/>
-      <c r="J145" s="75"/>
+      <c r="A145" s="76"/>
+      <c r="B145" s="76"/>
+      <c r="C145" s="76"/>
+      <c r="D145" s="76"/>
+      <c r="E145" s="76"/>
+      <c r="F145" s="76"/>
+      <c r="G145" s="76"/>
+      <c r="H145" s="76"/>
+      <c r="I145" s="76"/>
+      <c r="J145" s="76"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="76"/>
-      <c r="C146" s="73"/>
-      <c r="D146" s="73"/>
-      <c r="E146" s="73"/>
-      <c r="F146" s="73"/>
-      <c r="G146" s="73"/>
-      <c r="H146" s="73"/>
-      <c r="I146" s="73"/>
-      <c r="J146" s="77"/>
+      <c r="B146" s="73"/>
+      <c r="C146" s="74"/>
+      <c r="D146" s="74"/>
+      <c r="E146" s="74"/>
+      <c r="F146" s="74"/>
+      <c r="G146" s="74"/>
+      <c r="H146" s="74"/>
+      <c r="I146" s="74"/>
+      <c r="J146" s="75"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -5366,30 +5366,30 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A153" s="75"/>
-      <c r="B153" s="75"/>
-      <c r="C153" s="75"/>
-      <c r="D153" s="75"/>
-      <c r="E153" s="75"/>
-      <c r="F153" s="75"/>
-      <c r="G153" s="75"/>
-      <c r="H153" s="75"/>
-      <c r="I153" s="75"/>
-      <c r="J153" s="75"/>
+      <c r="A153" s="76"/>
+      <c r="B153" s="76"/>
+      <c r="C153" s="76"/>
+      <c r="D153" s="76"/>
+      <c r="E153" s="76"/>
+      <c r="F153" s="76"/>
+      <c r="G153" s="76"/>
+      <c r="H153" s="76"/>
+      <c r="I153" s="76"/>
+      <c r="J153" s="76"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="76"/>
-      <c r="C154" s="73"/>
-      <c r="D154" s="73"/>
-      <c r="E154" s="73"/>
-      <c r="F154" s="73"/>
-      <c r="G154" s="73"/>
-      <c r="H154" s="73"/>
-      <c r="I154" s="73"/>
-      <c r="J154" s="77"/>
+      <c r="B154" s="73"/>
+      <c r="C154" s="74"/>
+      <c r="D154" s="74"/>
+      <c r="E154" s="74"/>
+      <c r="F154" s="74"/>
+      <c r="G154" s="74"/>
+      <c r="H154" s="74"/>
+      <c r="I154" s="74"/>
+      <c r="J154" s="75"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -5580,30 +5580,30 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A161" s="75"/>
-      <c r="B161" s="75"/>
-      <c r="C161" s="75"/>
-      <c r="D161" s="75"/>
-      <c r="E161" s="75"/>
-      <c r="F161" s="75"/>
-      <c r="G161" s="75"/>
-      <c r="H161" s="75"/>
-      <c r="I161" s="75"/>
-      <c r="J161" s="75"/>
+      <c r="A161" s="76"/>
+      <c r="B161" s="76"/>
+      <c r="C161" s="76"/>
+      <c r="D161" s="76"/>
+      <c r="E161" s="76"/>
+      <c r="F161" s="76"/>
+      <c r="G161" s="76"/>
+      <c r="H161" s="76"/>
+      <c r="I161" s="76"/>
+      <c r="J161" s="76"/>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="76"/>
-      <c r="C162" s="73"/>
-      <c r="D162" s="73"/>
-      <c r="E162" s="73"/>
-      <c r="F162" s="73"/>
-      <c r="G162" s="73"/>
-      <c r="H162" s="73"/>
-      <c r="I162" s="73"/>
-      <c r="J162" s="77"/>
+      <c r="B162" s="73"/>
+      <c r="C162" s="74"/>
+      <c r="D162" s="74"/>
+      <c r="E162" s="74"/>
+      <c r="F162" s="74"/>
+      <c r="G162" s="74"/>
+      <c r="H162" s="74"/>
+      <c r="I162" s="74"/>
+      <c r="J162" s="75"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -5704,12 +5704,20 @@
       <c r="L165" s="8"/>
     </row>
     <row r="166" spans="1:12">
-      <c r="A166" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B166" s="8"/>
-      <c r="H166" s="67"/>
-      <c r="J166" s="1"/>
+      <c r="A166" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166" s="20"/>
+      <c r="C166" s="21"/>
+      <c r="D166" s="21"/>
+      <c r="E166" s="21"/>
+      <c r="F166" s="21"/>
+      <c r="G166" s="21"/>
+      <c r="H166" s="21"/>
+      <c r="I166" s="21"/>
+      <c r="J166" s="22" t="s">
+        <v>41</v>
+      </c>
       <c r="K166" s="23"/>
       <c r="L166" s="8"/>
     </row>
@@ -5717,14 +5725,30 @@
       <c r="A167" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B167" s="7"/>
-      <c r="C167" s="7"/>
-      <c r="D167" s="7"/>
-      <c r="E167" s="7"/>
-      <c r="F167" s="7"/>
-      <c r="G167" s="7"/>
-      <c r="H167" s="68"/>
-      <c r="I167" s="7"/>
+      <c r="B167" s="7">
+        <v>4</v>
+      </c>
+      <c r="C167" s="7">
+        <v>4</v>
+      </c>
+      <c r="D167" s="7">
+        <v>4</v>
+      </c>
+      <c r="E167" s="7">
+        <v>4</v>
+      </c>
+      <c r="F167" s="7">
+        <v>4</v>
+      </c>
+      <c r="G167" s="7">
+        <v>4</v>
+      </c>
+      <c r="H167" s="68">
+        <v>4</v>
+      </c>
+      <c r="I167" s="7">
+        <v>4</v>
+      </c>
       <c r="J167" s="2"/>
       <c r="K167" s="23"/>
       <c r="L167" s="8"/>
@@ -5735,65 +5759,65 @@
       </c>
       <c r="B168" s="34">
         <f>B163+B164+B165+B166+B167</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C168" s="35">
         <f t="shared" ref="C168:I168" si="20">SUM(C163:C167)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D168" s="35">
         <f t="shared" si="20"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E168" s="35">
         <f t="shared" si="20"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F168" s="35">
         <f t="shared" si="20"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G168" s="35">
         <f t="shared" si="20"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H168" s="35">
         <f t="shared" si="20"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I168" s="35">
         <f t="shared" si="20"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J168" s="36"/>
       <c r="K168" s="23"/>
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A169" s="75"/>
-      <c r="B169" s="75"/>
-      <c r="C169" s="75"/>
-      <c r="D169" s="75"/>
-      <c r="E169" s="75"/>
-      <c r="F169" s="75"/>
-      <c r="G169" s="75"/>
-      <c r="H169" s="75"/>
-      <c r="I169" s="75"/>
-      <c r="J169" s="75"/>
+      <c r="A169" s="76"/>
+      <c r="B169" s="76"/>
+      <c r="C169" s="76"/>
+      <c r="D169" s="76"/>
+      <c r="E169" s="76"/>
+      <c r="F169" s="76"/>
+      <c r="G169" s="76"/>
+      <c r="H169" s="76"/>
+      <c r="I169" s="76"/>
+      <c r="J169" s="76"/>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="76"/>
-      <c r="C170" s="73"/>
-      <c r="D170" s="73"/>
-      <c r="E170" s="73"/>
-      <c r="F170" s="73"/>
-      <c r="G170" s="73"/>
-      <c r="H170" s="73"/>
-      <c r="I170" s="73"/>
-      <c r="J170" s="77"/>
+      <c r="B170" s="73"/>
+      <c r="C170" s="74"/>
+      <c r="D170" s="74"/>
+      <c r="E170" s="74"/>
+      <c r="F170" s="74"/>
+      <c r="G170" s="74"/>
+      <c r="H170" s="74"/>
+      <c r="I170" s="74"/>
+      <c r="J170" s="75"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -5894,31 +5918,63 @@
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="73"/>
-      <c r="B177" s="73"/>
-      <c r="C177" s="73"/>
-      <c r="D177" s="73"/>
-      <c r="E177" s="73"/>
-      <c r="F177" s="73"/>
-      <c r="G177" s="73"/>
-      <c r="H177" s="73"/>
-      <c r="I177" s="73"/>
-      <c r="J177" s="73"/>
+      <c r="A177" s="74"/>
+      <c r="B177" s="74"/>
+      <c r="C177" s="74"/>
+      <c r="D177" s="74"/>
+      <c r="E177" s="74"/>
+      <c r="F177" s="74"/>
+      <c r="G177" s="74"/>
+      <c r="H177" s="74"/>
+      <c r="I177" s="74"/>
+      <c r="J177" s="74"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="74"/>
-      <c r="B178" s="74"/>
-      <c r="C178" s="74"/>
-      <c r="D178" s="74"/>
-      <c r="E178" s="74"/>
-      <c r="F178" s="74"/>
-      <c r="G178" s="74"/>
-      <c r="H178" s="74"/>
-      <c r="I178" s="74"/>
-      <c r="J178" s="74"/>
+      <c r="A178" s="77"/>
+      <c r="B178" s="77"/>
+      <c r="C178" s="77"/>
+      <c r="D178" s="77"/>
+      <c r="E178" s="77"/>
+      <c r="F178" s="77"/>
+      <c r="G178" s="77"/>
+      <c r="H178" s="77"/>
+      <c r="I178" s="77"/>
+      <c r="J178" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="B154:J154"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="B162:J162"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="B170:J170"/>
+    <mergeCell ref="B146:J146"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="B114:J114"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="B122:J122"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="B130:J130"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="B138:J138"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="B98:J98"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="B82:J82"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A97:J97"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="B2:J2"/>
@@ -5932,38 +5988,6 @@
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B98:J98"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A97:J97"/>
-    <mergeCell ref="B146:J146"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B114:J114"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="B122:J122"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="B130:J130"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="B138:J138"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="B154:J154"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="B162:J162"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="B170:J170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
uren reg + bgm manager scr
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -745,19 +745,19 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1040,7 +1040,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1052,7 +1052,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L170" sqref="L170"/>
+      <selection pane="bottomLeft" activeCell="K166" sqref="K166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1112,29 +1112,29 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="77"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="75"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.9691011235955056</v>
+        <v>0.96952908587257614</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>35</v>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.8398876404494382</v>
+        <v>0.82825484764542934</v>
       </c>
       <c r="O3" s="54" t="s">
         <v>34</v>
@@ -1226,11 +1226,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.9915730337078652</v>
+        <v>0.99168975069252074</v>
       </c>
       <c r="O4" s="55" t="s">
         <v>36</v>
@@ -1274,11 +1274,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.93258426966292129</v>
+        <v>0.93351800554016617</v>
       </c>
       <c r="O5" s="56" t="s">
         <v>37</v>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.7893258426966292</v>
+        <v>0.77839335180055402</v>
       </c>
       <c r="O6" s="57" t="s">
         <v>38</v>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.72752808988764039</v>
+        <v>0.7174515235457064</v>
       </c>
       <c r="O7" s="58" t="s">
         <v>39</v>
@@ -1410,11 +1410,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.9719101123595506</v>
+        <v>0.97229916897506929</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>40</v>
@@ -1424,30 +1424,30 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A9" s="75"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="77"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="75"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1654,30 +1654,30 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="75"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
+      <c r="A17" s="76"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="77"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="75"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1882,30 +1882,30 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="75"/>
+      <c r="A25" s="76"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="77"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="75"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -2110,30 +2110,30 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="75"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
+      <c r="A33" s="76"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="76"/>
+      <c r="J33" s="76"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="76"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="77"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="75"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2340,30 +2340,30 @@
       <c r="L40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A41" s="75"/>
-      <c r="B41" s="75"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="76"/>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="73"/>
-      <c r="J42" s="77"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="74"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="75"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2572,30 +2572,30 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="75"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="75"/>
-      <c r="I49" s="75"/>
-      <c r="J49" s="75"/>
+      <c r="A49" s="76"/>
+      <c r="B49" s="76"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
+      <c r="J49" s="76"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="76"/>
-      <c r="C50" s="73"/>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="73"/>
-      <c r="I50" s="73"/>
-      <c r="J50" s="77"/>
+      <c r="B50" s="73"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="75"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2800,30 +2800,30 @@
       <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="75"/>
-      <c r="B57" s="75"/>
-      <c r="C57" s="75"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="75"/>
-      <c r="I57" s="75"/>
-      <c r="J57" s="75"/>
+      <c r="A57" s="76"/>
+      <c r="B57" s="76"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="76"/>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="73"/>
-      <c r="G58" s="73"/>
-      <c r="H58" s="73"/>
-      <c r="I58" s="73"/>
-      <c r="J58" s="77"/>
+      <c r="B58" s="73"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="74"/>
+      <c r="I58" s="74"/>
+      <c r="J58" s="75"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -3032,30 +3032,30 @@
       <c r="L64" s="8"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A65" s="75"/>
-      <c r="B65" s="75"/>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="75"/>
-      <c r="H65" s="75"/>
-      <c r="I65" s="75"/>
-      <c r="J65" s="75"/>
+      <c r="A65" s="76"/>
+      <c r="B65" s="76"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="76"/>
+      <c r="G65" s="76"/>
+      <c r="H65" s="76"/>
+      <c r="I65" s="76"/>
+      <c r="J65" s="76"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="76"/>
-      <c r="C66" s="73"/>
-      <c r="D66" s="73"/>
-      <c r="E66" s="73"/>
-      <c r="F66" s="73"/>
-      <c r="G66" s="73"/>
-      <c r="H66" s="73"/>
-      <c r="I66" s="73"/>
-      <c r="J66" s="77"/>
+      <c r="B66" s="73"/>
+      <c r="C66" s="74"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
+      <c r="F66" s="74"/>
+      <c r="G66" s="74"/>
+      <c r="H66" s="74"/>
+      <c r="I66" s="74"/>
+      <c r="J66" s="75"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -3190,30 +3190,30 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A73" s="75"/>
-      <c r="B73" s="75"/>
-      <c r="C73" s="75"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
-      <c r="I73" s="75"/>
-      <c r="J73" s="75"/>
+      <c r="A73" s="76"/>
+      <c r="B73" s="76"/>
+      <c r="C73" s="76"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="76"/>
+      <c r="G73" s="76"/>
+      <c r="H73" s="76"/>
+      <c r="I73" s="76"/>
+      <c r="J73" s="76"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="76"/>
-      <c r="C74" s="73"/>
-      <c r="D74" s="73"/>
-      <c r="E74" s="73"/>
-      <c r="F74" s="73"/>
-      <c r="G74" s="73"/>
-      <c r="H74" s="73"/>
-      <c r="I74" s="73"/>
-      <c r="J74" s="77"/>
+      <c r="B74" s="73"/>
+      <c r="C74" s="74"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="74"/>
+      <c r="H74" s="74"/>
+      <c r="I74" s="74"/>
+      <c r="J74" s="75"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3404,30 +3404,30 @@
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A81" s="75"/>
-      <c r="B81" s="75"/>
-      <c r="C81" s="75"/>
-      <c r="D81" s="75"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="75"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
-      <c r="I81" s="75"/>
-      <c r="J81" s="75"/>
+      <c r="A81" s="76"/>
+      <c r="B81" s="76"/>
+      <c r="C81" s="76"/>
+      <c r="D81" s="76"/>
+      <c r="E81" s="76"/>
+      <c r="F81" s="76"/>
+      <c r="G81" s="76"/>
+      <c r="H81" s="76"/>
+      <c r="I81" s="76"/>
+      <c r="J81" s="76"/>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="76"/>
-      <c r="C82" s="73"/>
-      <c r="D82" s="73"/>
-      <c r="E82" s="73"/>
-      <c r="F82" s="73"/>
-      <c r="G82" s="73"/>
-      <c r="H82" s="73"/>
-      <c r="I82" s="73"/>
-      <c r="J82" s="77"/>
+      <c r="B82" s="73"/>
+      <c r="C82" s="74"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="74"/>
+      <c r="F82" s="74"/>
+      <c r="G82" s="74"/>
+      <c r="H82" s="74"/>
+      <c r="I82" s="74"/>
+      <c r="J82" s="75"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3634,30 +3634,30 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A89" s="75"/>
-      <c r="B89" s="75"/>
-      <c r="C89" s="75"/>
-      <c r="D89" s="75"/>
-      <c r="E89" s="75"/>
-      <c r="F89" s="75"/>
-      <c r="G89" s="75"/>
-      <c r="H89" s="75"/>
-      <c r="I89" s="75"/>
-      <c r="J89" s="75"/>
+      <c r="A89" s="76"/>
+      <c r="B89" s="76"/>
+      <c r="C89" s="76"/>
+      <c r="D89" s="76"/>
+      <c r="E89" s="76"/>
+      <c r="F89" s="76"/>
+      <c r="G89" s="76"/>
+      <c r="H89" s="76"/>
+      <c r="I89" s="76"/>
+      <c r="J89" s="76"/>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="76"/>
-      <c r="C90" s="73"/>
-      <c r="D90" s="73"/>
-      <c r="E90" s="73"/>
-      <c r="F90" s="73"/>
-      <c r="G90" s="73"/>
-      <c r="H90" s="73"/>
-      <c r="I90" s="73"/>
-      <c r="J90" s="77"/>
+      <c r="B90" s="73"/>
+      <c r="C90" s="74"/>
+      <c r="D90" s="74"/>
+      <c r="E90" s="74"/>
+      <c r="F90" s="74"/>
+      <c r="G90" s="74"/>
+      <c r="H90" s="74"/>
+      <c r="I90" s="74"/>
+      <c r="J90" s="75"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3862,30 +3862,30 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A97" s="75"/>
-      <c r="B97" s="75"/>
-      <c r="C97" s="75"/>
-      <c r="D97" s="75"/>
-      <c r="E97" s="75"/>
-      <c r="F97" s="75"/>
-      <c r="G97" s="75"/>
-      <c r="H97" s="75"/>
-      <c r="I97" s="75"/>
-      <c r="J97" s="75"/>
+      <c r="A97" s="76"/>
+      <c r="B97" s="76"/>
+      <c r="C97" s="76"/>
+      <c r="D97" s="76"/>
+      <c r="E97" s="76"/>
+      <c r="F97" s="76"/>
+      <c r="G97" s="76"/>
+      <c r="H97" s="76"/>
+      <c r="I97" s="76"/>
+      <c r="J97" s="76"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="76"/>
-      <c r="C98" s="73"/>
-      <c r="D98" s="73"/>
-      <c r="E98" s="73"/>
-      <c r="F98" s="73"/>
-      <c r="G98" s="73"/>
-      <c r="H98" s="73"/>
-      <c r="I98" s="73"/>
-      <c r="J98" s="77"/>
+      <c r="B98" s="73"/>
+      <c r="C98" s="74"/>
+      <c r="D98" s="74"/>
+      <c r="E98" s="74"/>
+      <c r="F98" s="74"/>
+      <c r="G98" s="74"/>
+      <c r="H98" s="74"/>
+      <c r="I98" s="74"/>
+      <c r="J98" s="75"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -4092,30 +4092,30 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A105" s="75"/>
-      <c r="B105" s="75"/>
-      <c r="C105" s="75"/>
-      <c r="D105" s="75"/>
-      <c r="E105" s="75"/>
-      <c r="F105" s="75"/>
-      <c r="G105" s="75"/>
-      <c r="H105" s="75"/>
-      <c r="I105" s="75"/>
-      <c r="J105" s="75"/>
+      <c r="A105" s="76"/>
+      <c r="B105" s="76"/>
+      <c r="C105" s="76"/>
+      <c r="D105" s="76"/>
+      <c r="E105" s="76"/>
+      <c r="F105" s="76"/>
+      <c r="G105" s="76"/>
+      <c r="H105" s="76"/>
+      <c r="I105" s="76"/>
+      <c r="J105" s="76"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="76"/>
-      <c r="C106" s="73"/>
-      <c r="D106" s="73"/>
-      <c r="E106" s="73"/>
-      <c r="F106" s="73"/>
-      <c r="G106" s="73"/>
-      <c r="H106" s="73"/>
-      <c r="I106" s="73"/>
-      <c r="J106" s="77"/>
+      <c r="B106" s="73"/>
+      <c r="C106" s="74"/>
+      <c r="D106" s="74"/>
+      <c r="E106" s="74"/>
+      <c r="F106" s="74"/>
+      <c r="G106" s="74"/>
+      <c r="H106" s="74"/>
+      <c r="I106" s="74"/>
+      <c r="J106" s="75"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -4322,30 +4322,30 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A113" s="75"/>
-      <c r="B113" s="75"/>
-      <c r="C113" s="75"/>
-      <c r="D113" s="75"/>
-      <c r="E113" s="75"/>
-      <c r="F113" s="75"/>
-      <c r="G113" s="75"/>
-      <c r="H113" s="75"/>
-      <c r="I113" s="75"/>
-      <c r="J113" s="75"/>
+      <c r="A113" s="76"/>
+      <c r="B113" s="76"/>
+      <c r="C113" s="76"/>
+      <c r="D113" s="76"/>
+      <c r="E113" s="76"/>
+      <c r="F113" s="76"/>
+      <c r="G113" s="76"/>
+      <c r="H113" s="76"/>
+      <c r="I113" s="76"/>
+      <c r="J113" s="76"/>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="76"/>
-      <c r="C114" s="73"/>
-      <c r="D114" s="73"/>
-      <c r="E114" s="73"/>
-      <c r="F114" s="73"/>
-      <c r="G114" s="73"/>
-      <c r="H114" s="73"/>
-      <c r="I114" s="73"/>
-      <c r="J114" s="77"/>
+      <c r="B114" s="73"/>
+      <c r="C114" s="74"/>
+      <c r="D114" s="74"/>
+      <c r="E114" s="74"/>
+      <c r="F114" s="74"/>
+      <c r="G114" s="74"/>
+      <c r="H114" s="74"/>
+      <c r="I114" s="74"/>
+      <c r="J114" s="75"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -4550,30 +4550,30 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A121" s="75"/>
-      <c r="B121" s="75"/>
-      <c r="C121" s="75"/>
-      <c r="D121" s="75"/>
-      <c r="E121" s="75"/>
-      <c r="F121" s="75"/>
-      <c r="G121" s="75"/>
-      <c r="H121" s="75"/>
-      <c r="I121" s="75"/>
-      <c r="J121" s="75"/>
+      <c r="A121" s="76"/>
+      <c r="B121" s="76"/>
+      <c r="C121" s="76"/>
+      <c r="D121" s="76"/>
+      <c r="E121" s="76"/>
+      <c r="F121" s="76"/>
+      <c r="G121" s="76"/>
+      <c r="H121" s="76"/>
+      <c r="I121" s="76"/>
+      <c r="J121" s="76"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="76"/>
-      <c r="C122" s="73"/>
-      <c r="D122" s="73"/>
-      <c r="E122" s="73"/>
-      <c r="F122" s="73"/>
-      <c r="G122" s="73"/>
-      <c r="H122" s="73"/>
-      <c r="I122" s="73"/>
-      <c r="J122" s="77"/>
+      <c r="B122" s="73"/>
+      <c r="C122" s="74"/>
+      <c r="D122" s="74"/>
+      <c r="E122" s="74"/>
+      <c r="F122" s="74"/>
+      <c r="G122" s="74"/>
+      <c r="H122" s="74"/>
+      <c r="I122" s="74"/>
+      <c r="J122" s="75"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -4766,30 +4766,30 @@
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A129" s="75"/>
-      <c r="B129" s="75"/>
-      <c r="C129" s="75"/>
-      <c r="D129" s="75"/>
-      <c r="E129" s="75"/>
-      <c r="F129" s="75"/>
-      <c r="G129" s="75"/>
-      <c r="H129" s="75"/>
-      <c r="I129" s="75"/>
-      <c r="J129" s="75"/>
+      <c r="A129" s="76"/>
+      <c r="B129" s="76"/>
+      <c r="C129" s="76"/>
+      <c r="D129" s="76"/>
+      <c r="E129" s="76"/>
+      <c r="F129" s="76"/>
+      <c r="G129" s="76"/>
+      <c r="H129" s="76"/>
+      <c r="I129" s="76"/>
+      <c r="J129" s="76"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="76"/>
-      <c r="C130" s="73"/>
-      <c r="D130" s="73"/>
-      <c r="E130" s="73"/>
-      <c r="F130" s="73"/>
-      <c r="G130" s="73"/>
-      <c r="H130" s="73"/>
-      <c r="I130" s="73"/>
-      <c r="J130" s="77"/>
+      <c r="B130" s="73"/>
+      <c r="C130" s="74"/>
+      <c r="D130" s="74"/>
+      <c r="E130" s="74"/>
+      <c r="F130" s="74"/>
+      <c r="G130" s="74"/>
+      <c r="H130" s="74"/>
+      <c r="I130" s="74"/>
+      <c r="J130" s="75"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -4994,30 +4994,30 @@
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A137" s="75"/>
-      <c r="B137" s="75"/>
-      <c r="C137" s="75"/>
-      <c r="D137" s="75"/>
-      <c r="E137" s="75"/>
-      <c r="F137" s="75"/>
-      <c r="G137" s="75"/>
-      <c r="H137" s="75"/>
-      <c r="I137" s="75"/>
-      <c r="J137" s="75"/>
+      <c r="A137" s="76"/>
+      <c r="B137" s="76"/>
+      <c r="C137" s="76"/>
+      <c r="D137" s="76"/>
+      <c r="E137" s="76"/>
+      <c r="F137" s="76"/>
+      <c r="G137" s="76"/>
+      <c r="H137" s="76"/>
+      <c r="I137" s="76"/>
+      <c r="J137" s="76"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="76"/>
-      <c r="C138" s="73"/>
-      <c r="D138" s="73"/>
-      <c r="E138" s="73"/>
-      <c r="F138" s="73"/>
-      <c r="G138" s="73"/>
-      <c r="H138" s="73"/>
-      <c r="I138" s="73"/>
-      <c r="J138" s="77"/>
+      <c r="B138" s="73"/>
+      <c r="C138" s="74"/>
+      <c r="D138" s="74"/>
+      <c r="E138" s="74"/>
+      <c r="F138" s="74"/>
+      <c r="G138" s="74"/>
+      <c r="H138" s="74"/>
+      <c r="I138" s="74"/>
+      <c r="J138" s="75"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -5152,30 +5152,30 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A145" s="75"/>
-      <c r="B145" s="75"/>
-      <c r="C145" s="75"/>
-      <c r="D145" s="75"/>
-      <c r="E145" s="75"/>
-      <c r="F145" s="75"/>
-      <c r="G145" s="75"/>
-      <c r="H145" s="75"/>
-      <c r="I145" s="75"/>
-      <c r="J145" s="75"/>
+      <c r="A145" s="76"/>
+      <c r="B145" s="76"/>
+      <c r="C145" s="76"/>
+      <c r="D145" s="76"/>
+      <c r="E145" s="76"/>
+      <c r="F145" s="76"/>
+      <c r="G145" s="76"/>
+      <c r="H145" s="76"/>
+      <c r="I145" s="76"/>
+      <c r="J145" s="76"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="76"/>
-      <c r="C146" s="73"/>
-      <c r="D146" s="73"/>
-      <c r="E146" s="73"/>
-      <c r="F146" s="73"/>
-      <c r="G146" s="73"/>
-      <c r="H146" s="73"/>
-      <c r="I146" s="73"/>
-      <c r="J146" s="77"/>
+      <c r="B146" s="73"/>
+      <c r="C146" s="74"/>
+      <c r="D146" s="74"/>
+      <c r="E146" s="74"/>
+      <c r="F146" s="74"/>
+      <c r="G146" s="74"/>
+      <c r="H146" s="74"/>
+      <c r="I146" s="74"/>
+      <c r="J146" s="75"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -5366,30 +5366,30 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A153" s="75"/>
-      <c r="B153" s="75"/>
-      <c r="C153" s="75"/>
-      <c r="D153" s="75"/>
-      <c r="E153" s="75"/>
-      <c r="F153" s="75"/>
-      <c r="G153" s="75"/>
-      <c r="H153" s="75"/>
-      <c r="I153" s="75"/>
-      <c r="J153" s="75"/>
+      <c r="A153" s="76"/>
+      <c r="B153" s="76"/>
+      <c r="C153" s="76"/>
+      <c r="D153" s="76"/>
+      <c r="E153" s="76"/>
+      <c r="F153" s="76"/>
+      <c r="G153" s="76"/>
+      <c r="H153" s="76"/>
+      <c r="I153" s="76"/>
+      <c r="J153" s="76"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="76"/>
-      <c r="C154" s="73"/>
-      <c r="D154" s="73"/>
-      <c r="E154" s="73"/>
-      <c r="F154" s="73"/>
-      <c r="G154" s="73"/>
-      <c r="H154" s="73"/>
-      <c r="I154" s="73"/>
-      <c r="J154" s="77"/>
+      <c r="B154" s="73"/>
+      <c r="C154" s="74"/>
+      <c r="D154" s="74"/>
+      <c r="E154" s="74"/>
+      <c r="F154" s="74"/>
+      <c r="G154" s="74"/>
+      <c r="H154" s="74"/>
+      <c r="I154" s="74"/>
+      <c r="J154" s="75"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -5580,30 +5580,30 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A161" s="75"/>
-      <c r="B161" s="75"/>
-      <c r="C161" s="75"/>
-      <c r="D161" s="75"/>
-      <c r="E161" s="75"/>
-      <c r="F161" s="75"/>
-      <c r="G161" s="75"/>
-      <c r="H161" s="75"/>
-      <c r="I161" s="75"/>
-      <c r="J161" s="75"/>
+      <c r="A161" s="76"/>
+      <c r="B161" s="76"/>
+      <c r="C161" s="76"/>
+      <c r="D161" s="76"/>
+      <c r="E161" s="76"/>
+      <c r="F161" s="76"/>
+      <c r="G161" s="76"/>
+      <c r="H161" s="76"/>
+      <c r="I161" s="76"/>
+      <c r="J161" s="76"/>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="76"/>
-      <c r="C162" s="73"/>
-      <c r="D162" s="73"/>
-      <c r="E162" s="73"/>
-      <c r="F162" s="73"/>
-      <c r="G162" s="73"/>
-      <c r="H162" s="73"/>
-      <c r="I162" s="73"/>
-      <c r="J162" s="77"/>
+      <c r="B162" s="73"/>
+      <c r="C162" s="74"/>
+      <c r="D162" s="74"/>
+      <c r="E162" s="74"/>
+      <c r="F162" s="74"/>
+      <c r="G162" s="74"/>
+      <c r="H162" s="74"/>
+      <c r="I162" s="74"/>
+      <c r="J162" s="75"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -5794,30 +5794,30 @@
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A169" s="75"/>
-      <c r="B169" s="75"/>
-      <c r="C169" s="75"/>
-      <c r="D169" s="75"/>
-      <c r="E169" s="75"/>
-      <c r="F169" s="75"/>
-      <c r="G169" s="75"/>
-      <c r="H169" s="75"/>
-      <c r="I169" s="75"/>
-      <c r="J169" s="75"/>
+      <c r="A169" s="76"/>
+      <c r="B169" s="76"/>
+      <c r="C169" s="76"/>
+      <c r="D169" s="76"/>
+      <c r="E169" s="76"/>
+      <c r="F169" s="76"/>
+      <c r="G169" s="76"/>
+      <c r="H169" s="76"/>
+      <c r="I169" s="76"/>
+      <c r="J169" s="76"/>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="76"/>
-      <c r="C170" s="73"/>
-      <c r="D170" s="73"/>
-      <c r="E170" s="73"/>
-      <c r="F170" s="73"/>
-      <c r="G170" s="73"/>
-      <c r="H170" s="73"/>
-      <c r="I170" s="73"/>
-      <c r="J170" s="77"/>
+      <c r="B170" s="73"/>
+      <c r="C170" s="74"/>
+      <c r="D170" s="74"/>
+      <c r="E170" s="74"/>
+      <c r="F170" s="74"/>
+      <c r="G170" s="74"/>
+      <c r="H170" s="74"/>
+      <c r="I170" s="74"/>
+      <c r="J170" s="75"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -5857,8 +5857,30 @@
       <c r="A172" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B172" s="8"/>
-      <c r="H172" s="67"/>
+      <c r="B172" s="8">
+        <v>5</v>
+      </c>
+      <c r="C172" s="6">
+        <v>5</v>
+      </c>
+      <c r="D172" s="28">
+        <v>0</v>
+      </c>
+      <c r="E172" s="6">
+        <v>5</v>
+      </c>
+      <c r="F172" s="6">
+        <v>5</v>
+      </c>
+      <c r="G172" s="28">
+        <v>0</v>
+      </c>
+      <c r="H172" s="72">
+        <v>0</v>
+      </c>
+      <c r="I172" s="6">
+        <v>5</v>
+      </c>
       <c r="J172" s="1"/>
       <c r="K172" s="23"/>
       <c r="L172" s="8"/>
@@ -5905,11 +5927,11 @@
       </c>
       <c r="B176" s="34">
         <f>B171+B172+B173+B174+B175</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C176" s="35">
         <f t="shared" ref="C176:I176" si="21">SUM(C171:C175)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D176" s="35">
         <f t="shared" si="21"/>
@@ -5917,11 +5939,11 @@
       </c>
       <c r="E176" s="35">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F176" s="35">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G176" s="35">
         <f t="shared" si="21"/>
@@ -5933,38 +5955,70 @@
       </c>
       <c r="I176" s="35">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J176" s="36"/>
       <c r="K176" s="23"/>
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="73"/>
-      <c r="B177" s="73"/>
-      <c r="C177" s="73"/>
-      <c r="D177" s="73"/>
-      <c r="E177" s="73"/>
-      <c r="F177" s="73"/>
-      <c r="G177" s="73"/>
-      <c r="H177" s="73"/>
-      <c r="I177" s="73"/>
-      <c r="J177" s="73"/>
+      <c r="A177" s="74"/>
+      <c r="B177" s="74"/>
+      <c r="C177" s="74"/>
+      <c r="D177" s="74"/>
+      <c r="E177" s="74"/>
+      <c r="F177" s="74"/>
+      <c r="G177" s="74"/>
+      <c r="H177" s="74"/>
+      <c r="I177" s="74"/>
+      <c r="J177" s="74"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="74"/>
-      <c r="B178" s="74"/>
-      <c r="C178" s="74"/>
-      <c r="D178" s="74"/>
-      <c r="E178" s="74"/>
-      <c r="F178" s="74"/>
-      <c r="G178" s="74"/>
-      <c r="H178" s="74"/>
-      <c r="I178" s="74"/>
-      <c r="J178" s="74"/>
+      <c r="A178" s="77"/>
+      <c r="B178" s="77"/>
+      <c r="C178" s="77"/>
+      <c r="D178" s="77"/>
+      <c r="E178" s="77"/>
+      <c r="F178" s="77"/>
+      <c r="G178" s="77"/>
+      <c r="H178" s="77"/>
+      <c r="I178" s="77"/>
+      <c r="J178" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="B154:J154"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="B162:J162"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="B170:J170"/>
+    <mergeCell ref="B146:J146"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="B114:J114"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="B122:J122"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="B130:J130"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="B138:J138"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="B98:J98"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="B82:J82"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A97:J97"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="B2:J2"/>
@@ -5978,38 +6032,6 @@
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B98:J98"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A97:J97"/>
-    <mergeCell ref="B146:J146"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B114:J114"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="B122:J122"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="B130:J130"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="B138:J138"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="B154:J154"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="B162:J162"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="B170:J170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
dying notice fix, particals
</commit_message>
<xml_diff>
--- a/Uren Registratie Game-Lab 01.xlsx
+++ b/Uren Registratie Game-Lab 01.xlsx
@@ -745,19 +745,19 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1040,7 +1040,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1051,8 +1051,8 @@
   <dimension ref="A1:P178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K166" sqref="K166"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L171" sqref="L171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1112,29 +1112,29 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="75"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="77"/>
       <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="8">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="M2" s="6">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="N2" s="17">
         <f>M2/L2</f>
-        <v>0.96952908587257614</v>
+        <v>0.96978021978021978</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>35</v>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>0.82825484764542934</v>
+        <v>0.8214285714285714</v>
       </c>
       <c r="O3" s="54" t="s">
         <v>34</v>
@@ -1226,11 +1226,11 @@
       <c r="L4" s="8"/>
       <c r="M4" s="6">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L2</f>
-        <v>0.99168975069252074</v>
+        <v>0.99175824175824179</v>
       </c>
       <c r="O4" s="55" t="s">
         <v>36</v>
@@ -1274,11 +1274,11 @@
       <c r="L5" s="8"/>
       <c r="M5" s="6">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="N5" s="17">
         <f>M5/L2</f>
-        <v>0.93351800554016617</v>
+        <v>0.93406593406593408</v>
       </c>
       <c r="O5" s="56" t="s">
         <v>37</v>
@@ -1308,11 +1308,11 @@
       <c r="L6" s="8"/>
       <c r="M6" s="6">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="N6" s="17">
         <f>M6/L2</f>
-        <v>0.77839335180055402</v>
+        <v>0.79395604395604391</v>
       </c>
       <c r="O6" s="57" t="s">
         <v>38</v>
@@ -1356,11 +1356,11 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="N7" s="17">
         <f>M7/L2</f>
-        <v>0.7174515235457064</v>
+        <v>0.71978021978021978</v>
       </c>
       <c r="O7" s="58" t="s">
         <v>39</v>
@@ -1410,11 +1410,11 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6">
         <f>I8+I16+I24+I32+I40+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="N8" s="17">
         <f>M8/L2</f>
-        <v>0.97229916897506929</v>
+        <v>0.97252747252747251</v>
       </c>
       <c r="O8" s="59" t="s">
         <v>40</v>
@@ -1424,30 +1424,30 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="75"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="77"/>
       <c r="K10" s="23"/>
       <c r="L10" s="8"/>
     </row>
@@ -1654,30 +1654,30 @@
       <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="76"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="75"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="75"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="77"/>
       <c r="K18" s="23"/>
       <c r="L18" s="8"/>
     </row>
@@ -1882,30 +1882,30 @@
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="76"/>
-      <c r="B25" s="76"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="76"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="75"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="77"/>
       <c r="K26" s="23"/>
       <c r="L26" s="8"/>
     </row>
@@ -2110,30 +2110,30 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="76"/>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="76"/>
-      <c r="J33" s="76"/>
+      <c r="A33" s="75"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="75"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="77"/>
       <c r="K34" s="23"/>
       <c r="L34" s="8"/>
     </row>
@@ -2340,30 +2340,30 @@
       <c r="L40" s="8"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A41" s="76"/>
-      <c r="B41" s="76"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="76"/>
+      <c r="A41" s="75"/>
+      <c r="B41" s="75"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="75"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="73"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="75"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="77"/>
       <c r="K42" s="23"/>
       <c r="L42" s="8"/>
     </row>
@@ -2572,30 +2572,30 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="76"/>
-      <c r="B49" s="76"/>
-      <c r="C49" s="76"/>
-      <c r="D49" s="76"/>
-      <c r="E49" s="76"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="76"/>
-      <c r="H49" s="76"/>
-      <c r="I49" s="76"/>
-      <c r="J49" s="76"/>
+      <c r="A49" s="75"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="75"/>
+      <c r="I49" s="75"/>
+      <c r="J49" s="75"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="73"/>
-      <c r="C50" s="74"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="75"/>
+      <c r="B50" s="76"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="73"/>
+      <c r="F50" s="73"/>
+      <c r="G50" s="73"/>
+      <c r="H50" s="73"/>
+      <c r="I50" s="73"/>
+      <c r="J50" s="77"/>
       <c r="K50" s="23"/>
       <c r="L50" s="8"/>
     </row>
@@ -2800,30 +2800,30 @@
       <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="76"/>
-      <c r="B57" s="76"/>
-      <c r="C57" s="76"/>
-      <c r="D57" s="76"/>
-      <c r="E57" s="76"/>
-      <c r="F57" s="76"/>
-      <c r="G57" s="76"/>
-      <c r="H57" s="76"/>
-      <c r="I57" s="76"/>
-      <c r="J57" s="76"/>
+      <c r="A57" s="75"/>
+      <c r="B57" s="75"/>
+      <c r="C57" s="75"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="75"/>
+      <c r="F57" s="75"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="75"/>
+      <c r="I57" s="75"/>
+      <c r="J57" s="75"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="73"/>
-      <c r="C58" s="74"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
-      <c r="F58" s="74"/>
-      <c r="G58" s="74"/>
-      <c r="H58" s="74"/>
-      <c r="I58" s="74"/>
-      <c r="J58" s="75"/>
+      <c r="B58" s="76"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="73"/>
+      <c r="J58" s="77"/>
       <c r="K58" s="23"/>
       <c r="L58" s="8"/>
     </row>
@@ -3032,30 +3032,30 @@
       <c r="L64" s="8"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A65" s="76"/>
-      <c r="B65" s="76"/>
-      <c r="C65" s="76"/>
-      <c r="D65" s="76"/>
-      <c r="E65" s="76"/>
-      <c r="F65" s="76"/>
-      <c r="G65" s="76"/>
-      <c r="H65" s="76"/>
-      <c r="I65" s="76"/>
-      <c r="J65" s="76"/>
+      <c r="A65" s="75"/>
+      <c r="B65" s="75"/>
+      <c r="C65" s="75"/>
+      <c r="D65" s="75"/>
+      <c r="E65" s="75"/>
+      <c r="F65" s="75"/>
+      <c r="G65" s="75"/>
+      <c r="H65" s="75"/>
+      <c r="I65" s="75"/>
+      <c r="J65" s="75"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="73"/>
-      <c r="C66" s="74"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="74"/>
-      <c r="H66" s="74"/>
-      <c r="I66" s="74"/>
-      <c r="J66" s="75"/>
+      <c r="B66" s="76"/>
+      <c r="C66" s="73"/>
+      <c r="D66" s="73"/>
+      <c r="E66" s="73"/>
+      <c r="F66" s="73"/>
+      <c r="G66" s="73"/>
+      <c r="H66" s="73"/>
+      <c r="I66" s="73"/>
+      <c r="J66" s="77"/>
       <c r="K66" s="23"/>
       <c r="L66" s="8"/>
     </row>
@@ -3190,30 +3190,30 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A73" s="76"/>
-      <c r="B73" s="76"/>
-      <c r="C73" s="76"/>
-      <c r="D73" s="76"/>
-      <c r="E73" s="76"/>
-      <c r="F73" s="76"/>
-      <c r="G73" s="76"/>
-      <c r="H73" s="76"/>
-      <c r="I73" s="76"/>
-      <c r="J73" s="76"/>
+      <c r="A73" s="75"/>
+      <c r="B73" s="75"/>
+      <c r="C73" s="75"/>
+      <c r="D73" s="75"/>
+      <c r="E73" s="75"/>
+      <c r="F73" s="75"/>
+      <c r="G73" s="75"/>
+      <c r="H73" s="75"/>
+      <c r="I73" s="75"/>
+      <c r="J73" s="75"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="73"/>
-      <c r="C74" s="74"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="74"/>
-      <c r="H74" s="74"/>
-      <c r="I74" s="74"/>
-      <c r="J74" s="75"/>
+      <c r="B74" s="76"/>
+      <c r="C74" s="73"/>
+      <c r="D74" s="73"/>
+      <c r="E74" s="73"/>
+      <c r="F74" s="73"/>
+      <c r="G74" s="73"/>
+      <c r="H74" s="73"/>
+      <c r="I74" s="73"/>
+      <c r="J74" s="77"/>
       <c r="K74" s="23"/>
       <c r="L74" s="8"/>
     </row>
@@ -3404,30 +3404,30 @@
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A81" s="76"/>
-      <c r="B81" s="76"/>
-      <c r="C81" s="76"/>
-      <c r="D81" s="76"/>
-      <c r="E81" s="76"/>
-      <c r="F81" s="76"/>
-      <c r="G81" s="76"/>
-      <c r="H81" s="76"/>
-      <c r="I81" s="76"/>
-      <c r="J81" s="76"/>
+      <c r="A81" s="75"/>
+      <c r="B81" s="75"/>
+      <c r="C81" s="75"/>
+      <c r="D81" s="75"/>
+      <c r="E81" s="75"/>
+      <c r="F81" s="75"/>
+      <c r="G81" s="75"/>
+      <c r="H81" s="75"/>
+      <c r="I81" s="75"/>
+      <c r="J81" s="75"/>
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="73"/>
-      <c r="C82" s="74"/>
-      <c r="D82" s="74"/>
-      <c r="E82" s="74"/>
-      <c r="F82" s="74"/>
-      <c r="G82" s="74"/>
-      <c r="H82" s="74"/>
-      <c r="I82" s="74"/>
-      <c r="J82" s="75"/>
+      <c r="B82" s="76"/>
+      <c r="C82" s="73"/>
+      <c r="D82" s="73"/>
+      <c r="E82" s="73"/>
+      <c r="F82" s="73"/>
+      <c r="G82" s="73"/>
+      <c r="H82" s="73"/>
+      <c r="I82" s="73"/>
+      <c r="J82" s="77"/>
       <c r="K82" s="23"/>
       <c r="L82" s="8"/>
     </row>
@@ -3634,30 +3634,30 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A89" s="76"/>
-      <c r="B89" s="76"/>
-      <c r="C89" s="76"/>
-      <c r="D89" s="76"/>
-      <c r="E89" s="76"/>
-      <c r="F89" s="76"/>
-      <c r="G89" s="76"/>
-      <c r="H89" s="76"/>
-      <c r="I89" s="76"/>
-      <c r="J89" s="76"/>
+      <c r="A89" s="75"/>
+      <c r="B89" s="75"/>
+      <c r="C89" s="75"/>
+      <c r="D89" s="75"/>
+      <c r="E89" s="75"/>
+      <c r="F89" s="75"/>
+      <c r="G89" s="75"/>
+      <c r="H89" s="75"/>
+      <c r="I89" s="75"/>
+      <c r="J89" s="75"/>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B90" s="73"/>
-      <c r="C90" s="74"/>
-      <c r="D90" s="74"/>
-      <c r="E90" s="74"/>
-      <c r="F90" s="74"/>
-      <c r="G90" s="74"/>
-      <c r="H90" s="74"/>
-      <c r="I90" s="74"/>
-      <c r="J90" s="75"/>
+      <c r="B90" s="76"/>
+      <c r="C90" s="73"/>
+      <c r="D90" s="73"/>
+      <c r="E90" s="73"/>
+      <c r="F90" s="73"/>
+      <c r="G90" s="73"/>
+      <c r="H90" s="73"/>
+      <c r="I90" s="73"/>
+      <c r="J90" s="77"/>
       <c r="K90" s="23"/>
       <c r="L90" s="8"/>
     </row>
@@ -3862,30 +3862,30 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A97" s="76"/>
-      <c r="B97" s="76"/>
-      <c r="C97" s="76"/>
-      <c r="D97" s="76"/>
-      <c r="E97" s="76"/>
-      <c r="F97" s="76"/>
-      <c r="G97" s="76"/>
-      <c r="H97" s="76"/>
-      <c r="I97" s="76"/>
-      <c r="J97" s="76"/>
+      <c r="A97" s="75"/>
+      <c r="B97" s="75"/>
+      <c r="C97" s="75"/>
+      <c r="D97" s="75"/>
+      <c r="E97" s="75"/>
+      <c r="F97" s="75"/>
+      <c r="G97" s="75"/>
+      <c r="H97" s="75"/>
+      <c r="I97" s="75"/>
+      <c r="J97" s="75"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="73"/>
-      <c r="C98" s="74"/>
-      <c r="D98" s="74"/>
-      <c r="E98" s="74"/>
-      <c r="F98" s="74"/>
-      <c r="G98" s="74"/>
-      <c r="H98" s="74"/>
-      <c r="I98" s="74"/>
-      <c r="J98" s="75"/>
+      <c r="B98" s="76"/>
+      <c r="C98" s="73"/>
+      <c r="D98" s="73"/>
+      <c r="E98" s="73"/>
+      <c r="F98" s="73"/>
+      <c r="G98" s="73"/>
+      <c r="H98" s="73"/>
+      <c r="I98" s="73"/>
+      <c r="J98" s="77"/>
       <c r="K98" s="23"/>
       <c r="L98" s="8"/>
     </row>
@@ -4092,30 +4092,30 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A105" s="76"/>
-      <c r="B105" s="76"/>
-      <c r="C105" s="76"/>
-      <c r="D105" s="76"/>
-      <c r="E105" s="76"/>
-      <c r="F105" s="76"/>
-      <c r="G105" s="76"/>
-      <c r="H105" s="76"/>
-      <c r="I105" s="76"/>
-      <c r="J105" s="76"/>
+      <c r="A105" s="75"/>
+      <c r="B105" s="75"/>
+      <c r="C105" s="75"/>
+      <c r="D105" s="75"/>
+      <c r="E105" s="75"/>
+      <c r="F105" s="75"/>
+      <c r="G105" s="75"/>
+      <c r="H105" s="75"/>
+      <c r="I105" s="75"/>
+      <c r="J105" s="75"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B106" s="73"/>
-      <c r="C106" s="74"/>
-      <c r="D106" s="74"/>
-      <c r="E106" s="74"/>
-      <c r="F106" s="74"/>
-      <c r="G106" s="74"/>
-      <c r="H106" s="74"/>
-      <c r="I106" s="74"/>
-      <c r="J106" s="75"/>
+      <c r="B106" s="76"/>
+      <c r="C106" s="73"/>
+      <c r="D106" s="73"/>
+      <c r="E106" s="73"/>
+      <c r="F106" s="73"/>
+      <c r="G106" s="73"/>
+      <c r="H106" s="73"/>
+      <c r="I106" s="73"/>
+      <c r="J106" s="77"/>
       <c r="K106" s="23"/>
       <c r="L106" s="8"/>
     </row>
@@ -4322,30 +4322,30 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A113" s="76"/>
-      <c r="B113" s="76"/>
-      <c r="C113" s="76"/>
-      <c r="D113" s="76"/>
-      <c r="E113" s="76"/>
-      <c r="F113" s="76"/>
-      <c r="G113" s="76"/>
-      <c r="H113" s="76"/>
-      <c r="I113" s="76"/>
-      <c r="J113" s="76"/>
+      <c r="A113" s="75"/>
+      <c r="B113" s="75"/>
+      <c r="C113" s="75"/>
+      <c r="D113" s="75"/>
+      <c r="E113" s="75"/>
+      <c r="F113" s="75"/>
+      <c r="G113" s="75"/>
+      <c r="H113" s="75"/>
+      <c r="I113" s="75"/>
+      <c r="J113" s="75"/>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="73"/>
-      <c r="C114" s="74"/>
-      <c r="D114" s="74"/>
-      <c r="E114" s="74"/>
-      <c r="F114" s="74"/>
-      <c r="G114" s="74"/>
-      <c r="H114" s="74"/>
-      <c r="I114" s="74"/>
-      <c r="J114" s="75"/>
+      <c r="B114" s="76"/>
+      <c r="C114" s="73"/>
+      <c r="D114" s="73"/>
+      <c r="E114" s="73"/>
+      <c r="F114" s="73"/>
+      <c r="G114" s="73"/>
+      <c r="H114" s="73"/>
+      <c r="I114" s="73"/>
+      <c r="J114" s="77"/>
       <c r="K114" s="23"/>
       <c r="L114" s="8"/>
     </row>
@@ -4550,30 +4550,30 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A121" s="76"/>
-      <c r="B121" s="76"/>
-      <c r="C121" s="76"/>
-      <c r="D121" s="76"/>
-      <c r="E121" s="76"/>
-      <c r="F121" s="76"/>
-      <c r="G121" s="76"/>
-      <c r="H121" s="76"/>
-      <c r="I121" s="76"/>
-      <c r="J121" s="76"/>
+      <c r="A121" s="75"/>
+      <c r="B121" s="75"/>
+      <c r="C121" s="75"/>
+      <c r="D121" s="75"/>
+      <c r="E121" s="75"/>
+      <c r="F121" s="75"/>
+      <c r="G121" s="75"/>
+      <c r="H121" s="75"/>
+      <c r="I121" s="75"/>
+      <c r="J121" s="75"/>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B122" s="73"/>
-      <c r="C122" s="74"/>
-      <c r="D122" s="74"/>
-      <c r="E122" s="74"/>
-      <c r="F122" s="74"/>
-      <c r="G122" s="74"/>
-      <c r="H122" s="74"/>
-      <c r="I122" s="74"/>
-      <c r="J122" s="75"/>
+      <c r="B122" s="76"/>
+      <c r="C122" s="73"/>
+      <c r="D122" s="73"/>
+      <c r="E122" s="73"/>
+      <c r="F122" s="73"/>
+      <c r="G122" s="73"/>
+      <c r="H122" s="73"/>
+      <c r="I122" s="73"/>
+      <c r="J122" s="77"/>
       <c r="K122" s="23"/>
       <c r="L122" s="8"/>
     </row>
@@ -4766,30 +4766,30 @@
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A129" s="76"/>
-      <c r="B129" s="76"/>
-      <c r="C129" s="76"/>
-      <c r="D129" s="76"/>
-      <c r="E129" s="76"/>
-      <c r="F129" s="76"/>
-      <c r="G129" s="76"/>
-      <c r="H129" s="76"/>
-      <c r="I129" s="76"/>
-      <c r="J129" s="76"/>
+      <c r="A129" s="75"/>
+      <c r="B129" s="75"/>
+      <c r="C129" s="75"/>
+      <c r="D129" s="75"/>
+      <c r="E129" s="75"/>
+      <c r="F129" s="75"/>
+      <c r="G129" s="75"/>
+      <c r="H129" s="75"/>
+      <c r="I129" s="75"/>
+      <c r="J129" s="75"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="73"/>
-      <c r="C130" s="74"/>
-      <c r="D130" s="74"/>
-      <c r="E130" s="74"/>
-      <c r="F130" s="74"/>
-      <c r="G130" s="74"/>
-      <c r="H130" s="74"/>
-      <c r="I130" s="74"/>
-      <c r="J130" s="75"/>
+      <c r="B130" s="76"/>
+      <c r="C130" s="73"/>
+      <c r="D130" s="73"/>
+      <c r="E130" s="73"/>
+      <c r="F130" s="73"/>
+      <c r="G130" s="73"/>
+      <c r="H130" s="73"/>
+      <c r="I130" s="73"/>
+      <c r="J130" s="77"/>
       <c r="K130" s="23"/>
       <c r="L130" s="8"/>
     </row>
@@ -4994,30 +4994,30 @@
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A137" s="76"/>
-      <c r="B137" s="76"/>
-      <c r="C137" s="76"/>
-      <c r="D137" s="76"/>
-      <c r="E137" s="76"/>
-      <c r="F137" s="76"/>
-      <c r="G137" s="76"/>
-      <c r="H137" s="76"/>
-      <c r="I137" s="76"/>
-      <c r="J137" s="76"/>
+      <c r="A137" s="75"/>
+      <c r="B137" s="75"/>
+      <c r="C137" s="75"/>
+      <c r="D137" s="75"/>
+      <c r="E137" s="75"/>
+      <c r="F137" s="75"/>
+      <c r="G137" s="75"/>
+      <c r="H137" s="75"/>
+      <c r="I137" s="75"/>
+      <c r="J137" s="75"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="73"/>
-      <c r="C138" s="74"/>
-      <c r="D138" s="74"/>
-      <c r="E138" s="74"/>
-      <c r="F138" s="74"/>
-      <c r="G138" s="74"/>
-      <c r="H138" s="74"/>
-      <c r="I138" s="74"/>
-      <c r="J138" s="75"/>
+      <c r="B138" s="76"/>
+      <c r="C138" s="73"/>
+      <c r="D138" s="73"/>
+      <c r="E138" s="73"/>
+      <c r="F138" s="73"/>
+      <c r="G138" s="73"/>
+      <c r="H138" s="73"/>
+      <c r="I138" s="73"/>
+      <c r="J138" s="77"/>
       <c r="K138" s="23"/>
       <c r="L138" s="8"/>
     </row>
@@ -5152,30 +5152,30 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A145" s="76"/>
-      <c r="B145" s="76"/>
-      <c r="C145" s="76"/>
-      <c r="D145" s="76"/>
-      <c r="E145" s="76"/>
-      <c r="F145" s="76"/>
-      <c r="G145" s="76"/>
-      <c r="H145" s="76"/>
-      <c r="I145" s="76"/>
-      <c r="J145" s="76"/>
+      <c r="A145" s="75"/>
+      <c r="B145" s="75"/>
+      <c r="C145" s="75"/>
+      <c r="D145" s="75"/>
+      <c r="E145" s="75"/>
+      <c r="F145" s="75"/>
+      <c r="G145" s="75"/>
+      <c r="H145" s="75"/>
+      <c r="I145" s="75"/>
+      <c r="J145" s="75"/>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B146" s="73"/>
-      <c r="C146" s="74"/>
-      <c r="D146" s="74"/>
-      <c r="E146" s="74"/>
-      <c r="F146" s="74"/>
-      <c r="G146" s="74"/>
-      <c r="H146" s="74"/>
-      <c r="I146" s="74"/>
-      <c r="J146" s="75"/>
+      <c r="B146" s="76"/>
+      <c r="C146" s="73"/>
+      <c r="D146" s="73"/>
+      <c r="E146" s="73"/>
+      <c r="F146" s="73"/>
+      <c r="G146" s="73"/>
+      <c r="H146" s="73"/>
+      <c r="I146" s="73"/>
+      <c r="J146" s="77"/>
       <c r="K146" s="23"/>
       <c r="L146" s="8"/>
     </row>
@@ -5366,30 +5366,30 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A153" s="76"/>
-      <c r="B153" s="76"/>
-      <c r="C153" s="76"/>
-      <c r="D153" s="76"/>
-      <c r="E153" s="76"/>
-      <c r="F153" s="76"/>
-      <c r="G153" s="76"/>
-      <c r="H153" s="76"/>
-      <c r="I153" s="76"/>
-      <c r="J153" s="76"/>
+      <c r="A153" s="75"/>
+      <c r="B153" s="75"/>
+      <c r="C153" s="75"/>
+      <c r="D153" s="75"/>
+      <c r="E153" s="75"/>
+      <c r="F153" s="75"/>
+      <c r="G153" s="75"/>
+      <c r="H153" s="75"/>
+      <c r="I153" s="75"/>
+      <c r="J153" s="75"/>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B154" s="73"/>
-      <c r="C154" s="74"/>
-      <c r="D154" s="74"/>
-      <c r="E154" s="74"/>
-      <c r="F154" s="74"/>
-      <c r="G154" s="74"/>
-      <c r="H154" s="74"/>
-      <c r="I154" s="74"/>
-      <c r="J154" s="75"/>
+      <c r="B154" s="76"/>
+      <c r="C154" s="73"/>
+      <c r="D154" s="73"/>
+      <c r="E154" s="73"/>
+      <c r="F154" s="73"/>
+      <c r="G154" s="73"/>
+      <c r="H154" s="73"/>
+      <c r="I154" s="73"/>
+      <c r="J154" s="77"/>
       <c r="K154" s="23"/>
       <c r="L154" s="8"/>
     </row>
@@ -5580,30 +5580,30 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A161" s="76"/>
-      <c r="B161" s="76"/>
-      <c r="C161" s="76"/>
-      <c r="D161" s="76"/>
-      <c r="E161" s="76"/>
-      <c r="F161" s="76"/>
-      <c r="G161" s="76"/>
-      <c r="H161" s="76"/>
-      <c r="I161" s="76"/>
-      <c r="J161" s="76"/>
+      <c r="A161" s="75"/>
+      <c r="B161" s="75"/>
+      <c r="C161" s="75"/>
+      <c r="D161" s="75"/>
+      <c r="E161" s="75"/>
+      <c r="F161" s="75"/>
+      <c r="G161" s="75"/>
+      <c r="H161" s="75"/>
+      <c r="I161" s="75"/>
+      <c r="J161" s="75"/>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="73"/>
-      <c r="C162" s="74"/>
-      <c r="D162" s="74"/>
-      <c r="E162" s="74"/>
-      <c r="F162" s="74"/>
-      <c r="G162" s="74"/>
-      <c r="H162" s="74"/>
-      <c r="I162" s="74"/>
-      <c r="J162" s="75"/>
+      <c r="B162" s="76"/>
+      <c r="C162" s="73"/>
+      <c r="D162" s="73"/>
+      <c r="E162" s="73"/>
+      <c r="F162" s="73"/>
+      <c r="G162" s="73"/>
+      <c r="H162" s="73"/>
+      <c r="I162" s="73"/>
+      <c r="J162" s="77"/>
       <c r="K162" s="23"/>
       <c r="L162" s="8"/>
     </row>
@@ -5794,30 +5794,30 @@
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A169" s="76"/>
-      <c r="B169" s="76"/>
-      <c r="C169" s="76"/>
-      <c r="D169" s="76"/>
-      <c r="E169" s="76"/>
-      <c r="F169" s="76"/>
-      <c r="G169" s="76"/>
-      <c r="H169" s="76"/>
-      <c r="I169" s="76"/>
-      <c r="J169" s="76"/>
+      <c r="A169" s="75"/>
+      <c r="B169" s="75"/>
+      <c r="C169" s="75"/>
+      <c r="D169" s="75"/>
+      <c r="E169" s="75"/>
+      <c r="F169" s="75"/>
+      <c r="G169" s="75"/>
+      <c r="H169" s="75"/>
+      <c r="I169" s="75"/>
+      <c r="J169" s="75"/>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="73"/>
-      <c r="C170" s="74"/>
-      <c r="D170" s="74"/>
-      <c r="E170" s="74"/>
-      <c r="F170" s="74"/>
-      <c r="G170" s="74"/>
-      <c r="H170" s="74"/>
-      <c r="I170" s="74"/>
-      <c r="J170" s="75"/>
+      <c r="B170" s="76"/>
+      <c r="C170" s="73"/>
+      <c r="D170" s="73"/>
+      <c r="E170" s="73"/>
+      <c r="F170" s="73"/>
+      <c r="G170" s="73"/>
+      <c r="H170" s="73"/>
+      <c r="I170" s="73"/>
+      <c r="J170" s="77"/>
       <c r="K170" s="23"/>
       <c r="L170" s="8"/>
     </row>
@@ -5872,8 +5872,8 @@
       <c r="F172" s="6">
         <v>5</v>
       </c>
-      <c r="G172" s="28">
-        <v>0</v>
+      <c r="G172" s="61">
+        <v>5</v>
       </c>
       <c r="H172" s="72">
         <v>0</v>
@@ -5889,8 +5889,30 @@
       <c r="A173" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B173" s="8"/>
-      <c r="H173" s="67"/>
+      <c r="B173" s="8">
+        <v>3</v>
+      </c>
+      <c r="C173" s="6">
+        <v>3</v>
+      </c>
+      <c r="D173" s="28">
+        <v>0</v>
+      </c>
+      <c r="E173" s="6">
+        <v>3</v>
+      </c>
+      <c r="F173" s="6">
+        <v>3</v>
+      </c>
+      <c r="G173" s="6">
+        <v>3</v>
+      </c>
+      <c r="H173" s="67">
+        <v>3</v>
+      </c>
+      <c r="I173" s="6">
+        <v>3</v>
+      </c>
       <c r="J173" s="1"/>
       <c r="K173" s="23"/>
       <c r="L173" s="8"/>
@@ -5927,11 +5949,11 @@
       </c>
       <c r="B176" s="34">
         <f>B171+B172+B173+B174+B175</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C176" s="35">
         <f t="shared" ref="C176:I176" si="21">SUM(C171:C175)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D176" s="35">
         <f t="shared" si="21"/>
@@ -5939,86 +5961,54 @@
       </c>
       <c r="E176" s="35">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F176" s="35">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G176" s="35">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H176" s="35">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I176" s="35">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J176" s="36"/>
       <c r="K176" s="23"/>
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="74"/>
-      <c r="B177" s="74"/>
-      <c r="C177" s="74"/>
-      <c r="D177" s="74"/>
-      <c r="E177" s="74"/>
-      <c r="F177" s="74"/>
-      <c r="G177" s="74"/>
-      <c r="H177" s="74"/>
-      <c r="I177" s="74"/>
-      <c r="J177" s="74"/>
+      <c r="A177" s="73"/>
+      <c r="B177" s="73"/>
+      <c r="C177" s="73"/>
+      <c r="D177" s="73"/>
+      <c r="E177" s="73"/>
+      <c r="F177" s="73"/>
+      <c r="G177" s="73"/>
+      <c r="H177" s="73"/>
+      <c r="I177" s="73"/>
+      <c r="J177" s="73"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="77"/>
-      <c r="B178" s="77"/>
-      <c r="C178" s="77"/>
-      <c r="D178" s="77"/>
-      <c r="E178" s="77"/>
-      <c r="F178" s="77"/>
-      <c r="G178" s="77"/>
-      <c r="H178" s="77"/>
-      <c r="I178" s="77"/>
-      <c r="J178" s="77"/>
+      <c r="A178" s="74"/>
+      <c r="B178" s="74"/>
+      <c r="C178" s="74"/>
+      <c r="D178" s="74"/>
+      <c r="E178" s="74"/>
+      <c r="F178" s="74"/>
+      <c r="G178" s="74"/>
+      <c r="H178" s="74"/>
+      <c r="I178" s="74"/>
+      <c r="J178" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="B154:J154"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="B162:J162"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="B170:J170"/>
-    <mergeCell ref="B146:J146"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="B106:J106"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B114:J114"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="B122:J122"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="B130:J130"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="B138:J138"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="B98:J98"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="B90:J90"/>
-    <mergeCell ref="A97:J97"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="B2:J2"/>
@@ -6032,6 +6022,38 @@
     <mergeCell ref="B34:J34"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B98:J98"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="B82:J82"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="B90:J90"/>
+    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="B146:J146"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="B114:J114"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="B122:J122"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="B130:J130"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="B138:J138"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="B154:J154"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="B162:J162"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="B170:J170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>